<commit_message>
Fixed the problem with lead products and duplicates results
</commit_message>
<xml_diff>
--- a/Projects/PNGRO/Data/Template.xlsx
+++ b/Projects/PNGRO/Data/Template.xlsx
@@ -13,19 +13,20 @@
     <sheet name="Eye-level" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">SBD_kpis!$A$2:$W$43</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">SBD_kpis!$A$2:$W$43</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">SBD_kpis!$A$2:$W$43</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">SBD_kpis!$A$2:$W$43</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">SBD_kpis!$A$2:$W$43</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">SBD_kpis!$A$2:$W$43</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">SBD_kpis!$A$2:$W$43</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$A$2:$W$43</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$A$2:$W$43</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$A$2:$W$43</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$A$2:$W$43</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$A$2:$W$43</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$A$2:$W$43</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">SBD_kpis!$A$2:$W$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">SBD_kpis!$A$2:$W$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">SBD_kpis!$A$2:$W$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">SBD_kpis!$A$2:$W$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">SBD_kpis!$A$2:$W$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">SBD_kpis!$A$2:$W$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">SBD_kpis!$A$2:$W$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$A$2:$W$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$A$2:$W$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$A$2:$W$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$A$2:$W$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$A$2:$W$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$A$2:$W$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$A$2:$W$42</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="124">
   <si>
     <t>General Data</t>
   </si>
@@ -160,144 +161,135 @@
     <t>Hair Care</t>
   </si>
   <si>
+    <t>Survey</t>
+  </si>
+  <si>
+    <t>Binary</t>
+  </si>
+  <si>
+    <t>survey question</t>
+  </si>
+  <si>
+    <t>question_text</t>
+  </si>
+  <si>
+    <t>Sunt SKU-urile de Pantene Gold plasate in mijlocul raftului de Pantene?</t>
+  </si>
+  <si>
+    <t>question_answer</t>
+  </si>
+  <si>
+    <t>Da</t>
+  </si>
+  <si>
+    <t>Are H&amp;S male skus placed in hair care main shelf?</t>
+  </si>
+  <si>
+    <t>Is Always Platinum min 15% of Always Pads shelf?</t>
+  </si>
+  <si>
+    <t>Fem</t>
+  </si>
+  <si>
+    <t>Brand=always and category=pads and form=Platinum out of Brand=always and alient sucategory=pads</t>
+  </si>
+  <si>
+    <t>ALWAYS</t>
+  </si>
+  <si>
+    <t>sub_category</t>
+  </si>
+  <si>
+    <t>PADS</t>
+  </si>
+  <si>
+    <t>Is Ariel Liquid Tabs min 15% from total Laundry category?</t>
+  </si>
+  <si>
+    <t>Laundry</t>
+  </si>
+  <si>
+    <t>Brand=Ariel and form=Liquid tabs out of Category=Laundry</t>
+  </si>
+  <si>
+    <t>Ariel</t>
+  </si>
+  <si>
+    <t>Liquid Tabs</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>LAUNDRY</t>
+  </si>
+  <si>
+    <t>Is Blue collection  min 30% from Lenor shelf?</t>
+  </si>
+  <si>
+    <t>Fabric Enhancers</t>
+  </si>
+  <si>
+    <t>Brand =Lenor and form=liquid and benefit = Spring out of Brand =lenor and form=liquid</t>
+  </si>
+  <si>
+    <t>Lenor</t>
+  </si>
+  <si>
+    <t>Liquid</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>Is Pants min 25% of Pampers shelf?</t>
+  </si>
+  <si>
+    <t>Baby</t>
+  </si>
+  <si>
+    <t>Category = diapers  and brand=pampers and form=taped out of category = diapers and brand=pampers</t>
+  </si>
+  <si>
+    <t>DIAPERS</t>
+  </si>
+  <si>
+    <t>PAMPERS</t>
+  </si>
+  <si>
+    <t>taped</t>
+  </si>
+  <si>
+    <t>POC listed and placed within brushing</t>
+  </si>
+  <si>
+    <t>Oral Care</t>
+  </si>
+  <si>
     <t>Relative Position</t>
   </si>
   <si>
-    <t>Brand = Pantene, Color = golden river. Placed in the middle of brand = Pantene.</t>
-  </si>
-  <si>
-    <t>Pantene</t>
-  </si>
-  <si>
-    <t>Color</t>
-  </si>
-  <si>
-    <t>golden river</t>
-  </si>
-  <si>
-    <t>Are H&amp;S male skus placed in hair care main shelf?</t>
-  </si>
-  <si>
-    <t>Survey</t>
-  </si>
-  <si>
-    <t>Binary</t>
-  </si>
-  <si>
-    <t>survey question</t>
-  </si>
-  <si>
-    <t>question_text</t>
+    <t>segment = poc(power oral care) and PG adjecent to toothbrush sub cat</t>
+  </si>
+  <si>
+    <t>Segment</t>
+  </si>
+  <si>
+    <t>poc</t>
+  </si>
+  <si>
+    <t>TOOTHBRUSH</t>
+  </si>
+  <si>
+    <t>Are Female Blades &amp; Razors placed in a distinct block than male Blades &amp; Razors?</t>
+  </si>
+  <si>
+    <t>Shave Care (Female)</t>
   </si>
   <si>
     <t>Sunt aparatele de ras si razoarele pentru femei plasate in bloc separat fata de cele pentru barbati?</t>
   </si>
   <si>
-    <t>question_answer</t>
-  </si>
-  <si>
-    <t>Da</t>
-  </si>
-  <si>
-    <t>Is Always Platinum min 15% of Always Pads shelf?</t>
-  </si>
-  <si>
-    <t>Fem</t>
-  </si>
-  <si>
-    <t>Brand=always and category=pads and form=Platinum out of Brand=always and alient sucategory=pads</t>
-  </si>
-  <si>
-    <t>ALWAYS</t>
-  </si>
-  <si>
-    <t>sub_category</t>
-  </si>
-  <si>
-    <t>PADS</t>
-  </si>
-  <si>
-    <t>Is Ariel Liquid Tabs min 15% from total Laundry category?</t>
-  </si>
-  <si>
-    <t>Laundry</t>
-  </si>
-  <si>
-    <t>Brand=Ariel and form=Liquid tabs out of Category=Laundry</t>
-  </si>
-  <si>
-    <t>Ariel</t>
-  </si>
-  <si>
-    <t>Liquid Tabs</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>LAUNDRY</t>
-  </si>
-  <si>
-    <t>Is Blue collection  min 30% from Lenor shelf?</t>
-  </si>
-  <si>
-    <t>Fabric Enhancers</t>
-  </si>
-  <si>
-    <t>Brand =Lenor and form=liquid and benefit = Spring out of Brand =lenor and form=liquid</t>
-  </si>
-  <si>
-    <t>Lenor</t>
-  </si>
-  <si>
-    <t>Liquid</t>
-  </si>
-  <si>
-    <t>Spring</t>
-  </si>
-  <si>
-    <t>Is Pants min 25% of Pampers shelf?</t>
-  </si>
-  <si>
-    <t>Baby</t>
-  </si>
-  <si>
-    <t>Category = diapers  and brand=pampers and form=taped out of category = diapers and brand=pampers</t>
-  </si>
-  <si>
-    <t>DIAPERS</t>
-  </si>
-  <si>
-    <t>PAMPERS</t>
-  </si>
-  <si>
-    <t>taped</t>
-  </si>
-  <si>
-    <t>POC listed and placed within brushing</t>
-  </si>
-  <si>
-    <t>Oral Care</t>
-  </si>
-  <si>
-    <t>segment = poc(power oral care) and PG adjecent to toothbrush sub cat</t>
-  </si>
-  <si>
-    <t>Segment</t>
-  </si>
-  <si>
-    <t>poc</t>
-  </si>
-  <si>
-    <t>TOOTHBRUSH</t>
-  </si>
-  <si>
-    <t>Are Female Blades &amp; Razors placed in a distinct block than male Blades &amp; Razors?</t>
-  </si>
-  <si>
-    <t>Shave Care (Female)</t>
-  </si>
-  <si>
     <t>POC listed and placed within eye-level</t>
   </si>
   <si>
@@ -310,7 +302,7 @@
     <t>ORAL CARE</t>
   </si>
   <si>
-    <t>See sheet 2</t>
+    <t>3,4,5</t>
   </si>
   <si>
     <t>display name</t>
@@ -401,9 +393,6 @@
   </si>
   <si>
     <t>CARREFOUR</t>
-  </si>
-  <si>
-    <t>3,4,5</t>
   </si>
   <si>
     <t>CARREFOUR M</t>
@@ -592,7 +581,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -637,10 +626,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -649,7 +634,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -657,12 +642,28 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -775,32 +776,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:14"/>
+  <dimension ref="1:13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I25" activeCellId="0" sqref="I25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="61.336032388664"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.7894736842105"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.1457489878543"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.6032388663968"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.3846153846154"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="20.3157894736842"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.2631578947368"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="14.4736842105263"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="75.5627530364373"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="23.9595141700405"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="16.3481781376518"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="25.7246963562753"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="16.3481781376518"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="10.834008097166"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="16.3481781376518"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="13.3765182186235"/>
-    <col collapsed="false" hidden="false" max="1020" min="17" style="1" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="1025" min="1021" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="61.8056680161943"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.9230769230769"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.1417004048583"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="76.1619433198381"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="24.2105263157895"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="10.8178137651822"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1020" min="17" style="1" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1025" min="1021" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -893,7 +894,7 @@
       <c r="AMI2" s="0"/>
       <c r="AMJ2" s="0"/>
     </row>
-    <row r="3" s="12" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="11" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
         <v>21</v>
       </c>
@@ -918,13 +919,13 @@
       <c r="J3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="10" t="s">
         <v>28</v>
       </c>
       <c r="L3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="M3" s="10" t="s">
         <v>30</v>
       </c>
       <c r="N3" s="10"/>
@@ -941,7 +942,7 @@
       <c r="AMI3" s="0"/>
       <c r="AMJ3" s="0"/>
     </row>
-    <row r="4" s="12" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
         <v>31</v>
       </c>
@@ -972,7 +973,7 @@
       <c r="L4" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="M4" s="13" t="s">
+      <c r="M4" s="12" t="s">
         <v>37</v>
       </c>
       <c r="N4" s="10"/>
@@ -980,20 +981,1016 @@
       <c r="P4" s="10" t="n">
         <v>40</v>
       </c>
+      <c r="Q4" s="0"/>
+      <c r="R4" s="0"/>
+      <c r="S4" s="0"/>
+      <c r="T4" s="0"/>
+      <c r="U4" s="0"/>
+      <c r="V4" s="0"/>
+      <c r="W4" s="0"/>
+      <c r="X4" s="0"/>
+      <c r="Y4" s="0"/>
+      <c r="Z4" s="0"/>
+      <c r="AA4" s="0"/>
+      <c r="AB4" s="0"/>
+      <c r="AC4" s="0"/>
+      <c r="AD4" s="0"/>
+      <c r="AE4" s="0"/>
+      <c r="AF4" s="0"/>
+      <c r="AG4" s="0"/>
+      <c r="AH4" s="0"/>
+      <c r="AI4" s="0"/>
+      <c r="AJ4" s="0"/>
+      <c r="AK4" s="0"/>
+      <c r="AL4" s="0"/>
+      <c r="AM4" s="0"/>
+      <c r="AN4" s="0"/>
+      <c r="AO4" s="0"/>
+      <c r="AP4" s="0"/>
+      <c r="AQ4" s="0"/>
+      <c r="AR4" s="0"/>
+      <c r="AS4" s="0"/>
+      <c r="AT4" s="0"/>
+      <c r="AU4" s="0"/>
+      <c r="AV4" s="0"/>
+      <c r="AW4" s="0"/>
+      <c r="AX4" s="0"/>
+      <c r="AY4" s="0"/>
+      <c r="AZ4" s="0"/>
+      <c r="BA4" s="0"/>
+      <c r="BB4" s="0"/>
+      <c r="BC4" s="0"/>
+      <c r="BD4" s="0"/>
+      <c r="BE4" s="0"/>
+      <c r="BF4" s="0"/>
+      <c r="BG4" s="0"/>
+      <c r="BH4" s="0"/>
+      <c r="BI4" s="0"/>
+      <c r="BJ4" s="0"/>
+      <c r="BK4" s="0"/>
+      <c r="BL4" s="0"/>
+      <c r="BM4" s="0"/>
+      <c r="BN4" s="0"/>
+      <c r="BO4" s="0"/>
+      <c r="BP4" s="0"/>
+      <c r="BQ4" s="0"/>
+      <c r="BR4" s="0"/>
+      <c r="BS4" s="0"/>
+      <c r="BT4" s="0"/>
+      <c r="BU4" s="0"/>
+      <c r="BV4" s="0"/>
+      <c r="BW4" s="0"/>
+      <c r="BX4" s="0"/>
+      <c r="BY4" s="0"/>
+      <c r="BZ4" s="0"/>
+      <c r="CA4" s="0"/>
+      <c r="CB4" s="0"/>
+      <c r="CC4" s="0"/>
+      <c r="CD4" s="0"/>
+      <c r="CE4" s="0"/>
+      <c r="CF4" s="0"/>
+      <c r="CG4" s="0"/>
+      <c r="CH4" s="0"/>
+      <c r="CI4" s="0"/>
+      <c r="CJ4" s="0"/>
+      <c r="CK4" s="0"/>
+      <c r="CL4" s="0"/>
+      <c r="CM4" s="0"/>
+      <c r="CN4" s="0"/>
+      <c r="CO4" s="0"/>
+      <c r="CP4" s="0"/>
+      <c r="CQ4" s="0"/>
+      <c r="CR4" s="0"/>
+      <c r="CS4" s="0"/>
+      <c r="CT4" s="0"/>
+      <c r="CU4" s="0"/>
+      <c r="CV4" s="0"/>
+      <c r="CW4" s="0"/>
+      <c r="CX4" s="0"/>
+      <c r="CY4" s="0"/>
+      <c r="CZ4" s="0"/>
+      <c r="DA4" s="0"/>
+      <c r="DB4" s="0"/>
+      <c r="DC4" s="0"/>
+      <c r="DD4" s="0"/>
+      <c r="DE4" s="0"/>
+      <c r="DF4" s="0"/>
+      <c r="DG4" s="0"/>
+      <c r="DH4" s="0"/>
+      <c r="DI4" s="0"/>
+      <c r="DJ4" s="0"/>
+      <c r="DK4" s="0"/>
+      <c r="DL4" s="0"/>
+      <c r="DM4" s="0"/>
+      <c r="DN4" s="0"/>
+      <c r="DO4" s="0"/>
+      <c r="DP4" s="0"/>
+      <c r="DQ4" s="0"/>
+      <c r="DR4" s="0"/>
+      <c r="DS4" s="0"/>
+      <c r="DT4" s="0"/>
+      <c r="DU4" s="0"/>
+      <c r="DV4" s="0"/>
+      <c r="DW4" s="0"/>
+      <c r="DX4" s="0"/>
+      <c r="DY4" s="0"/>
+      <c r="DZ4" s="0"/>
+      <c r="EA4" s="0"/>
+      <c r="EB4" s="0"/>
+      <c r="EC4" s="0"/>
+      <c r="ED4" s="0"/>
+      <c r="EE4" s="0"/>
+      <c r="EF4" s="0"/>
+      <c r="EG4" s="0"/>
+      <c r="EH4" s="0"/>
+      <c r="EI4" s="0"/>
+      <c r="EJ4" s="0"/>
+      <c r="EK4" s="0"/>
+      <c r="EL4" s="0"/>
+      <c r="EM4" s="0"/>
+      <c r="EN4" s="0"/>
+      <c r="EO4" s="0"/>
+      <c r="EP4" s="0"/>
+      <c r="EQ4" s="0"/>
+      <c r="ER4" s="0"/>
+      <c r="ES4" s="0"/>
+      <c r="ET4" s="0"/>
+      <c r="EU4" s="0"/>
+      <c r="EV4" s="0"/>
+      <c r="EW4" s="0"/>
+      <c r="EX4" s="0"/>
+      <c r="EY4" s="0"/>
+      <c r="EZ4" s="0"/>
+      <c r="FA4" s="0"/>
+      <c r="FB4" s="0"/>
+      <c r="FC4" s="0"/>
+      <c r="FD4" s="0"/>
+      <c r="FE4" s="0"/>
+      <c r="FF4" s="0"/>
+      <c r="FG4" s="0"/>
+      <c r="FH4" s="0"/>
+      <c r="FI4" s="0"/>
+      <c r="FJ4" s="0"/>
+      <c r="FK4" s="0"/>
+      <c r="FL4" s="0"/>
+      <c r="FM4" s="0"/>
+      <c r="FN4" s="0"/>
+      <c r="FO4" s="0"/>
+      <c r="FP4" s="0"/>
+      <c r="FQ4" s="0"/>
+      <c r="FR4" s="0"/>
+      <c r="FS4" s="0"/>
+      <c r="FT4" s="0"/>
+      <c r="FU4" s="0"/>
+      <c r="FV4" s="0"/>
+      <c r="FW4" s="0"/>
+      <c r="FX4" s="0"/>
+      <c r="FY4" s="0"/>
+      <c r="FZ4" s="0"/>
+      <c r="GA4" s="0"/>
+      <c r="GB4" s="0"/>
+      <c r="GC4" s="0"/>
+      <c r="GD4" s="0"/>
+      <c r="GE4" s="0"/>
+      <c r="GF4" s="0"/>
+      <c r="GG4" s="0"/>
+      <c r="GH4" s="0"/>
+      <c r="GI4" s="0"/>
+      <c r="GJ4" s="0"/>
+      <c r="GK4" s="0"/>
+      <c r="GL4" s="0"/>
+      <c r="GM4" s="0"/>
+      <c r="GN4" s="0"/>
+      <c r="GO4" s="0"/>
+      <c r="GP4" s="0"/>
+      <c r="GQ4" s="0"/>
+      <c r="GR4" s="0"/>
+      <c r="GS4" s="0"/>
+      <c r="GT4" s="0"/>
+      <c r="GU4" s="0"/>
+      <c r="GV4" s="0"/>
+      <c r="GW4" s="0"/>
+      <c r="GX4" s="0"/>
+      <c r="GY4" s="0"/>
+      <c r="GZ4" s="0"/>
+      <c r="HA4" s="0"/>
+      <c r="HB4" s="0"/>
+      <c r="HC4" s="0"/>
+      <c r="HD4" s="0"/>
+      <c r="HE4" s="0"/>
+      <c r="HF4" s="0"/>
+      <c r="HG4" s="0"/>
+      <c r="HH4" s="0"/>
+      <c r="HI4" s="0"/>
+      <c r="HJ4" s="0"/>
+      <c r="HK4" s="0"/>
+      <c r="HL4" s="0"/>
+      <c r="HM4" s="0"/>
+      <c r="HN4" s="0"/>
+      <c r="HO4" s="0"/>
+      <c r="HP4" s="0"/>
+      <c r="HQ4" s="0"/>
+      <c r="HR4" s="0"/>
+      <c r="HS4" s="0"/>
+      <c r="HT4" s="0"/>
+      <c r="HU4" s="0"/>
+      <c r="HV4" s="0"/>
+      <c r="HW4" s="0"/>
+      <c r="HX4" s="0"/>
+      <c r="HY4" s="0"/>
+      <c r="HZ4" s="0"/>
+      <c r="IA4" s="0"/>
+      <c r="IB4" s="0"/>
+      <c r="IC4" s="0"/>
+      <c r="ID4" s="0"/>
+      <c r="IE4" s="0"/>
+      <c r="IF4" s="0"/>
+      <c r="IG4" s="0"/>
+      <c r="IH4" s="0"/>
+      <c r="II4" s="0"/>
+      <c r="IJ4" s="0"/>
+      <c r="IK4" s="0"/>
+      <c r="IL4" s="0"/>
+      <c r="IM4" s="0"/>
+      <c r="IN4" s="0"/>
+      <c r="IO4" s="0"/>
+      <c r="IP4" s="0"/>
+      <c r="IQ4" s="0"/>
+      <c r="IR4" s="0"/>
+      <c r="IS4" s="0"/>
+      <c r="IT4" s="0"/>
+      <c r="IU4" s="0"/>
+      <c r="IV4" s="0"/>
+      <c r="IW4" s="0"/>
+      <c r="IX4" s="0"/>
+      <c r="IY4" s="0"/>
+      <c r="IZ4" s="0"/>
+      <c r="JA4" s="0"/>
+      <c r="JB4" s="0"/>
+      <c r="JC4" s="0"/>
+      <c r="JD4" s="0"/>
+      <c r="JE4" s="0"/>
+      <c r="JF4" s="0"/>
+      <c r="JG4" s="0"/>
+      <c r="JH4" s="0"/>
+      <c r="JI4" s="0"/>
+      <c r="JJ4" s="0"/>
+      <c r="JK4" s="0"/>
+      <c r="JL4" s="0"/>
+      <c r="JM4" s="0"/>
+      <c r="JN4" s="0"/>
+      <c r="JO4" s="0"/>
+      <c r="JP4" s="0"/>
+      <c r="JQ4" s="0"/>
+      <c r="JR4" s="0"/>
+      <c r="JS4" s="0"/>
+      <c r="JT4" s="0"/>
+      <c r="JU4" s="0"/>
+      <c r="JV4" s="0"/>
+      <c r="JW4" s="0"/>
+      <c r="JX4" s="0"/>
+      <c r="JY4" s="0"/>
+      <c r="JZ4" s="0"/>
+      <c r="KA4" s="0"/>
+      <c r="KB4" s="0"/>
+      <c r="KC4" s="0"/>
+      <c r="KD4" s="0"/>
+      <c r="KE4" s="0"/>
+      <c r="KF4" s="0"/>
+      <c r="KG4" s="0"/>
+      <c r="KH4" s="0"/>
+      <c r="KI4" s="0"/>
+      <c r="KJ4" s="0"/>
+      <c r="KK4" s="0"/>
+      <c r="KL4" s="0"/>
+      <c r="KM4" s="0"/>
+      <c r="KN4" s="0"/>
+      <c r="KO4" s="0"/>
+      <c r="KP4" s="0"/>
+      <c r="KQ4" s="0"/>
+      <c r="KR4" s="0"/>
+      <c r="KS4" s="0"/>
+      <c r="KT4" s="0"/>
+      <c r="KU4" s="0"/>
+      <c r="KV4" s="0"/>
+      <c r="KW4" s="0"/>
+      <c r="KX4" s="0"/>
+      <c r="KY4" s="0"/>
+      <c r="KZ4" s="0"/>
+      <c r="LA4" s="0"/>
+      <c r="LB4" s="0"/>
+      <c r="LC4" s="0"/>
+      <c r="LD4" s="0"/>
+      <c r="LE4" s="0"/>
+      <c r="LF4" s="0"/>
+      <c r="LG4" s="0"/>
+      <c r="LH4" s="0"/>
+      <c r="LI4" s="0"/>
+      <c r="LJ4" s="0"/>
+      <c r="LK4" s="0"/>
+      <c r="LL4" s="0"/>
+      <c r="LM4" s="0"/>
+      <c r="LN4" s="0"/>
+      <c r="LO4" s="0"/>
+      <c r="LP4" s="0"/>
+      <c r="LQ4" s="0"/>
+      <c r="LR4" s="0"/>
+      <c r="LS4" s="0"/>
+      <c r="LT4" s="0"/>
+      <c r="LU4" s="0"/>
+      <c r="LV4" s="0"/>
+      <c r="LW4" s="0"/>
+      <c r="LX4" s="0"/>
+      <c r="LY4" s="0"/>
+      <c r="LZ4" s="0"/>
+      <c r="MA4" s="0"/>
+      <c r="MB4" s="0"/>
+      <c r="MC4" s="0"/>
+      <c r="MD4" s="0"/>
+      <c r="ME4" s="0"/>
+      <c r="MF4" s="0"/>
+      <c r="MG4" s="0"/>
+      <c r="MH4" s="0"/>
+      <c r="MI4" s="0"/>
+      <c r="MJ4" s="0"/>
+      <c r="MK4" s="0"/>
+      <c r="ML4" s="0"/>
+      <c r="MM4" s="0"/>
+      <c r="MN4" s="0"/>
+      <c r="MO4" s="0"/>
+      <c r="MP4" s="0"/>
+      <c r="MQ4" s="0"/>
+      <c r="MR4" s="0"/>
+      <c r="MS4" s="0"/>
+      <c r="MT4" s="0"/>
+      <c r="MU4" s="0"/>
+      <c r="MV4" s="0"/>
+      <c r="MW4" s="0"/>
+      <c r="MX4" s="0"/>
+      <c r="MY4" s="0"/>
+      <c r="MZ4" s="0"/>
+      <c r="NA4" s="0"/>
+      <c r="NB4" s="0"/>
+      <c r="NC4" s="0"/>
+      <c r="ND4" s="0"/>
+      <c r="NE4" s="0"/>
+      <c r="NF4" s="0"/>
+      <c r="NG4" s="0"/>
+      <c r="NH4" s="0"/>
+      <c r="NI4" s="0"/>
+      <c r="NJ4" s="0"/>
+      <c r="NK4" s="0"/>
+      <c r="NL4" s="0"/>
+      <c r="NM4" s="0"/>
+      <c r="NN4" s="0"/>
+      <c r="NO4" s="0"/>
+      <c r="NP4" s="0"/>
+      <c r="NQ4" s="0"/>
+      <c r="NR4" s="0"/>
+      <c r="NS4" s="0"/>
+      <c r="NT4" s="0"/>
+      <c r="NU4" s="0"/>
+      <c r="NV4" s="0"/>
+      <c r="NW4" s="0"/>
+      <c r="NX4" s="0"/>
+      <c r="NY4" s="0"/>
+      <c r="NZ4" s="0"/>
+      <c r="OA4" s="0"/>
+      <c r="OB4" s="0"/>
+      <c r="OC4" s="0"/>
+      <c r="OD4" s="0"/>
+      <c r="OE4" s="0"/>
+      <c r="OF4" s="0"/>
+      <c r="OG4" s="0"/>
+      <c r="OH4" s="0"/>
+      <c r="OI4" s="0"/>
+      <c r="OJ4" s="0"/>
+      <c r="OK4" s="0"/>
+      <c r="OL4" s="0"/>
+      <c r="OM4" s="0"/>
+      <c r="ON4" s="0"/>
+      <c r="OO4" s="0"/>
+      <c r="OP4" s="0"/>
+      <c r="OQ4" s="0"/>
+      <c r="OR4" s="0"/>
+      <c r="OS4" s="0"/>
+      <c r="OT4" s="0"/>
+      <c r="OU4" s="0"/>
+      <c r="OV4" s="0"/>
+      <c r="OW4" s="0"/>
+      <c r="OX4" s="0"/>
+      <c r="OY4" s="0"/>
+      <c r="OZ4" s="0"/>
+      <c r="PA4" s="0"/>
+      <c r="PB4" s="0"/>
+      <c r="PC4" s="0"/>
+      <c r="PD4" s="0"/>
+      <c r="PE4" s="0"/>
+      <c r="PF4" s="0"/>
+      <c r="PG4" s="0"/>
+      <c r="PH4" s="0"/>
+      <c r="PI4" s="0"/>
+      <c r="PJ4" s="0"/>
+      <c r="PK4" s="0"/>
+      <c r="PL4" s="0"/>
+      <c r="PM4" s="0"/>
+      <c r="PN4" s="0"/>
+      <c r="PO4" s="0"/>
+      <c r="PP4" s="0"/>
+      <c r="PQ4" s="0"/>
+      <c r="PR4" s="0"/>
+      <c r="PS4" s="0"/>
+      <c r="PT4" s="0"/>
+      <c r="PU4" s="0"/>
+      <c r="PV4" s="0"/>
+      <c r="PW4" s="0"/>
+      <c r="PX4" s="0"/>
+      <c r="PY4" s="0"/>
+      <c r="PZ4" s="0"/>
+      <c r="QA4" s="0"/>
+      <c r="QB4" s="0"/>
+      <c r="QC4" s="0"/>
+      <c r="QD4" s="0"/>
+      <c r="QE4" s="0"/>
+      <c r="QF4" s="0"/>
+      <c r="QG4" s="0"/>
+      <c r="QH4" s="0"/>
+      <c r="QI4" s="0"/>
+      <c r="QJ4" s="0"/>
+      <c r="QK4" s="0"/>
+      <c r="QL4" s="0"/>
+      <c r="QM4" s="0"/>
+      <c r="QN4" s="0"/>
+      <c r="QO4" s="0"/>
+      <c r="QP4" s="0"/>
+      <c r="QQ4" s="0"/>
+      <c r="QR4" s="0"/>
+      <c r="QS4" s="0"/>
+      <c r="QT4" s="0"/>
+      <c r="QU4" s="0"/>
+      <c r="QV4" s="0"/>
+      <c r="QW4" s="0"/>
+      <c r="QX4" s="0"/>
+      <c r="QY4" s="0"/>
+      <c r="QZ4" s="0"/>
+      <c r="RA4" s="0"/>
+      <c r="RB4" s="0"/>
+      <c r="RC4" s="0"/>
+      <c r="RD4" s="0"/>
+      <c r="RE4" s="0"/>
+      <c r="RF4" s="0"/>
+      <c r="RG4" s="0"/>
+      <c r="RH4" s="0"/>
+      <c r="RI4" s="0"/>
+      <c r="RJ4" s="0"/>
+      <c r="RK4" s="0"/>
+      <c r="RL4" s="0"/>
+      <c r="RM4" s="0"/>
+      <c r="RN4" s="0"/>
+      <c r="RO4" s="0"/>
+      <c r="RP4" s="0"/>
+      <c r="RQ4" s="0"/>
+      <c r="RR4" s="0"/>
+      <c r="RS4" s="0"/>
+      <c r="RT4" s="0"/>
+      <c r="RU4" s="0"/>
+      <c r="RV4" s="0"/>
+      <c r="RW4" s="0"/>
+      <c r="RX4" s="0"/>
+      <c r="RY4" s="0"/>
+      <c r="RZ4" s="0"/>
+      <c r="SA4" s="0"/>
+      <c r="SB4" s="0"/>
+      <c r="SC4" s="0"/>
+      <c r="SD4" s="0"/>
+      <c r="SE4" s="0"/>
+      <c r="SF4" s="0"/>
+      <c r="SG4" s="0"/>
+      <c r="SH4" s="0"/>
+      <c r="SI4" s="0"/>
+      <c r="SJ4" s="0"/>
+      <c r="SK4" s="0"/>
+      <c r="SL4" s="0"/>
+      <c r="SM4" s="0"/>
+      <c r="SN4" s="0"/>
+      <c r="SO4" s="0"/>
+      <c r="SP4" s="0"/>
+      <c r="SQ4" s="0"/>
+      <c r="SR4" s="0"/>
+      <c r="SS4" s="0"/>
+      <c r="ST4" s="0"/>
+      <c r="SU4" s="0"/>
+      <c r="SV4" s="0"/>
+      <c r="SW4" s="0"/>
+      <c r="SX4" s="0"/>
+      <c r="SY4" s="0"/>
+      <c r="SZ4" s="0"/>
+      <c r="TA4" s="0"/>
+      <c r="TB4" s="0"/>
+      <c r="TC4" s="0"/>
+      <c r="TD4" s="0"/>
+      <c r="TE4" s="0"/>
+      <c r="TF4" s="0"/>
+      <c r="TG4" s="0"/>
+      <c r="TH4" s="0"/>
+      <c r="TI4" s="0"/>
+      <c r="TJ4" s="0"/>
+      <c r="TK4" s="0"/>
+      <c r="TL4" s="0"/>
+      <c r="TM4" s="0"/>
+      <c r="TN4" s="0"/>
+      <c r="TO4" s="0"/>
+      <c r="TP4" s="0"/>
+      <c r="TQ4" s="0"/>
+      <c r="TR4" s="0"/>
+      <c r="TS4" s="0"/>
+      <c r="TT4" s="0"/>
+      <c r="TU4" s="0"/>
+      <c r="TV4" s="0"/>
+      <c r="TW4" s="0"/>
+      <c r="TX4" s="0"/>
+      <c r="TY4" s="0"/>
+      <c r="TZ4" s="0"/>
+      <c r="UA4" s="0"/>
+      <c r="UB4" s="0"/>
+      <c r="UC4" s="0"/>
+      <c r="UD4" s="0"/>
+      <c r="UE4" s="0"/>
+      <c r="UF4" s="0"/>
+      <c r="UG4" s="0"/>
+      <c r="UH4" s="0"/>
+      <c r="UI4" s="0"/>
+      <c r="UJ4" s="0"/>
+      <c r="UK4" s="0"/>
+      <c r="UL4" s="0"/>
+      <c r="UM4" s="0"/>
+      <c r="UN4" s="0"/>
+      <c r="UO4" s="0"/>
+      <c r="UP4" s="0"/>
+      <c r="UQ4" s="0"/>
+      <c r="UR4" s="0"/>
+      <c r="US4" s="0"/>
+      <c r="UT4" s="0"/>
+      <c r="UU4" s="0"/>
+      <c r="UV4" s="0"/>
+      <c r="UW4" s="0"/>
+      <c r="UX4" s="0"/>
+      <c r="UY4" s="0"/>
+      <c r="UZ4" s="0"/>
+      <c r="VA4" s="0"/>
+      <c r="VB4" s="0"/>
+      <c r="VC4" s="0"/>
+      <c r="VD4" s="0"/>
+      <c r="VE4" s="0"/>
+      <c r="VF4" s="0"/>
+      <c r="VG4" s="0"/>
+      <c r="VH4" s="0"/>
+      <c r="VI4" s="0"/>
+      <c r="VJ4" s="0"/>
+      <c r="VK4" s="0"/>
+      <c r="VL4" s="0"/>
+      <c r="VM4" s="0"/>
+      <c r="VN4" s="0"/>
+      <c r="VO4" s="0"/>
+      <c r="VP4" s="0"/>
+      <c r="VQ4" s="0"/>
+      <c r="VR4" s="0"/>
+      <c r="VS4" s="0"/>
+      <c r="VT4" s="0"/>
+      <c r="VU4" s="0"/>
+      <c r="VV4" s="0"/>
+      <c r="VW4" s="0"/>
+      <c r="VX4" s="0"/>
+      <c r="VY4" s="0"/>
+      <c r="VZ4" s="0"/>
+      <c r="WA4" s="0"/>
+      <c r="WB4" s="0"/>
+      <c r="WC4" s="0"/>
+      <c r="WD4" s="0"/>
+      <c r="WE4" s="0"/>
+      <c r="WF4" s="0"/>
+      <c r="WG4" s="0"/>
+      <c r="WH4" s="0"/>
+      <c r="WI4" s="0"/>
+      <c r="WJ4" s="0"/>
+      <c r="WK4" s="0"/>
+      <c r="WL4" s="0"/>
+      <c r="WM4" s="0"/>
+      <c r="WN4" s="0"/>
+      <c r="WO4" s="0"/>
+      <c r="WP4" s="0"/>
+      <c r="WQ4" s="0"/>
+      <c r="WR4" s="0"/>
+      <c r="WS4" s="0"/>
+      <c r="WT4" s="0"/>
+      <c r="WU4" s="0"/>
+      <c r="WV4" s="0"/>
+      <c r="WW4" s="0"/>
+      <c r="WX4" s="0"/>
+      <c r="WY4" s="0"/>
+      <c r="WZ4" s="0"/>
+      <c r="XA4" s="0"/>
+      <c r="XB4" s="0"/>
+      <c r="XC4" s="0"/>
+      <c r="XD4" s="0"/>
+      <c r="XE4" s="0"/>
+      <c r="XF4" s="0"/>
+      <c r="XG4" s="0"/>
+      <c r="XH4" s="0"/>
+      <c r="XI4" s="0"/>
+      <c r="XJ4" s="0"/>
+      <c r="XK4" s="0"/>
+      <c r="XL4" s="0"/>
+      <c r="XM4" s="0"/>
+      <c r="XN4" s="0"/>
+      <c r="XO4" s="0"/>
+      <c r="XP4" s="0"/>
+      <c r="XQ4" s="0"/>
+      <c r="XR4" s="0"/>
+      <c r="XS4" s="0"/>
+      <c r="XT4" s="0"/>
+      <c r="XU4" s="0"/>
+      <c r="XV4" s="0"/>
+      <c r="XW4" s="0"/>
+      <c r="XX4" s="0"/>
+      <c r="XY4" s="0"/>
+      <c r="XZ4" s="0"/>
+      <c r="YA4" s="0"/>
+      <c r="YB4" s="0"/>
+      <c r="YC4" s="0"/>
+      <c r="YD4" s="0"/>
+      <c r="YE4" s="0"/>
+      <c r="YF4" s="0"/>
+      <c r="YG4" s="0"/>
+      <c r="YH4" s="0"/>
+      <c r="YI4" s="0"/>
+      <c r="YJ4" s="0"/>
+      <c r="YK4" s="0"/>
+      <c r="YL4" s="0"/>
+      <c r="YM4" s="0"/>
+      <c r="YN4" s="0"/>
+      <c r="YO4" s="0"/>
+      <c r="YP4" s="0"/>
+      <c r="YQ4" s="0"/>
+      <c r="YR4" s="0"/>
+      <c r="YS4" s="0"/>
+      <c r="YT4" s="0"/>
+      <c r="YU4" s="0"/>
+      <c r="YV4" s="0"/>
+      <c r="YW4" s="0"/>
+      <c r="YX4" s="0"/>
+      <c r="YY4" s="0"/>
+      <c r="YZ4" s="0"/>
+      <c r="ZA4" s="0"/>
+      <c r="ZB4" s="0"/>
+      <c r="ZC4" s="0"/>
+      <c r="ZD4" s="0"/>
+      <c r="ZE4" s="0"/>
+      <c r="ZF4" s="0"/>
+      <c r="ZG4" s="0"/>
+      <c r="ZH4" s="0"/>
+      <c r="ZI4" s="0"/>
+      <c r="ZJ4" s="0"/>
+      <c r="ZK4" s="0"/>
+      <c r="ZL4" s="0"/>
+      <c r="ZM4" s="0"/>
+      <c r="ZN4" s="0"/>
+      <c r="ZO4" s="0"/>
+      <c r="ZP4" s="0"/>
+      <c r="ZQ4" s="0"/>
+      <c r="ZR4" s="0"/>
+      <c r="ZS4" s="0"/>
+      <c r="ZT4" s="0"/>
+      <c r="ZU4" s="0"/>
+      <c r="ZV4" s="0"/>
+      <c r="ZW4" s="0"/>
+      <c r="ZX4" s="0"/>
+      <c r="ZY4" s="0"/>
+      <c r="ZZ4" s="0"/>
+      <c r="AAA4" s="0"/>
+      <c r="AAB4" s="0"/>
+      <c r="AAC4" s="0"/>
+      <c r="AAD4" s="0"/>
+      <c r="AAE4" s="0"/>
+      <c r="AAF4" s="0"/>
+      <c r="AAG4" s="0"/>
+      <c r="AAH4" s="0"/>
+      <c r="AAI4" s="0"/>
+      <c r="AAJ4" s="0"/>
+      <c r="AAK4" s="0"/>
+      <c r="AAL4" s="0"/>
+      <c r="AAM4" s="0"/>
+      <c r="AAN4" s="0"/>
+      <c r="AAO4" s="0"/>
+      <c r="AAP4" s="0"/>
+      <c r="AAQ4" s="0"/>
+      <c r="AAR4" s="0"/>
+      <c r="AAS4" s="0"/>
+      <c r="AAT4" s="0"/>
+      <c r="AAU4" s="0"/>
+      <c r="AAV4" s="0"/>
+      <c r="AAW4" s="0"/>
+      <c r="AAX4" s="0"/>
+      <c r="AAY4" s="0"/>
+      <c r="AAZ4" s="0"/>
+      <c r="ABA4" s="0"/>
+      <c r="ABB4" s="0"/>
+      <c r="ABC4" s="0"/>
+      <c r="ABD4" s="0"/>
+      <c r="ABE4" s="0"/>
+      <c r="ABF4" s="0"/>
+      <c r="ABG4" s="0"/>
+      <c r="ABH4" s="0"/>
+      <c r="ABI4" s="0"/>
+      <c r="ABJ4" s="0"/>
+      <c r="ABK4" s="0"/>
+      <c r="ABL4" s="0"/>
+      <c r="ABM4" s="0"/>
+      <c r="ABN4" s="0"/>
+      <c r="ABO4" s="0"/>
+      <c r="ABP4" s="0"/>
+      <c r="ABQ4" s="0"/>
+      <c r="ABR4" s="0"/>
+      <c r="ABS4" s="0"/>
+      <c r="ABT4" s="0"/>
+      <c r="ABU4" s="0"/>
+      <c r="ABV4" s="0"/>
+      <c r="ABW4" s="0"/>
+      <c r="ABX4" s="0"/>
+      <c r="ABY4" s="0"/>
+      <c r="ABZ4" s="0"/>
+      <c r="ACA4" s="0"/>
+      <c r="ACB4" s="0"/>
+      <c r="ACC4" s="0"/>
+      <c r="ACD4" s="0"/>
+      <c r="ACE4" s="0"/>
+      <c r="ACF4" s="0"/>
+      <c r="ACG4" s="0"/>
+      <c r="ACH4" s="0"/>
+      <c r="ACI4" s="0"/>
+      <c r="ACJ4" s="0"/>
+      <c r="ACK4" s="0"/>
+      <c r="ACL4" s="0"/>
+      <c r="ACM4" s="0"/>
+      <c r="ACN4" s="0"/>
+      <c r="ACO4" s="0"/>
+      <c r="ACP4" s="0"/>
+      <c r="ACQ4" s="0"/>
+      <c r="ACR4" s="0"/>
+      <c r="ACS4" s="0"/>
+      <c r="ACT4" s="0"/>
+      <c r="ACU4" s="0"/>
+      <c r="ACV4" s="0"/>
+      <c r="ACW4" s="0"/>
+      <c r="ACX4" s="0"/>
+      <c r="ACY4" s="0"/>
+      <c r="ACZ4" s="0"/>
+      <c r="ADA4" s="0"/>
+      <c r="ADB4" s="0"/>
+      <c r="ADC4" s="0"/>
+      <c r="ADD4" s="0"/>
+      <c r="ADE4" s="0"/>
+      <c r="ADF4" s="0"/>
+      <c r="ADG4" s="0"/>
+      <c r="ADH4" s="0"/>
+      <c r="ADI4" s="0"/>
+      <c r="ADJ4" s="0"/>
+      <c r="ADK4" s="0"/>
+      <c r="ADL4" s="0"/>
+      <c r="ADM4" s="0"/>
+      <c r="ADN4" s="0"/>
+      <c r="ADO4" s="0"/>
+      <c r="ADP4" s="0"/>
+      <c r="ADQ4" s="0"/>
+      <c r="ADR4" s="0"/>
+      <c r="ADS4" s="0"/>
+      <c r="ADT4" s="0"/>
+      <c r="ADU4" s="0"/>
+      <c r="ADV4" s="0"/>
+      <c r="ADW4" s="0"/>
+      <c r="ADX4" s="0"/>
+      <c r="ADY4" s="0"/>
+      <c r="ADZ4" s="0"/>
+      <c r="AEA4" s="0"/>
+      <c r="AEB4" s="0"/>
+      <c r="AEC4" s="0"/>
+      <c r="AED4" s="0"/>
+      <c r="AEE4" s="0"/>
+      <c r="AEF4" s="0"/>
+      <c r="AEG4" s="0"/>
+      <c r="AEH4" s="0"/>
+      <c r="AEI4" s="0"/>
+      <c r="AEJ4" s="0"/>
+      <c r="AEK4" s="0"/>
+      <c r="AEL4" s="0"/>
+      <c r="AEM4" s="0"/>
+      <c r="AEN4" s="0"/>
+      <c r="AEO4" s="0"/>
+      <c r="AEP4" s="0"/>
+      <c r="AEQ4" s="0"/>
+      <c r="AER4" s="0"/>
+      <c r="AES4" s="0"/>
+      <c r="AET4" s="0"/>
+      <c r="AEU4" s="0"/>
+      <c r="AEV4" s="0"/>
+      <c r="AEW4" s="0"/>
+      <c r="AEX4" s="0"/>
+      <c r="AEY4" s="0"/>
+      <c r="AEZ4" s="0"/>
+      <c r="AFA4" s="0"/>
+      <c r="AFB4" s="0"/>
+      <c r="AFC4" s="0"/>
+      <c r="AFD4" s="0"/>
+      <c r="AFE4" s="0"/>
+      <c r="AFF4" s="0"/>
+      <c r="AFG4" s="0"/>
+      <c r="AFH4" s="0"/>
+      <c r="AFI4" s="0"/>
+      <c r="AFJ4" s="0"/>
+      <c r="AFK4" s="0"/>
+      <c r="AFL4" s="0"/>
+      <c r="AFM4" s="0"/>
+      <c r="AFN4" s="0"/>
+      <c r="AFO4" s="0"/>
+      <c r="AFP4" s="0"/>
+      <c r="AFQ4" s="0"/>
+      <c r="AFR4" s="0"/>
+      <c r="AFS4" s="0"/>
+      <c r="AFT4" s="0"/>
+      <c r="AFU4" s="0"/>
+      <c r="AFV4" s="0"/>
+      <c r="AFW4" s="0"/>
+      <c r="AFX4" s="0"/>
+      <c r="AFY4" s="0"/>
+      <c r="AFZ4" s="0"/>
+      <c r="AGA4" s="0"/>
+      <c r="AGB4" s="0"/>
+      <c r="AGC4" s="0"/>
+      <c r="AGD4" s="0"/>
+      <c r="AGE4" s="0"/>
+      <c r="AGF4" s="0"/>
+      <c r="AGG4" s="0"/>
+      <c r="AGH4" s="0"/>
+      <c r="AGI4" s="0"/>
+      <c r="AGJ4" s="0"/>
+      <c r="AGK4" s="0"/>
+      <c r="AGL4" s="0"/>
+      <c r="AGM4" s="0"/>
+      <c r="AGN4" s="0"/>
+      <c r="AGO4" s="0"/>
+      <c r="AGP4" s="0"/>
+      <c r="AGQ4" s="0"/>
+      <c r="AGR4" s="0"/>
+      <c r="AGS4" s="0"/>
+      <c r="AGT4" s="0"/>
+      <c r="AGU4" s="0"/>
+      <c r="AGV4" s="0"/>
+      <c r="AGW4" s="0"/>
+      <c r="AGX4" s="0"/>
+      <c r="AGY4" s="0"/>
+      <c r="AGZ4" s="0"/>
+      <c r="AHA4" s="0"/>
+      <c r="AHB4" s="0"/>
+      <c r="AHC4" s="0"/>
+      <c r="AHD4" s="0"/>
+      <c r="AHE4" s="0"/>
+      <c r="AHF4" s="0"/>
+      <c r="AHG4" s="0"/>
+      <c r="AHH4" s="0"/>
+      <c r="AHI4" s="0"/>
+      <c r="AHJ4" s="0"/>
+      <c r="AHK4" s="0"/>
+      <c r="AHL4" s="0"/>
+      <c r="AHM4" s="0"/>
+      <c r="AHN4" s="0"/>
+      <c r="AHO4" s="0"/>
+      <c r="AHP4" s="0"/>
+      <c r="AHQ4" s="0"/>
+      <c r="AHR4" s="0"/>
+      <c r="AHS4" s="0"/>
+      <c r="AHT4" s="0"/>
+      <c r="AHU4" s="0"/>
+      <c r="AHV4" s="0"/>
+      <c r="AHW4" s="0"/>
+      <c r="AHX4" s="0"/>
+      <c r="AHY4" s="0"/>
+      <c r="AHZ4" s="0"/>
+      <c r="AIA4" s="0"/>
+      <c r="AIB4" s="0"/>
+      <c r="AIC4" s="0"/>
+      <c r="AID4" s="0"/>
+      <c r="AIE4" s="0"/>
+      <c r="AIF4" s="0"/>
+      <c r="AIG4" s="0"/>
+      <c r="AIH4" s="0"/>
+      <c r="AII4" s="0"/>
+      <c r="AIJ4" s="0"/>
+      <c r="AIK4" s="0"/>
+      <c r="AIL4" s="0"/>
+      <c r="AIM4" s="0"/>
+      <c r="AIN4" s="0"/>
+      <c r="AIO4" s="0"/>
+      <c r="AIP4" s="0"/>
+      <c r="AIQ4" s="0"/>
+      <c r="AIR4" s="0"/>
+      <c r="AIS4" s="0"/>
+      <c r="AIT4" s="0"/>
+      <c r="AIU4" s="0"/>
+      <c r="AIV4" s="0"/>
+      <c r="AIW4" s="0"/>
+      <c r="AIX4" s="0"/>
+      <c r="AIY4" s="0"/>
+      <c r="AIZ4" s="0"/>
+      <c r="AJA4" s="0"/>
+      <c r="AJB4" s="0"/>
+      <c r="AJC4" s="0"/>
+      <c r="AJD4" s="0"/>
+      <c r="AJE4" s="0"/>
+      <c r="AJF4" s="0"/>
+      <c r="AJG4" s="0"/>
+      <c r="AJH4" s="0"/>
+      <c r="AJI4" s="0"/>
+      <c r="AJJ4" s="0"/>
+      <c r="AJK4" s="0"/>
+      <c r="AJL4" s="0"/>
+      <c r="AJM4" s="0"/>
+      <c r="AJN4" s="0"/>
+      <c r="AJO4" s="0"/>
+      <c r="AJP4" s="0"/>
+      <c r="AJQ4" s="0"/>
+      <c r="AJR4" s="0"/>
+      <c r="AJS4" s="0"/>
+      <c r="AJT4" s="0"/>
+      <c r="AJU4" s="0"/>
+      <c r="AJV4" s="0"/>
+      <c r="AJW4" s="0"/>
+      <c r="AJX4" s="0"/>
+      <c r="AJY4" s="0"/>
+      <c r="AJZ4" s="0"/>
+      <c r="AKA4" s="0"/>
+      <c r="AKB4" s="0"/>
+      <c r="AKC4" s="0"/>
+      <c r="AKD4" s="0"/>
+      <c r="AKE4" s="0"/>
+      <c r="AKF4" s="0"/>
+      <c r="AKG4" s="0"/>
+      <c r="AKH4" s="0"/>
+      <c r="AKI4" s="0"/>
+      <c r="AKJ4" s="0"/>
+      <c r="AKK4" s="0"/>
+      <c r="AKL4" s="0"/>
+      <c r="AKM4" s="0"/>
+      <c r="AKN4" s="0"/>
+      <c r="AKO4" s="0"/>
+      <c r="AKP4" s="0"/>
+      <c r="AKQ4" s="0"/>
+      <c r="AKR4" s="0"/>
+      <c r="AKS4" s="0"/>
+      <c r="AKT4" s="0"/>
+      <c r="AKU4" s="0"/>
+      <c r="AKV4" s="0"/>
+      <c r="AKW4" s="0"/>
+      <c r="AKX4" s="0"/>
+      <c r="AKY4" s="0"/>
+      <c r="AKZ4" s="0"/>
+      <c r="ALA4" s="0"/>
+      <c r="ALB4" s="0"/>
+      <c r="ALC4" s="0"/>
+      <c r="ALD4" s="0"/>
+      <c r="ALE4" s="0"/>
+      <c r="ALF4" s="0"/>
+      <c r="ALG4" s="0"/>
+      <c r="ALH4" s="0"/>
+      <c r="ALI4" s="0"/>
+      <c r="ALJ4" s="0"/>
+      <c r="ALK4" s="0"/>
+      <c r="ALL4" s="0"/>
+      <c r="ALM4" s="0"/>
+      <c r="ALN4" s="0"/>
+      <c r="ALO4" s="0"/>
+      <c r="ALP4" s="0"/>
+      <c r="ALQ4" s="0"/>
+      <c r="ALR4" s="0"/>
+      <c r="ALS4" s="0"/>
+      <c r="ALT4" s="0"/>
+      <c r="ALU4" s="0"/>
+      <c r="ALV4" s="0"/>
+      <c r="ALW4" s="0"/>
+      <c r="ALX4" s="0"/>
+      <c r="ALY4" s="0"/>
+      <c r="ALZ4" s="0"/>
+      <c r="AMA4" s="0"/>
+      <c r="AMB4" s="0"/>
       <c r="AMC4" s="7"/>
       <c r="AMD4" s="7"/>
       <c r="AME4" s="7"/>
       <c r="AMF4" s="7"/>
-      <c r="AMG4" s="0"/>
-      <c r="AMH4" s="0"/>
-      <c r="AMI4" s="0"/>
-      <c r="AMJ4" s="0"/>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14" t="s">
+    <row r="5" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>39</v>
       </c>
       <c r="C5" s="10" t="s">
@@ -1005,21 +2002,23 @@
       <c r="G5" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="10"/>
+      <c r="H5" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="I5" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="L5" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="M5" s="13" t="s">
+      <c r="K5" s="15" t="s">
         <v>44</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
@@ -2029,1054 +3028,52 @@
       <c r="AME5" s="7"/>
       <c r="AMF5" s="7"/>
     </row>
-    <row r="6" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" s="18"/>
+      <c r="L6" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10" t="s">
+      <c r="M6" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="K6" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="L6" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="M6" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="0"/>
-      <c r="R6" s="0"/>
-      <c r="S6" s="0"/>
-      <c r="T6" s="0"/>
-      <c r="U6" s="0"/>
-      <c r="V6" s="0"/>
-      <c r="W6" s="0"/>
-      <c r="X6" s="0"/>
-      <c r="Y6" s="0"/>
-      <c r="Z6" s="0"/>
-      <c r="AA6" s="0"/>
-      <c r="AB6" s="0"/>
-      <c r="AC6" s="0"/>
-      <c r="AD6" s="0"/>
-      <c r="AE6" s="0"/>
-      <c r="AF6" s="0"/>
-      <c r="AG6" s="0"/>
-      <c r="AH6" s="0"/>
-      <c r="AI6" s="0"/>
-      <c r="AJ6" s="0"/>
-      <c r="AK6" s="0"/>
-      <c r="AL6" s="0"/>
-      <c r="AM6" s="0"/>
-      <c r="AN6" s="0"/>
-      <c r="AO6" s="0"/>
-      <c r="AP6" s="0"/>
-      <c r="AQ6" s="0"/>
-      <c r="AR6" s="0"/>
-      <c r="AS6" s="0"/>
-      <c r="AT6" s="0"/>
-      <c r="AU6" s="0"/>
-      <c r="AV6" s="0"/>
-      <c r="AW6" s="0"/>
-      <c r="AX6" s="0"/>
-      <c r="AY6" s="0"/>
-      <c r="AZ6" s="0"/>
-      <c r="BA6" s="0"/>
-      <c r="BB6" s="0"/>
-      <c r="BC6" s="0"/>
-      <c r="BD6" s="0"/>
-      <c r="BE6" s="0"/>
-      <c r="BF6" s="0"/>
-      <c r="BG6" s="0"/>
-      <c r="BH6" s="0"/>
-      <c r="BI6" s="0"/>
-      <c r="BJ6" s="0"/>
-      <c r="BK6" s="0"/>
-      <c r="BL6" s="0"/>
-      <c r="BM6" s="0"/>
-      <c r="BN6" s="0"/>
-      <c r="BO6" s="0"/>
-      <c r="BP6" s="0"/>
-      <c r="BQ6" s="0"/>
-      <c r="BR6" s="0"/>
-      <c r="BS6" s="0"/>
-      <c r="BT6" s="0"/>
-      <c r="BU6" s="0"/>
-      <c r="BV6" s="0"/>
-      <c r="BW6" s="0"/>
-      <c r="BX6" s="0"/>
-      <c r="BY6" s="0"/>
-      <c r="BZ6" s="0"/>
-      <c r="CA6" s="0"/>
-      <c r="CB6" s="0"/>
-      <c r="CC6" s="0"/>
-      <c r="CD6" s="0"/>
-      <c r="CE6" s="0"/>
-      <c r="CF6" s="0"/>
-      <c r="CG6" s="0"/>
-      <c r="CH6" s="0"/>
-      <c r="CI6" s="0"/>
-      <c r="CJ6" s="0"/>
-      <c r="CK6" s="0"/>
-      <c r="CL6" s="0"/>
-      <c r="CM6" s="0"/>
-      <c r="CN6" s="0"/>
-      <c r="CO6" s="0"/>
-      <c r="CP6" s="0"/>
-      <c r="CQ6" s="0"/>
-      <c r="CR6" s="0"/>
-      <c r="CS6" s="0"/>
-      <c r="CT6" s="0"/>
-      <c r="CU6" s="0"/>
-      <c r="CV6" s="0"/>
-      <c r="CW6" s="0"/>
-      <c r="CX6" s="0"/>
-      <c r="CY6" s="0"/>
-      <c r="CZ6" s="0"/>
-      <c r="DA6" s="0"/>
-      <c r="DB6" s="0"/>
-      <c r="DC6" s="0"/>
-      <c r="DD6" s="0"/>
-      <c r="DE6" s="0"/>
-      <c r="DF6" s="0"/>
-      <c r="DG6" s="0"/>
-      <c r="DH6" s="0"/>
-      <c r="DI6" s="0"/>
-      <c r="DJ6" s="0"/>
-      <c r="DK6" s="0"/>
-      <c r="DL6" s="0"/>
-      <c r="DM6" s="0"/>
-      <c r="DN6" s="0"/>
-      <c r="DO6" s="0"/>
-      <c r="DP6" s="0"/>
-      <c r="DQ6" s="0"/>
-      <c r="DR6" s="0"/>
-      <c r="DS6" s="0"/>
-      <c r="DT6" s="0"/>
-      <c r="DU6" s="0"/>
-      <c r="DV6" s="0"/>
-      <c r="DW6" s="0"/>
-      <c r="DX6" s="0"/>
-      <c r="DY6" s="0"/>
-      <c r="DZ6" s="0"/>
-      <c r="EA6" s="0"/>
-      <c r="EB6" s="0"/>
-      <c r="EC6" s="0"/>
-      <c r="ED6" s="0"/>
-      <c r="EE6" s="0"/>
-      <c r="EF6" s="0"/>
-      <c r="EG6" s="0"/>
-      <c r="EH6" s="0"/>
-      <c r="EI6" s="0"/>
-      <c r="EJ6" s="0"/>
-      <c r="EK6" s="0"/>
-      <c r="EL6" s="0"/>
-      <c r="EM6" s="0"/>
-      <c r="EN6" s="0"/>
-      <c r="EO6" s="0"/>
-      <c r="EP6" s="0"/>
-      <c r="EQ6" s="0"/>
-      <c r="ER6" s="0"/>
-      <c r="ES6" s="0"/>
-      <c r="ET6" s="0"/>
-      <c r="EU6" s="0"/>
-      <c r="EV6" s="0"/>
-      <c r="EW6" s="0"/>
-      <c r="EX6" s="0"/>
-      <c r="EY6" s="0"/>
-      <c r="EZ6" s="0"/>
-      <c r="FA6" s="0"/>
-      <c r="FB6" s="0"/>
-      <c r="FC6" s="0"/>
-      <c r="FD6" s="0"/>
-      <c r="FE6" s="0"/>
-      <c r="FF6" s="0"/>
-      <c r="FG6" s="0"/>
-      <c r="FH6" s="0"/>
-      <c r="FI6" s="0"/>
-      <c r="FJ6" s="0"/>
-      <c r="FK6" s="0"/>
-      <c r="FL6" s="0"/>
-      <c r="FM6" s="0"/>
-      <c r="FN6" s="0"/>
-      <c r="FO6" s="0"/>
-      <c r="FP6" s="0"/>
-      <c r="FQ6" s="0"/>
-      <c r="FR6" s="0"/>
-      <c r="FS6" s="0"/>
-      <c r="FT6" s="0"/>
-      <c r="FU6" s="0"/>
-      <c r="FV6" s="0"/>
-      <c r="FW6" s="0"/>
-      <c r="FX6" s="0"/>
-      <c r="FY6" s="0"/>
-      <c r="FZ6" s="0"/>
-      <c r="GA6" s="0"/>
-      <c r="GB6" s="0"/>
-      <c r="GC6" s="0"/>
-      <c r="GD6" s="0"/>
-      <c r="GE6" s="0"/>
-      <c r="GF6" s="0"/>
-      <c r="GG6" s="0"/>
-      <c r="GH6" s="0"/>
-      <c r="GI6" s="0"/>
-      <c r="GJ6" s="0"/>
-      <c r="GK6" s="0"/>
-      <c r="GL6" s="0"/>
-      <c r="GM6" s="0"/>
-      <c r="GN6" s="0"/>
-      <c r="GO6" s="0"/>
-      <c r="GP6" s="0"/>
-      <c r="GQ6" s="0"/>
-      <c r="GR6" s="0"/>
-      <c r="GS6" s="0"/>
-      <c r="GT6" s="0"/>
-      <c r="GU6" s="0"/>
-      <c r="GV6" s="0"/>
-      <c r="GW6" s="0"/>
-      <c r="GX6" s="0"/>
-      <c r="GY6" s="0"/>
-      <c r="GZ6" s="0"/>
-      <c r="HA6" s="0"/>
-      <c r="HB6" s="0"/>
-      <c r="HC6" s="0"/>
-      <c r="HD6" s="0"/>
-      <c r="HE6" s="0"/>
-      <c r="HF6" s="0"/>
-      <c r="HG6" s="0"/>
-      <c r="HH6" s="0"/>
-      <c r="HI6" s="0"/>
-      <c r="HJ6" s="0"/>
-      <c r="HK6" s="0"/>
-      <c r="HL6" s="0"/>
-      <c r="HM6" s="0"/>
-      <c r="HN6" s="0"/>
-      <c r="HO6" s="0"/>
-      <c r="HP6" s="0"/>
-      <c r="HQ6" s="0"/>
-      <c r="HR6" s="0"/>
-      <c r="HS6" s="0"/>
-      <c r="HT6" s="0"/>
-      <c r="HU6" s="0"/>
-      <c r="HV6" s="0"/>
-      <c r="HW6" s="0"/>
-      <c r="HX6" s="0"/>
-      <c r="HY6" s="0"/>
-      <c r="HZ6" s="0"/>
-      <c r="IA6" s="0"/>
-      <c r="IB6" s="0"/>
-      <c r="IC6" s="0"/>
-      <c r="ID6" s="0"/>
-      <c r="IE6" s="0"/>
-      <c r="IF6" s="0"/>
-      <c r="IG6" s="0"/>
-      <c r="IH6" s="0"/>
-      <c r="II6" s="0"/>
-      <c r="IJ6" s="0"/>
-      <c r="IK6" s="0"/>
-      <c r="IL6" s="0"/>
-      <c r="IM6" s="0"/>
-      <c r="IN6" s="0"/>
-      <c r="IO6" s="0"/>
-      <c r="IP6" s="0"/>
-      <c r="IQ6" s="0"/>
-      <c r="IR6" s="0"/>
-      <c r="IS6" s="0"/>
-      <c r="IT6" s="0"/>
-      <c r="IU6" s="0"/>
-      <c r="IV6" s="0"/>
-      <c r="IW6" s="0"/>
-      <c r="IX6" s="0"/>
-      <c r="IY6" s="0"/>
-      <c r="IZ6" s="0"/>
-      <c r="JA6" s="0"/>
-      <c r="JB6" s="0"/>
-      <c r="JC6" s="0"/>
-      <c r="JD6" s="0"/>
-      <c r="JE6" s="0"/>
-      <c r="JF6" s="0"/>
-      <c r="JG6" s="0"/>
-      <c r="JH6" s="0"/>
-      <c r="JI6" s="0"/>
-      <c r="JJ6" s="0"/>
-      <c r="JK6" s="0"/>
-      <c r="JL6" s="0"/>
-      <c r="JM6" s="0"/>
-      <c r="JN6" s="0"/>
-      <c r="JO6" s="0"/>
-      <c r="JP6" s="0"/>
-      <c r="JQ6" s="0"/>
-      <c r="JR6" s="0"/>
-      <c r="JS6" s="0"/>
-      <c r="JT6" s="0"/>
-      <c r="JU6" s="0"/>
-      <c r="JV6" s="0"/>
-      <c r="JW6" s="0"/>
-      <c r="JX6" s="0"/>
-      <c r="JY6" s="0"/>
-      <c r="JZ6" s="0"/>
-      <c r="KA6" s="0"/>
-      <c r="KB6" s="0"/>
-      <c r="KC6" s="0"/>
-      <c r="KD6" s="0"/>
-      <c r="KE6" s="0"/>
-      <c r="KF6" s="0"/>
-      <c r="KG6" s="0"/>
-      <c r="KH6" s="0"/>
-      <c r="KI6" s="0"/>
-      <c r="KJ6" s="0"/>
-      <c r="KK6" s="0"/>
-      <c r="KL6" s="0"/>
-      <c r="KM6" s="0"/>
-      <c r="KN6" s="0"/>
-      <c r="KO6" s="0"/>
-      <c r="KP6" s="0"/>
-      <c r="KQ6" s="0"/>
-      <c r="KR6" s="0"/>
-      <c r="KS6" s="0"/>
-      <c r="KT6" s="0"/>
-      <c r="KU6" s="0"/>
-      <c r="KV6" s="0"/>
-      <c r="KW6" s="0"/>
-      <c r="KX6" s="0"/>
-      <c r="KY6" s="0"/>
-      <c r="KZ6" s="0"/>
-      <c r="LA6" s="0"/>
-      <c r="LB6" s="0"/>
-      <c r="LC6" s="0"/>
-      <c r="LD6" s="0"/>
-      <c r="LE6" s="0"/>
-      <c r="LF6" s="0"/>
-      <c r="LG6" s="0"/>
-      <c r="LH6" s="0"/>
-      <c r="LI6" s="0"/>
-      <c r="LJ6" s="0"/>
-      <c r="LK6" s="0"/>
-      <c r="LL6" s="0"/>
-      <c r="LM6" s="0"/>
-      <c r="LN6" s="0"/>
-      <c r="LO6" s="0"/>
-      <c r="LP6" s="0"/>
-      <c r="LQ6" s="0"/>
-      <c r="LR6" s="0"/>
-      <c r="LS6" s="0"/>
-      <c r="LT6" s="0"/>
-      <c r="LU6" s="0"/>
-      <c r="LV6" s="0"/>
-      <c r="LW6" s="0"/>
-      <c r="LX6" s="0"/>
-      <c r="LY6" s="0"/>
-      <c r="LZ6" s="0"/>
-      <c r="MA6" s="0"/>
-      <c r="MB6" s="0"/>
-      <c r="MC6" s="0"/>
-      <c r="MD6" s="0"/>
-      <c r="ME6" s="0"/>
-      <c r="MF6" s="0"/>
-      <c r="MG6" s="0"/>
-      <c r="MH6" s="0"/>
-      <c r="MI6" s="0"/>
-      <c r="MJ6" s="0"/>
-      <c r="MK6" s="0"/>
-      <c r="ML6" s="0"/>
-      <c r="MM6" s="0"/>
-      <c r="MN6" s="0"/>
-      <c r="MO6" s="0"/>
-      <c r="MP6" s="0"/>
-      <c r="MQ6" s="0"/>
-      <c r="MR6" s="0"/>
-      <c r="MS6" s="0"/>
-      <c r="MT6" s="0"/>
-      <c r="MU6" s="0"/>
-      <c r="MV6" s="0"/>
-      <c r="MW6" s="0"/>
-      <c r="MX6" s="0"/>
-      <c r="MY6" s="0"/>
-      <c r="MZ6" s="0"/>
-      <c r="NA6" s="0"/>
-      <c r="NB6" s="0"/>
-      <c r="NC6" s="0"/>
-      <c r="ND6" s="0"/>
-      <c r="NE6" s="0"/>
-      <c r="NF6" s="0"/>
-      <c r="NG6" s="0"/>
-      <c r="NH6" s="0"/>
-      <c r="NI6" s="0"/>
-      <c r="NJ6" s="0"/>
-      <c r="NK6" s="0"/>
-      <c r="NL6" s="0"/>
-      <c r="NM6" s="0"/>
-      <c r="NN6" s="0"/>
-      <c r="NO6" s="0"/>
-      <c r="NP6" s="0"/>
-      <c r="NQ6" s="0"/>
-      <c r="NR6" s="0"/>
-      <c r="NS6" s="0"/>
-      <c r="NT6" s="0"/>
-      <c r="NU6" s="0"/>
-      <c r="NV6" s="0"/>
-      <c r="NW6" s="0"/>
-      <c r="NX6" s="0"/>
-      <c r="NY6" s="0"/>
-      <c r="NZ6" s="0"/>
-      <c r="OA6" s="0"/>
-      <c r="OB6" s="0"/>
-      <c r="OC6" s="0"/>
-      <c r="OD6" s="0"/>
-      <c r="OE6" s="0"/>
-      <c r="OF6" s="0"/>
-      <c r="OG6" s="0"/>
-      <c r="OH6" s="0"/>
-      <c r="OI6" s="0"/>
-      <c r="OJ6" s="0"/>
-      <c r="OK6" s="0"/>
-      <c r="OL6" s="0"/>
-      <c r="OM6" s="0"/>
-      <c r="ON6" s="0"/>
-      <c r="OO6" s="0"/>
-      <c r="OP6" s="0"/>
-      <c r="OQ6" s="0"/>
-      <c r="OR6" s="0"/>
-      <c r="OS6" s="0"/>
-      <c r="OT6" s="0"/>
-      <c r="OU6" s="0"/>
-      <c r="OV6" s="0"/>
-      <c r="OW6" s="0"/>
-      <c r="OX6" s="0"/>
-      <c r="OY6" s="0"/>
-      <c r="OZ6" s="0"/>
-      <c r="PA6" s="0"/>
-      <c r="PB6" s="0"/>
-      <c r="PC6" s="0"/>
-      <c r="PD6" s="0"/>
-      <c r="PE6" s="0"/>
-      <c r="PF6" s="0"/>
-      <c r="PG6" s="0"/>
-      <c r="PH6" s="0"/>
-      <c r="PI6" s="0"/>
-      <c r="PJ6" s="0"/>
-      <c r="PK6" s="0"/>
-      <c r="PL6" s="0"/>
-      <c r="PM6" s="0"/>
-      <c r="PN6" s="0"/>
-      <c r="PO6" s="0"/>
-      <c r="PP6" s="0"/>
-      <c r="PQ6" s="0"/>
-      <c r="PR6" s="0"/>
-      <c r="PS6" s="0"/>
-      <c r="PT6" s="0"/>
-      <c r="PU6" s="0"/>
-      <c r="PV6" s="0"/>
-      <c r="PW6" s="0"/>
-      <c r="PX6" s="0"/>
-      <c r="PY6" s="0"/>
-      <c r="PZ6" s="0"/>
-      <c r="QA6" s="0"/>
-      <c r="QB6" s="0"/>
-      <c r="QC6" s="0"/>
-      <c r="QD6" s="0"/>
-      <c r="QE6" s="0"/>
-      <c r="QF6" s="0"/>
-      <c r="QG6" s="0"/>
-      <c r="QH6" s="0"/>
-      <c r="QI6" s="0"/>
-      <c r="QJ6" s="0"/>
-      <c r="QK6" s="0"/>
-      <c r="QL6" s="0"/>
-      <c r="QM6" s="0"/>
-      <c r="QN6" s="0"/>
-      <c r="QO6" s="0"/>
-      <c r="QP6" s="0"/>
-      <c r="QQ6" s="0"/>
-      <c r="QR6" s="0"/>
-      <c r="QS6" s="0"/>
-      <c r="QT6" s="0"/>
-      <c r="QU6" s="0"/>
-      <c r="QV6" s="0"/>
-      <c r="QW6" s="0"/>
-      <c r="QX6" s="0"/>
-      <c r="QY6" s="0"/>
-      <c r="QZ6" s="0"/>
-      <c r="RA6" s="0"/>
-      <c r="RB6" s="0"/>
-      <c r="RC6" s="0"/>
-      <c r="RD6" s="0"/>
-      <c r="RE6" s="0"/>
-      <c r="RF6" s="0"/>
-      <c r="RG6" s="0"/>
-      <c r="RH6" s="0"/>
-      <c r="RI6" s="0"/>
-      <c r="RJ6" s="0"/>
-      <c r="RK6" s="0"/>
-      <c r="RL6" s="0"/>
-      <c r="RM6" s="0"/>
-      <c r="RN6" s="0"/>
-      <c r="RO6" s="0"/>
-      <c r="RP6" s="0"/>
-      <c r="RQ6" s="0"/>
-      <c r="RR6" s="0"/>
-      <c r="RS6" s="0"/>
-      <c r="RT6" s="0"/>
-      <c r="RU6" s="0"/>
-      <c r="RV6" s="0"/>
-      <c r="RW6" s="0"/>
-      <c r="RX6" s="0"/>
-      <c r="RY6" s="0"/>
-      <c r="RZ6" s="0"/>
-      <c r="SA6" s="0"/>
-      <c r="SB6" s="0"/>
-      <c r="SC6" s="0"/>
-      <c r="SD6" s="0"/>
-      <c r="SE6" s="0"/>
-      <c r="SF6" s="0"/>
-      <c r="SG6" s="0"/>
-      <c r="SH6" s="0"/>
-      <c r="SI6" s="0"/>
-      <c r="SJ6" s="0"/>
-      <c r="SK6" s="0"/>
-      <c r="SL6" s="0"/>
-      <c r="SM6" s="0"/>
-      <c r="SN6" s="0"/>
-      <c r="SO6" s="0"/>
-      <c r="SP6" s="0"/>
-      <c r="SQ6" s="0"/>
-      <c r="SR6" s="0"/>
-      <c r="SS6" s="0"/>
-      <c r="ST6" s="0"/>
-      <c r="SU6" s="0"/>
-      <c r="SV6" s="0"/>
-      <c r="SW6" s="0"/>
-      <c r="SX6" s="0"/>
-      <c r="SY6" s="0"/>
-      <c r="SZ6" s="0"/>
-      <c r="TA6" s="0"/>
-      <c r="TB6" s="0"/>
-      <c r="TC6" s="0"/>
-      <c r="TD6" s="0"/>
-      <c r="TE6" s="0"/>
-      <c r="TF6" s="0"/>
-      <c r="TG6" s="0"/>
-      <c r="TH6" s="0"/>
-      <c r="TI6" s="0"/>
-      <c r="TJ6" s="0"/>
-      <c r="TK6" s="0"/>
-      <c r="TL6" s="0"/>
-      <c r="TM6" s="0"/>
-      <c r="TN6" s="0"/>
-      <c r="TO6" s="0"/>
-      <c r="TP6" s="0"/>
-      <c r="TQ6" s="0"/>
-      <c r="TR6" s="0"/>
-      <c r="TS6" s="0"/>
-      <c r="TT6" s="0"/>
-      <c r="TU6" s="0"/>
-      <c r="TV6" s="0"/>
-      <c r="TW6" s="0"/>
-      <c r="TX6" s="0"/>
-      <c r="TY6" s="0"/>
-      <c r="TZ6" s="0"/>
-      <c r="UA6" s="0"/>
-      <c r="UB6" s="0"/>
-      <c r="UC6" s="0"/>
-      <c r="UD6" s="0"/>
-      <c r="UE6" s="0"/>
-      <c r="UF6" s="0"/>
-      <c r="UG6" s="0"/>
-      <c r="UH6" s="0"/>
-      <c r="UI6" s="0"/>
-      <c r="UJ6" s="0"/>
-      <c r="UK6" s="0"/>
-      <c r="UL6" s="0"/>
-      <c r="UM6" s="0"/>
-      <c r="UN6" s="0"/>
-      <c r="UO6" s="0"/>
-      <c r="UP6" s="0"/>
-      <c r="UQ6" s="0"/>
-      <c r="UR6" s="0"/>
-      <c r="US6" s="0"/>
-      <c r="UT6" s="0"/>
-      <c r="UU6" s="0"/>
-      <c r="UV6" s="0"/>
-      <c r="UW6" s="0"/>
-      <c r="UX6" s="0"/>
-      <c r="UY6" s="0"/>
-      <c r="UZ6" s="0"/>
-      <c r="VA6" s="0"/>
-      <c r="VB6" s="0"/>
-      <c r="VC6" s="0"/>
-      <c r="VD6" s="0"/>
-      <c r="VE6" s="0"/>
-      <c r="VF6" s="0"/>
-      <c r="VG6" s="0"/>
-      <c r="VH6" s="0"/>
-      <c r="VI6" s="0"/>
-      <c r="VJ6" s="0"/>
-      <c r="VK6" s="0"/>
-      <c r="VL6" s="0"/>
-      <c r="VM6" s="0"/>
-      <c r="VN6" s="0"/>
-      <c r="VO6" s="0"/>
-      <c r="VP6" s="0"/>
-      <c r="VQ6" s="0"/>
-      <c r="VR6" s="0"/>
-      <c r="VS6" s="0"/>
-      <c r="VT6" s="0"/>
-      <c r="VU6" s="0"/>
-      <c r="VV6" s="0"/>
-      <c r="VW6" s="0"/>
-      <c r="VX6" s="0"/>
-      <c r="VY6" s="0"/>
-      <c r="VZ6" s="0"/>
-      <c r="WA6" s="0"/>
-      <c r="WB6" s="0"/>
-      <c r="WC6" s="0"/>
-      <c r="WD6" s="0"/>
-      <c r="WE6" s="0"/>
-      <c r="WF6" s="0"/>
-      <c r="WG6" s="0"/>
-      <c r="WH6" s="0"/>
-      <c r="WI6" s="0"/>
-      <c r="WJ6" s="0"/>
-      <c r="WK6" s="0"/>
-      <c r="WL6" s="0"/>
-      <c r="WM6" s="0"/>
-      <c r="WN6" s="0"/>
-      <c r="WO6" s="0"/>
-      <c r="WP6" s="0"/>
-      <c r="WQ6" s="0"/>
-      <c r="WR6" s="0"/>
-      <c r="WS6" s="0"/>
-      <c r="WT6" s="0"/>
-      <c r="WU6" s="0"/>
-      <c r="WV6" s="0"/>
-      <c r="WW6" s="0"/>
-      <c r="WX6" s="0"/>
-      <c r="WY6" s="0"/>
-      <c r="WZ6" s="0"/>
-      <c r="XA6" s="0"/>
-      <c r="XB6" s="0"/>
-      <c r="XC6" s="0"/>
-      <c r="XD6" s="0"/>
-      <c r="XE6" s="0"/>
-      <c r="XF6" s="0"/>
-      <c r="XG6" s="0"/>
-      <c r="XH6" s="0"/>
-      <c r="XI6" s="0"/>
-      <c r="XJ6" s="0"/>
-      <c r="XK6" s="0"/>
-      <c r="XL6" s="0"/>
-      <c r="XM6" s="0"/>
-      <c r="XN6" s="0"/>
-      <c r="XO6" s="0"/>
-      <c r="XP6" s="0"/>
-      <c r="XQ6" s="0"/>
-      <c r="XR6" s="0"/>
-      <c r="XS6" s="0"/>
-      <c r="XT6" s="0"/>
-      <c r="XU6" s="0"/>
-      <c r="XV6" s="0"/>
-      <c r="XW6" s="0"/>
-      <c r="XX6" s="0"/>
-      <c r="XY6" s="0"/>
-      <c r="XZ6" s="0"/>
-      <c r="YA6" s="0"/>
-      <c r="YB6" s="0"/>
-      <c r="YC6" s="0"/>
-      <c r="YD6" s="0"/>
-      <c r="YE6" s="0"/>
-      <c r="YF6" s="0"/>
-      <c r="YG6" s="0"/>
-      <c r="YH6" s="0"/>
-      <c r="YI6" s="0"/>
-      <c r="YJ6" s="0"/>
-      <c r="YK6" s="0"/>
-      <c r="YL6" s="0"/>
-      <c r="YM6" s="0"/>
-      <c r="YN6" s="0"/>
-      <c r="YO6" s="0"/>
-      <c r="YP6" s="0"/>
-      <c r="YQ6" s="0"/>
-      <c r="YR6" s="0"/>
-      <c r="YS6" s="0"/>
-      <c r="YT6" s="0"/>
-      <c r="YU6" s="0"/>
-      <c r="YV6" s="0"/>
-      <c r="YW6" s="0"/>
-      <c r="YX6" s="0"/>
-      <c r="YY6" s="0"/>
-      <c r="YZ6" s="0"/>
-      <c r="ZA6" s="0"/>
-      <c r="ZB6" s="0"/>
-      <c r="ZC6" s="0"/>
-      <c r="ZD6" s="0"/>
-      <c r="ZE6" s="0"/>
-      <c r="ZF6" s="0"/>
-      <c r="ZG6" s="0"/>
-      <c r="ZH6" s="0"/>
-      <c r="ZI6" s="0"/>
-      <c r="ZJ6" s="0"/>
-      <c r="ZK6" s="0"/>
-      <c r="ZL6" s="0"/>
-      <c r="ZM6" s="0"/>
-      <c r="ZN6" s="0"/>
-      <c r="ZO6" s="0"/>
-      <c r="ZP6" s="0"/>
-      <c r="ZQ6" s="0"/>
-      <c r="ZR6" s="0"/>
-      <c r="ZS6" s="0"/>
-      <c r="ZT6" s="0"/>
-      <c r="ZU6" s="0"/>
-      <c r="ZV6" s="0"/>
-      <c r="ZW6" s="0"/>
-      <c r="ZX6" s="0"/>
-      <c r="ZY6" s="0"/>
-      <c r="ZZ6" s="0"/>
-      <c r="AAA6" s="0"/>
-      <c r="AAB6" s="0"/>
-      <c r="AAC6" s="0"/>
-      <c r="AAD6" s="0"/>
-      <c r="AAE6" s="0"/>
-      <c r="AAF6" s="0"/>
-      <c r="AAG6" s="0"/>
-      <c r="AAH6" s="0"/>
-      <c r="AAI6" s="0"/>
-      <c r="AAJ6" s="0"/>
-      <c r="AAK6" s="0"/>
-      <c r="AAL6" s="0"/>
-      <c r="AAM6" s="0"/>
-      <c r="AAN6" s="0"/>
-      <c r="AAO6" s="0"/>
-      <c r="AAP6" s="0"/>
-      <c r="AAQ6" s="0"/>
-      <c r="AAR6" s="0"/>
-      <c r="AAS6" s="0"/>
-      <c r="AAT6" s="0"/>
-      <c r="AAU6" s="0"/>
-      <c r="AAV6" s="0"/>
-      <c r="AAW6" s="0"/>
-      <c r="AAX6" s="0"/>
-      <c r="AAY6" s="0"/>
-      <c r="AAZ6" s="0"/>
-      <c r="ABA6" s="0"/>
-      <c r="ABB6" s="0"/>
-      <c r="ABC6" s="0"/>
-      <c r="ABD6" s="0"/>
-      <c r="ABE6" s="0"/>
-      <c r="ABF6" s="0"/>
-      <c r="ABG6" s="0"/>
-      <c r="ABH6" s="0"/>
-      <c r="ABI6" s="0"/>
-      <c r="ABJ6" s="0"/>
-      <c r="ABK6" s="0"/>
-      <c r="ABL6" s="0"/>
-      <c r="ABM6" s="0"/>
-      <c r="ABN6" s="0"/>
-      <c r="ABO6" s="0"/>
-      <c r="ABP6" s="0"/>
-      <c r="ABQ6" s="0"/>
-      <c r="ABR6" s="0"/>
-      <c r="ABS6" s="0"/>
-      <c r="ABT6" s="0"/>
-      <c r="ABU6" s="0"/>
-      <c r="ABV6" s="0"/>
-      <c r="ABW6" s="0"/>
-      <c r="ABX6" s="0"/>
-      <c r="ABY6" s="0"/>
-      <c r="ABZ6" s="0"/>
-      <c r="ACA6" s="0"/>
-      <c r="ACB6" s="0"/>
-      <c r="ACC6" s="0"/>
-      <c r="ACD6" s="0"/>
-      <c r="ACE6" s="0"/>
-      <c r="ACF6" s="0"/>
-      <c r="ACG6" s="0"/>
-      <c r="ACH6" s="0"/>
-      <c r="ACI6" s="0"/>
-      <c r="ACJ6" s="0"/>
-      <c r="ACK6" s="0"/>
-      <c r="ACL6" s="0"/>
-      <c r="ACM6" s="0"/>
-      <c r="ACN6" s="0"/>
-      <c r="ACO6" s="0"/>
-      <c r="ACP6" s="0"/>
-      <c r="ACQ6" s="0"/>
-      <c r="ACR6" s="0"/>
-      <c r="ACS6" s="0"/>
-      <c r="ACT6" s="0"/>
-      <c r="ACU6" s="0"/>
-      <c r="ACV6" s="0"/>
-      <c r="ACW6" s="0"/>
-      <c r="ACX6" s="0"/>
-      <c r="ACY6" s="0"/>
-      <c r="ACZ6" s="0"/>
-      <c r="ADA6" s="0"/>
-      <c r="ADB6" s="0"/>
-      <c r="ADC6" s="0"/>
-      <c r="ADD6" s="0"/>
-      <c r="ADE6" s="0"/>
-      <c r="ADF6" s="0"/>
-      <c r="ADG6" s="0"/>
-      <c r="ADH6" s="0"/>
-      <c r="ADI6" s="0"/>
-      <c r="ADJ6" s="0"/>
-      <c r="ADK6" s="0"/>
-      <c r="ADL6" s="0"/>
-      <c r="ADM6" s="0"/>
-      <c r="ADN6" s="0"/>
-      <c r="ADO6" s="0"/>
-      <c r="ADP6" s="0"/>
-      <c r="ADQ6" s="0"/>
-      <c r="ADR6" s="0"/>
-      <c r="ADS6" s="0"/>
-      <c r="ADT6" s="0"/>
-      <c r="ADU6" s="0"/>
-      <c r="ADV6" s="0"/>
-      <c r="ADW6" s="0"/>
-      <c r="ADX6" s="0"/>
-      <c r="ADY6" s="0"/>
-      <c r="ADZ6" s="0"/>
-      <c r="AEA6" s="0"/>
-      <c r="AEB6" s="0"/>
-      <c r="AEC6" s="0"/>
-      <c r="AED6" s="0"/>
-      <c r="AEE6" s="0"/>
-      <c r="AEF6" s="0"/>
-      <c r="AEG6" s="0"/>
-      <c r="AEH6" s="0"/>
-      <c r="AEI6" s="0"/>
-      <c r="AEJ6" s="0"/>
-      <c r="AEK6" s="0"/>
-      <c r="AEL6" s="0"/>
-      <c r="AEM6" s="0"/>
-      <c r="AEN6" s="0"/>
-      <c r="AEO6" s="0"/>
-      <c r="AEP6" s="0"/>
-      <c r="AEQ6" s="0"/>
-      <c r="AER6" s="0"/>
-      <c r="AES6" s="0"/>
-      <c r="AET6" s="0"/>
-      <c r="AEU6" s="0"/>
-      <c r="AEV6" s="0"/>
-      <c r="AEW6" s="0"/>
-      <c r="AEX6" s="0"/>
-      <c r="AEY6" s="0"/>
-      <c r="AEZ6" s="0"/>
-      <c r="AFA6" s="0"/>
-      <c r="AFB6" s="0"/>
-      <c r="AFC6" s="0"/>
-      <c r="AFD6" s="0"/>
-      <c r="AFE6" s="0"/>
-      <c r="AFF6" s="0"/>
-      <c r="AFG6" s="0"/>
-      <c r="AFH6" s="0"/>
-      <c r="AFI6" s="0"/>
-      <c r="AFJ6" s="0"/>
-      <c r="AFK6" s="0"/>
-      <c r="AFL6" s="0"/>
-      <c r="AFM6" s="0"/>
-      <c r="AFN6" s="0"/>
-      <c r="AFO6" s="0"/>
-      <c r="AFP6" s="0"/>
-      <c r="AFQ6" s="0"/>
-      <c r="AFR6" s="0"/>
-      <c r="AFS6" s="0"/>
-      <c r="AFT6" s="0"/>
-      <c r="AFU6" s="0"/>
-      <c r="AFV6" s="0"/>
-      <c r="AFW6" s="0"/>
-      <c r="AFX6" s="0"/>
-      <c r="AFY6" s="0"/>
-      <c r="AFZ6" s="0"/>
-      <c r="AGA6" s="0"/>
-      <c r="AGB6" s="0"/>
-      <c r="AGC6" s="0"/>
-      <c r="AGD6" s="0"/>
-      <c r="AGE6" s="0"/>
-      <c r="AGF6" s="0"/>
-      <c r="AGG6" s="0"/>
-      <c r="AGH6" s="0"/>
-      <c r="AGI6" s="0"/>
-      <c r="AGJ6" s="0"/>
-      <c r="AGK6" s="0"/>
-      <c r="AGL6" s="0"/>
-      <c r="AGM6" s="0"/>
-      <c r="AGN6" s="0"/>
-      <c r="AGO6" s="0"/>
-      <c r="AGP6" s="0"/>
-      <c r="AGQ6" s="0"/>
-      <c r="AGR6" s="0"/>
-      <c r="AGS6" s="0"/>
-      <c r="AGT6" s="0"/>
-      <c r="AGU6" s="0"/>
-      <c r="AGV6" s="0"/>
-      <c r="AGW6" s="0"/>
-      <c r="AGX6" s="0"/>
-      <c r="AGY6" s="0"/>
-      <c r="AGZ6" s="0"/>
-      <c r="AHA6" s="0"/>
-      <c r="AHB6" s="0"/>
-      <c r="AHC6" s="0"/>
-      <c r="AHD6" s="0"/>
-      <c r="AHE6" s="0"/>
-      <c r="AHF6" s="0"/>
-      <c r="AHG6" s="0"/>
-      <c r="AHH6" s="0"/>
-      <c r="AHI6" s="0"/>
-      <c r="AHJ6" s="0"/>
-      <c r="AHK6" s="0"/>
-      <c r="AHL6" s="0"/>
-      <c r="AHM6" s="0"/>
-      <c r="AHN6" s="0"/>
-      <c r="AHO6" s="0"/>
-      <c r="AHP6" s="0"/>
-      <c r="AHQ6" s="0"/>
-      <c r="AHR6" s="0"/>
-      <c r="AHS6" s="0"/>
-      <c r="AHT6" s="0"/>
-      <c r="AHU6" s="0"/>
-      <c r="AHV6" s="0"/>
-      <c r="AHW6" s="0"/>
-      <c r="AHX6" s="0"/>
-      <c r="AHY6" s="0"/>
-      <c r="AHZ6" s="0"/>
-      <c r="AIA6" s="0"/>
-      <c r="AIB6" s="0"/>
-      <c r="AIC6" s="0"/>
-      <c r="AID6" s="0"/>
-      <c r="AIE6" s="0"/>
-      <c r="AIF6" s="0"/>
-      <c r="AIG6" s="0"/>
-      <c r="AIH6" s="0"/>
-      <c r="AII6" s="0"/>
-      <c r="AIJ6" s="0"/>
-      <c r="AIK6" s="0"/>
-      <c r="AIL6" s="0"/>
-      <c r="AIM6" s="0"/>
-      <c r="AIN6" s="0"/>
-      <c r="AIO6" s="0"/>
-      <c r="AIP6" s="0"/>
-      <c r="AIQ6" s="0"/>
-      <c r="AIR6" s="0"/>
-      <c r="AIS6" s="0"/>
-      <c r="AIT6" s="0"/>
-      <c r="AIU6" s="0"/>
-      <c r="AIV6" s="0"/>
-      <c r="AIW6" s="0"/>
-      <c r="AIX6" s="0"/>
-      <c r="AIY6" s="0"/>
-      <c r="AIZ6" s="0"/>
-      <c r="AJA6" s="0"/>
-      <c r="AJB6" s="0"/>
-      <c r="AJC6" s="0"/>
-      <c r="AJD6" s="0"/>
-      <c r="AJE6" s="0"/>
-      <c r="AJF6" s="0"/>
-      <c r="AJG6" s="0"/>
-      <c r="AJH6" s="0"/>
-      <c r="AJI6" s="0"/>
-      <c r="AJJ6" s="0"/>
-      <c r="AJK6" s="0"/>
-      <c r="AJL6" s="0"/>
-      <c r="AJM6" s="0"/>
-      <c r="AJN6" s="0"/>
-      <c r="AJO6" s="0"/>
-      <c r="AJP6" s="0"/>
-      <c r="AJQ6" s="0"/>
-      <c r="AJR6" s="0"/>
-      <c r="AJS6" s="0"/>
-      <c r="AJT6" s="0"/>
-      <c r="AJU6" s="0"/>
-      <c r="AJV6" s="0"/>
-      <c r="AJW6" s="0"/>
-      <c r="AJX6" s="0"/>
-      <c r="AJY6" s="0"/>
-      <c r="AJZ6" s="0"/>
-      <c r="AKA6" s="0"/>
-      <c r="AKB6" s="0"/>
-      <c r="AKC6" s="0"/>
-      <c r="AKD6" s="0"/>
-      <c r="AKE6" s="0"/>
-      <c r="AKF6" s="0"/>
-      <c r="AKG6" s="0"/>
-      <c r="AKH6" s="0"/>
-      <c r="AKI6" s="0"/>
-      <c r="AKJ6" s="0"/>
-      <c r="AKK6" s="0"/>
-      <c r="AKL6" s="0"/>
-      <c r="AKM6" s="0"/>
-      <c r="AKN6" s="0"/>
-      <c r="AKO6" s="0"/>
-      <c r="AKP6" s="0"/>
-      <c r="AKQ6" s="0"/>
-      <c r="AKR6" s="0"/>
-      <c r="AKS6" s="0"/>
-      <c r="AKT6" s="0"/>
-      <c r="AKU6" s="0"/>
-      <c r="AKV6" s="0"/>
-      <c r="AKW6" s="0"/>
-      <c r="AKX6" s="0"/>
-      <c r="AKY6" s="0"/>
-      <c r="AKZ6" s="0"/>
-      <c r="ALA6" s="0"/>
-      <c r="ALB6" s="0"/>
-      <c r="ALC6" s="0"/>
-      <c r="ALD6" s="0"/>
-      <c r="ALE6" s="0"/>
-      <c r="ALF6" s="0"/>
-      <c r="ALG6" s="0"/>
-      <c r="ALH6" s="0"/>
-      <c r="ALI6" s="0"/>
-      <c r="ALJ6" s="0"/>
-      <c r="ALK6" s="0"/>
-      <c r="ALL6" s="0"/>
-      <c r="ALM6" s="0"/>
-      <c r="ALN6" s="0"/>
-      <c r="ALO6" s="0"/>
-      <c r="ALP6" s="0"/>
-      <c r="ALQ6" s="0"/>
-      <c r="ALR6" s="0"/>
-      <c r="ALS6" s="0"/>
-      <c r="ALT6" s="0"/>
-      <c r="ALU6" s="0"/>
-      <c r="ALV6" s="0"/>
-      <c r="ALW6" s="0"/>
-      <c r="ALX6" s="0"/>
-      <c r="ALY6" s="0"/>
-      <c r="ALZ6" s="0"/>
-      <c r="AMA6" s="0"/>
-      <c r="AMB6" s="0"/>
-      <c r="AMC6" s="7"/>
-      <c r="AMD6" s="7"/>
-      <c r="AME6" s="7"/>
-      <c r="AMF6" s="7"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="AMC6" s="20"/>
+      <c r="AMD6" s="20"/>
+      <c r="AME6" s="20"/>
+      <c r="AMF6" s="20"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>54</v>
+        <v>48</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>49</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>23</v>
@@ -3091,19 +3088,19 @@
         <v>33</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="J7" s="10" t="s">
         <v>27</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="N7" s="10"/>
       <c r="O7" s="10"/>
@@ -4117,10 +4114,10 @@
     </row>
     <row r="8" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>60</v>
+        <v>54</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>55</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>23</v>
@@ -4135,25 +4132,25 @@
         <v>33</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="J8" s="10" t="s">
         <v>27</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="L8" s="10" t="s">
         <v>29</v>
       </c>
       <c r="M8" s="10" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="N8" s="10" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="O8" s="10" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="P8" s="10" t="n">
         <v>15</v>
@@ -4163,12 +4160,12 @@
       <c r="AMI8" s="0"/>
       <c r="AMJ8" s="0"/>
     </row>
-    <row r="9" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>67</v>
+        <v>61</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>62</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>23</v>
@@ -4183,40 +4180,36 @@
         <v>33</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="J9" s="10" t="s">
         <v>27</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="L9" s="10" t="s">
         <v>29</v>
       </c>
       <c r="M9" s="10" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="N9" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="O9" s="13" t="s">
-        <v>71</v>
+      <c r="O9" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="P9" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="AMG9" s="0"/>
-      <c r="AMH9" s="0"/>
-      <c r="AMI9" s="0"/>
-      <c r="AMJ9" s="0"/>
     </row>
-    <row r="10" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>73</v>
+        <v>67</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>68</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>23</v>
@@ -4231,40 +4224,36 @@
         <v>33</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>75</v>
+        <v>52</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>70</v>
       </c>
       <c r="L10" s="10" t="s">
         <v>27</v>
       </c>
       <c r="M10" s="10" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="N10" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="O10" s="13" t="s">
-        <v>77</v>
+      <c r="O10" s="12" t="s">
+        <v>72</v>
       </c>
       <c r="P10" s="10" t="n">
         <v>25</v>
       </c>
-      <c r="AMG10" s="0"/>
-      <c r="AMH10" s="0"/>
-      <c r="AMI10" s="0"/>
-      <c r="AMJ10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>79</v>
+        <v>73</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>74</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>23</v>
@@ -4273,36 +4262,74 @@
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="K11" s="13" t="s">
-        <v>82</v>
+        <v>77</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>78</v>
       </c>
       <c r="L11" s="10" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="M11" s="10" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="N11" s="10"/>
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
     </row>
-    <row r="13" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="M12" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>74</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>23</v>
@@ -4311,72 +4338,34 @@
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>48</v>
+        <v>85</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="K13" s="17" t="s">
-        <v>50</v>
+        <v>77</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>78</v>
       </c>
       <c r="L13" s="10" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="M13" s="10" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10" t="s">
+      <c r="P13" s="10" t="s">
         <v>87</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="J14" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="K14" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="L14" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="M14" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:W43"/>
+  <autoFilter ref="A2:W42"/>
   <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:F1"/>
@@ -4413,15 +4402,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>2</v>
@@ -4429,7 +4418,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>1.5</v>
@@ -4437,7 +4426,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>2</v>
@@ -4445,7 +4434,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>2</v>
@@ -4453,7 +4442,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>3</v>
@@ -4461,7 +4450,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>4</v>
@@ -4469,7 +4458,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>5</v>
@@ -4477,7 +4466,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>2</v>
@@ -4485,7 +4474,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>4</v>
@@ -4493,7 +4482,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>6</v>
@@ -4501,7 +4490,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>1</v>
@@ -4509,7 +4498,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>1</v>
@@ -4517,7 +4506,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>0.5</v>
@@ -4525,7 +4514,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>0.25</v>
@@ -4533,7 +4522,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>0.5</v>
@@ -4541,7 +4530,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>1</v>
@@ -4549,7 +4538,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B18" s="1" t="n">
         <v>0.3</v>
@@ -4557,7 +4546,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B19" s="1" t="n">
         <v>0.1</v>
@@ -4582,30 +4571,30 @@
   <dimension ref="1:15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="18" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="18" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="18" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="1018" min="5" style="18" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="21" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="21" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="1018" min="5" style="21" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="1019" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
-    <row r="1" s="20" customFormat="true" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="19" t="s">
+    <row r="1" s="23" customFormat="true" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" s="22" t="s">
         <v>111</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>114</v>
       </c>
       <c r="AME1" s="0"/>
       <c r="AMF1" s="0"/>
@@ -4615,176 +4604,176 @@
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" s="23" t="n">
+      <c r="A2" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="26" t="n">
         <v>6</v>
       </c>
-      <c r="D2" s="23" t="s">
-        <v>116</v>
+      <c r="D2" s="26" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="21" t="s">
-        <v>117</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" s="23" t="n">
+      <c r="A3" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="26" t="n">
         <v>8</v>
       </c>
-      <c r="D3" s="23" t="s">
-        <v>118</v>
+      <c r="D3" s="26" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4" s="23" t="n">
+      <c r="A4" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="26" t="n">
         <v>5</v>
       </c>
-      <c r="D4" s="23" t="s">
-        <v>116</v>
+      <c r="D4" s="26" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" s="23" t="n">
+      <c r="A5" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="26" t="n">
         <v>8</v>
       </c>
-      <c r="D5" s="23" t="s">
-        <v>121</v>
+      <c r="D5" s="26" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="C6" s="23" t="n">
+      <c r="A6" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="26" t="n">
         <v>4</v>
       </c>
-      <c r="D6" s="23" t="n">
+      <c r="D6" s="26" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="C7" s="23" t="n">
+      <c r="A7" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="26" t="n">
         <v>5</v>
       </c>
-      <c r="D7" s="23" t="n">
+      <c r="D7" s="26" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8" s="23" t="n">
+      <c r="A8" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="26" t="n">
         <v>5</v>
       </c>
-      <c r="D8" s="23" t="n">
+      <c r="D8" s="26" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="C9" s="23" t="n">
+      <c r="A9" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="26" t="n">
         <v>6</v>
       </c>
-      <c r="D9" s="23" t="s">
-        <v>118</v>
+      <c r="D9" s="26" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10" s="23" t="n">
+      <c r="A10" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="26" t="n">
         <v>5</v>
       </c>
-      <c r="D10" s="23" t="s">
-        <v>121</v>
+      <c r="D10" s="26" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="C11" s="23" t="n">
+      <c r="A11" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="26" t="n">
         <v>6</v>
       </c>
-      <c r="D11" s="23" t="s">
-        <v>118</v>
+      <c r="D11" s="26" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="24"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24" t="n">
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27" t="n">
         <v>3</v>
       </c>
-      <c r="D12" s="24"/>
+      <c r="D12" s="27"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="24"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24" t="n">
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27" t="n">
         <v>3</v>
       </c>
-      <c r="D13" s="24"/>
+      <c r="D13" s="27"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="24"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24" t="n">
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27" t="n">
         <v>3</v>
       </c>
-      <c r="D14" s="24"/>
+      <c r="D14" s="27"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="24"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24" t="n">
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27" t="n">
         <v>3</v>
       </c>
-      <c r="D15" s="24"/>
+      <c r="D15" s="27"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
minor change in the template (poc to Power Oral Care)
</commit_message>
<xml_diff>
--- a/Projects/PNGRO/Data/Template.xlsx
+++ b/Projects/PNGRO/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="SBD_kpis" sheetId="1" state="visible" r:id="rId2"/>
@@ -285,7 +285,7 @@
     <t xml:space="preserve">segment = poc(power oral care) and PG adjecent to toothbrush sub cat</t>
   </si>
   <si>
-    <t xml:space="preserve">poc</t>
+    <t xml:space="preserve">Power Oral Care</t>
   </si>
   <si>
     <t xml:space="preserve">TOOTHBRUSH</t>
@@ -773,23 +773,23 @@
   <dimension ref="1:13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="63.412955465587"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="63.9514170040486"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="17.3522267206478"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.8866396761134"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="14.8906882591093"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="78.0890688259109"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="24.8502024291498"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="31.3846153846154"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="78.8380566801619"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="25.0647773279352"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="31.5991902834008"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="26.5668016194332"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="1" width="10.8178137651822"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="1" width="16.3886639676113"/>
@@ -4590,9 +4590,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="15" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="15" width="22.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="15" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="15" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="15" width="21.3157894736842"/>
     <col collapsed="false" hidden="false" max="1018" min="5" style="15" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="1019" style="0" width="9.10526315789474"/>
   </cols>

</xml_diff>

<commit_message>
changes to the branch
</commit_message>
<xml_diff>
--- a/Projects/PNGRO/Data/Template.xlsx
+++ b/Projects/PNGRO/Data/Template.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="134">
   <si>
     <t xml:space="preserve">Retailer </t>
   </si>
@@ -379,6 +379,9 @@
   </si>
   <si>
     <t xml:space="preserve">Fairy SRPs implemented at shelf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRP</t>
   </si>
   <si>
     <t xml:space="preserve">display name</t>
@@ -829,9 +832,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.7085020242915"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="1018" min="5" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="1019" style="0" width="8.57085020242915"/>
   </cols>
@@ -1040,24 +1043,24 @@
   </sheetPr>
   <dimension ref="A1:AMG16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K27" activeCellId="0" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="64.5910931174089"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="8" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="65.1295546558705"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="8" width="17.5668016194332"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="8" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="8" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="8" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="8" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="8" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="8" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="8" width="21.1012145748988"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="8" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="8" width="12.2105263157895"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="8" width="88.2024291497976"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="8" width="30.1012145748988"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="8" width="31.8137651821862"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="8" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="8" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="8" width="89.0161943319838"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="8" width="30.3157894736842"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="8" width="32.0283400809717"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="8" width="26.995951417004"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="8" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="8" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="8" width="16.497975708502"/>
@@ -4666,8 +4669,12 @@
         <v>44</v>
       </c>
       <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
+      <c r="K14" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="L14" s="26" t="s">
+        <v>113</v>
+      </c>
       <c r="M14" s="26" t="s">
         <v>46</v>
       </c>
@@ -4754,15 +4761,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B2" s="8" t="n">
         <v>2</v>
@@ -4770,7 +4777,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B3" s="8" t="n">
         <v>1.5</v>
@@ -4778,7 +4785,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B4" s="8" t="n">
         <v>2</v>
@@ -4786,7 +4793,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B5" s="8" t="n">
         <v>2</v>
@@ -4794,7 +4801,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B6" s="8" t="n">
         <v>3</v>
@@ -4802,7 +4809,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B7" s="8" t="n">
         <v>4</v>
@@ -4810,7 +4817,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B8" s="8" t="n">
         <v>5</v>
@@ -4818,7 +4825,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B9" s="8" t="n">
         <v>2</v>
@@ -4826,7 +4833,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B10" s="8" t="n">
         <v>4</v>
@@ -4834,7 +4841,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B11" s="8" t="n">
         <v>6</v>
@@ -4842,7 +4849,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B12" s="8" t="n">
         <v>1</v>
@@ -4850,7 +4857,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B13" s="8" t="n">
         <v>1</v>
@@ -4858,7 +4865,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B14" s="8" t="n">
         <v>0.5</v>
@@ -4866,7 +4873,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B15" s="8" t="n">
         <v>0.25</v>
@@ -4874,7 +4881,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B16" s="8" t="n">
         <v>0.5</v>
@@ -4882,7 +4889,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B17" s="8" t="n">
         <v>1</v>
@@ -4890,7 +4897,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B18" s="8" t="n">
         <v>0.3</v>
@@ -4898,7 +4905,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B19" s="8" t="n">
         <v>0.1</v>

</xml_diff>

<commit_message>
adding facings sos calculations code
</commit_message>
<xml_diff>
--- a/Projects/PNGRO/Data/Template.xlsx
+++ b/Projects/PNGRO/Data/Template.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="135">
   <si>
     <t xml:space="preserve">Retailer </t>
   </si>
@@ -379,6 +379,9 @@
   </si>
   <si>
     <t xml:space="preserve">Fairy SRPs implemented at shelf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOS Facing</t>
   </si>
   <si>
     <t xml:space="preserve">SRP</t>
@@ -832,9 +835,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.8178137651822"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.9595141700405"/>
     <col collapsed="false" hidden="false" max="1018" min="5" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="1019" style="0" width="8.57085020242915"/>
   </cols>
@@ -1043,24 +1046,24 @@
   </sheetPr>
   <dimension ref="A1:AMG16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K27" activeCellId="0" sqref="K27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="65.1295546558705"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="8" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="65.663967611336"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="8" width="17.6761133603239"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="8" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="8" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="8" width="13.0688259109312"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="8" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="8" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="8" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="8" width="21.2105263157895"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="8" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="8" width="12.3198380566802"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="8" width="89.0161943319838"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="8" width="30.3157894736842"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="8" width="32.0283400809717"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="8" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="8" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="8" width="89.7651821862348"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="8" width="30.5303643724696"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="8" width="32.2429149797571"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="8" width="27.2064777327935"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="8" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="8" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="8" width="16.497975708502"/>
@@ -4663,17 +4666,17 @@
       <c r="F14" s="26"/>
       <c r="G14" s="26"/>
       <c r="H14" s="28" t="s">
-        <v>43</v>
+        <v>113</v>
       </c>
       <c r="I14" s="28" t="s">
         <v>44</v>
       </c>
       <c r="J14" s="26"/>
       <c r="K14" s="26" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L14" s="26" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="M14" s="26" t="s">
         <v>46</v>
@@ -4761,15 +4764,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B2" s="8" t="n">
         <v>2</v>
@@ -4777,7 +4780,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B3" s="8" t="n">
         <v>1.5</v>
@@ -4785,7 +4788,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B4" s="8" t="n">
         <v>2</v>
@@ -4793,7 +4796,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B5" s="8" t="n">
         <v>2</v>
@@ -4801,7 +4804,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B6" s="8" t="n">
         <v>3</v>
@@ -4809,7 +4812,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B7" s="8" t="n">
         <v>4</v>
@@ -4817,7 +4820,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B8" s="8" t="n">
         <v>5</v>
@@ -4825,7 +4828,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B9" s="8" t="n">
         <v>2</v>
@@ -4833,7 +4836,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B10" s="8" t="n">
         <v>4</v>
@@ -4841,7 +4844,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B11" s="8" t="n">
         <v>6</v>
@@ -4849,7 +4852,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B12" s="8" t="n">
         <v>1</v>
@@ -4857,7 +4860,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B13" s="8" t="n">
         <v>1</v>
@@ -4865,7 +4868,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B14" s="8" t="n">
         <v>0.5</v>
@@ -4873,7 +4876,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B15" s="8" t="n">
         <v>0.25</v>
@@ -4881,7 +4884,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B16" s="8" t="n">
         <v>0.5</v>
@@ -4889,7 +4892,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B17" s="8" t="n">
         <v>1</v>
@@ -4897,7 +4900,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B18" s="8" t="n">
         <v>0.3</v>
@@ -4905,7 +4908,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B19" s="8" t="n">
         <v>0.1</v>

</xml_diff>

<commit_message>
adding eye level kpi
</commit_message>
<xml_diff>
--- a/Projects/PNGRO/Data/Template.xlsx
+++ b/Projects/PNGRO/Data/Template.xlsx
@@ -11,6 +11,7 @@
     <sheet name="Eye-level" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="SBD_kpis" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="display weight" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="eye_level_parameters" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0" vbProcedure="false">SBD_kpis!$A$2:$X$41</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="141">
   <si>
     <t xml:space="preserve">Retailer </t>
   </si>
@@ -387,6 +388,12 @@
     <t xml:space="preserve">SRP</t>
   </si>
   <si>
+    <t xml:space="preserve">Head&amp;Shoulders at eye level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eye Level</t>
+  </si>
+  <si>
     <t xml:space="preserve">display name</t>
   </si>
   <si>
@@ -445,6 +452,18 @@
   </si>
   <si>
     <t xml:space="preserve">Parasite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of shelves min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of shelves max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ignore from top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ignore from bottom</t>
   </si>
 </sst>
 </file>
@@ -454,7 +473,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF626468"/>
@@ -526,6 +545,14 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -583,7 +610,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="14">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -596,6 +623,90 @@
       <right style="hair"/>
       <top style="hair"/>
       <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="thin"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="medium"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom style="medium"/>
       <diagonal/>
     </border>
   </borders>
@@ -628,7 +739,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="42">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -749,6 +860,54 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -829,15 +988,15 @@
   </sheetPr>
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.9230769230769"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.1740890688259"/>
     <col collapsed="false" hidden="false" max="1018" min="5" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="1019" style="0" width="8.57085020242915"/>
   </cols>
@@ -1046,26 +1205,26 @@
   </sheetPr>
   <dimension ref="A1:AMG16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="65.663967611336"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="8" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="66.1983805668016"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="8" width="17.7813765182186"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="8" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="8" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="8" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="8" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="8" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="8" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="8" width="21.3157894736842"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="8" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="8" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="8" width="89.7651821862348"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="8" width="30.5303643724696"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="8" width="32.2429149797571"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="8" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="8" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="8" width="90.5141700404858"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="8" width="30.7449392712551"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="8" width="32.4574898785425"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="8" width="27.4210526315789"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="8" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="8" width="10.497975708502"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="8" width="12.7165991902834"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="8" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="8" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="1021" min="18" style="8" width="9.10526315789474"/>
@@ -4691,23 +4850,37 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="26"/>
+      <c r="A15" s="26" t="s">
+        <v>115</v>
+      </c>
       <c r="B15" s="26"/>
       <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
+      <c r="D15" s="27" t="s">
+        <v>42</v>
+      </c>
       <c r="E15" s="26"/>
       <c r="F15" s="26"/>
       <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
+      <c r="H15" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="I15" s="28" t="s">
+        <v>52</v>
+      </c>
       <c r="J15" s="26"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
+      <c r="K15" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="L15" s="26" t="s">
+        <v>109</v>
+      </c>
       <c r="M15" s="29"/>
       <c r="N15" s="29"/>
-      <c r="O15" s="29"/>
-      <c r="P15" s="29"/>
-      <c r="Q15" s="29"/>
+      <c r="O15" s="26"/>
+      <c r="P15" s="26"/>
+      <c r="Q15" s="29" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="26"/>
@@ -4752,8 +4925,8 @@
   </sheetPr>
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4764,15 +4937,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B2" s="8" t="n">
         <v>2</v>
@@ -4780,7 +4953,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B3" s="8" t="n">
         <v>1.5</v>
@@ -4788,7 +4961,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B4" s="8" t="n">
         <v>2</v>
@@ -4796,7 +4969,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B5" s="8" t="n">
         <v>2</v>
@@ -4804,7 +4977,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B6" s="8" t="n">
         <v>3</v>
@@ -4812,7 +4985,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B7" s="8" t="n">
         <v>4</v>
@@ -4820,7 +4993,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B8" s="8" t="n">
         <v>5</v>
@@ -4828,7 +5001,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B9" s="8" t="n">
         <v>2</v>
@@ -4836,7 +5009,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B10" s="8" t="n">
         <v>4</v>
@@ -4844,7 +5017,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B11" s="8" t="n">
         <v>6</v>
@@ -4852,7 +5025,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B12" s="8" t="n">
         <v>1</v>
@@ -4860,7 +5033,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B13" s="8" t="n">
         <v>1</v>
@@ -4868,7 +5041,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B14" s="8" t="n">
         <v>0.5</v>
@@ -4876,7 +5049,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B15" s="8" t="n">
         <v>0.25</v>
@@ -4884,7 +5057,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B16" s="8" t="n">
         <v>0.5</v>
@@ -4892,7 +5065,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B17" s="8" t="n">
         <v>1</v>
@@ -4900,7 +5073,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B18" s="8" t="n">
         <v>0.3</v>
@@ -4908,10 +5081,125 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B19" s="8" t="n">
         <v>0.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3441295546559"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.1943319838057"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.8744939271255"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.6963562753036"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="33" t="n">
+        <v>3</v>
+      </c>
+      <c r="B2" s="33" t="n">
+        <v>3</v>
+      </c>
+      <c r="C2" s="34" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="35" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="36" t="n">
+        <v>4</v>
+      </c>
+      <c r="B3" s="36" t="n">
+        <v>4</v>
+      </c>
+      <c r="C3" s="37" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="38" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="36" t="n">
+        <v>5</v>
+      </c>
+      <c r="B4" s="36" t="n">
+        <v>5</v>
+      </c>
+      <c r="C4" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="38" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="36" t="n">
+        <v>6</v>
+      </c>
+      <c r="B5" s="36" t="n">
+        <v>6</v>
+      </c>
+      <c r="C5" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="38" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="39" t="n">
+        <v>7</v>
+      </c>
+      <c r="B6" s="39" t="n">
+        <v>100</v>
+      </c>
+      <c r="C6" s="40" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="41" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes to filters etc
</commit_message>
<xml_diff>
--- a/Projects/PNGRO/Data/Template.xlsx
+++ b/Projects/PNGRO/Data/Template.xlsx
@@ -16,23 +16,24 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">SBD_kpis!$A$3:$AD$35</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0" vbProcedure="false">SBD_kpis!$C$3:$AK$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0" vbProcedure="false">SBD_kpis!$C$3:$AK$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AK$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AK$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AK$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AK$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AK$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AK$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AK$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AK$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AK$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AK$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AK$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AK$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">SBD_kpis!$C$3:$AK$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">SBD_kpis!$A$3:$AD$35</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">SBD_kpis!$C$3:$AK$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">SBD_kpis!$A$3:$AC$35</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">SBD_kpis!$A$3:$AC$35</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -49,7 +50,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="AA28" authorId="0">
+    <comment ref="X28" authorId="0">
       <text>
         <r>
           <rPr>
@@ -80,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="209">
   <si>
     <t xml:space="preserve">Retailer </t>
   </si>
@@ -151,6 +152,12 @@
     <t xml:space="preserve">Scoring</t>
   </si>
   <si>
+    <t xml:space="preserve">Group 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">By Retailer</t>
   </si>
   <si>
@@ -179,9 +186,6 @@
   </si>
   <si>
     <t xml:space="preserve">KPI Calc. Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KPI Logic*</t>
   </si>
   <si>
     <t xml:space="preserve">Param Type (1)/ Numerator</t>
@@ -226,16 +230,19 @@
     <t xml:space="preserve">Param (3) Values</t>
   </si>
   <si>
-    <t xml:space="preserve">Param (4)</t>
+    <t xml:space="preserve">Facings</t>
   </si>
   <si>
-    <t xml:space="preserve">Param (4) Values</t>
+    <t xml:space="preserve">Min Shelf Number</t>
   </si>
   <si>
     <t xml:space="preserve">Manufacturer</t>
   </si>
   <si>
     <t xml:space="preserve">Target Policy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPI Logic*</t>
   </si>
   <si>
     <t xml:space="preserve">Is Mach3 segment 50% of Gillette Systems shelf?</t>
@@ -257,9 +264,6 @@
     <t xml:space="preserve">Precentages </t>
   </si>
   <si>
-    <t xml:space="preserve">Form = Mach3 out of segment=systems, PNG</t>
-  </si>
-  <si>
     <t xml:space="preserve">brand_name</t>
   </si>
   <si>
@@ -272,6 +276,9 @@
     <t xml:space="preserve">Systems</t>
   </si>
   <si>
+    <t xml:space="preserve">Form = Mach3 out of segment=systems, PNG</t>
+  </si>
+  <si>
     <t xml:space="preserve">Is lemon scent min 40% of Fairy shelf?</t>
   </si>
   <si>
@@ -281,9 +288,6 @@
     <t xml:space="preserve">Precentages</t>
   </si>
   <si>
-    <t xml:space="preserve">Brand = Fairy and Benefit = lemon out of Brand=fairy</t>
-  </si>
-  <si>
     <t xml:space="preserve">Benefit</t>
   </si>
   <si>
@@ -291,6 +295,9 @@
   </si>
   <si>
     <t xml:space="preserve">Fairy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brand = Fairy and Benefit = lemon out of Brand=fairy</t>
   </si>
   <si>
     <t xml:space="preserve">Are Pantene Gold skus placed in the middle of the Pantene shelf?</t>
@@ -305,9 +312,6 @@
     <t xml:space="preserve">Binary</t>
   </si>
   <si>
-    <t xml:space="preserve">survey question</t>
-  </si>
-  <si>
     <t xml:space="preserve">question_text</t>
   </si>
   <si>
@@ -320,6 +324,9 @@
     <t xml:space="preserve">Da</t>
   </si>
   <si>
+    <t xml:space="preserve">survey question</t>
+  </si>
+  <si>
     <t xml:space="preserve">Is Always Platinum min 15% of Always Pads shelf?</t>
   </si>
   <si>
@@ -327,9 +334,6 @@
   </si>
   <si>
     <t xml:space="preserve">Fem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brand=always and sub-category =pads and form=Platinum out of Brand=always and sub category=pads</t>
   </si>
   <si>
     <t xml:space="preserve">ALWAYS</t>
@@ -347,13 +351,13 @@
     <t xml:space="preserve">Platinum</t>
   </si>
   <si>
+    <t xml:space="preserve">Brand=always and sub-category =pads and form=Platinum out of Brand=always and sub category=pads</t>
+  </si>
+  <si>
     <t xml:space="preserve">Is Ariel Liquid Tabs min 15% from total Laundry category?</t>
   </si>
   <si>
     <t xml:space="preserve">Laundry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brand=Ariel and form=Liquid tabs out of Category=Laundry</t>
   </si>
   <si>
     <t xml:space="preserve">Ariel</t>
@@ -368,13 +372,13 @@
     <t xml:space="preserve">Liquid Tabs</t>
   </si>
   <si>
+    <t xml:space="preserve">Brand=Ariel and form=Liquid tabs out of Category=Laundry</t>
+  </si>
+  <si>
     <t xml:space="preserve">Is Blue collection min 30% from Lenor shelf?</t>
   </si>
   <si>
     <t xml:space="preserve">Fabric Enhancers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brand =Lenor and form=liquid and benefit = Spring out of Brand =lenor and form=liquid</t>
   </si>
   <si>
     <t xml:space="preserve">Liquid</t>
@@ -386,13 +390,13 @@
     <t xml:space="preserve">SPRING</t>
   </si>
   <si>
+    <t xml:space="preserve">Brand =Lenor and form=liquid and benefit = Spring out of Brand =lenor and form=liquid</t>
+  </si>
+  <si>
     <t xml:space="preserve">Is Pants min 25% of Pampers shelf?</t>
   </si>
   <si>
     <t xml:space="preserve">Baby</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> category=diapers and brand = pampers and segment=pants out of category=diapers and brand=pampers</t>
   </si>
   <si>
     <t xml:space="preserve">DIAPERS</t>
@@ -404,19 +408,22 @@
     <t xml:space="preserve">Taped</t>
   </si>
   <si>
+    <t xml:space="preserve"> category=diapers and brand = pampers and segment=pants out of category=diapers and brand=pampers</t>
+  </si>
+  <si>
     <t xml:space="preserve">POC listed and placed within brushing</t>
   </si>
   <si>
     <t xml:space="preserve">Relative Position</t>
   </si>
   <si>
-    <t xml:space="preserve">segment = poc(power oral care) and PG adjecent to toothbrush sub cat</t>
-  </si>
-  <si>
     <t xml:space="preserve">Power Oral Care</t>
   </si>
   <si>
     <t xml:space="preserve">TOOTHBRUSH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">segment = poc(power oral care) and PG adjecent to toothbrush sub cat</t>
   </si>
   <si>
     <t xml:space="preserve">Are Female Blades &amp; Razors placed in a distinct block than male Blades &amp; Razors?</t>
@@ -434,13 +441,13 @@
     <t xml:space="preserve">Shelf Position</t>
   </si>
   <si>
-    <t xml:space="preserve">segment = poc(power oral care) and PG at eye level according to eye level matrix (TBD)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Old Category Name</t>
   </si>
   <si>
     <t xml:space="preserve">ORAL CARE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">segment = poc(power oral care) and PG at eye level according to eye level matrix (TBD)</t>
   </si>
   <si>
     <t xml:space="preserve">Are H&amp;S male skus placed in hair care main shelf?</t>
@@ -533,16 +540,10 @@
     <t xml:space="preserve">HAIR CARE</t>
   </si>
   <si>
-    <t xml:space="preserve">facings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">min_shelf_num</t>
-  </si>
-  <si>
     <t xml:space="preserve">Hair Care vertical brand blocks</t>
   </si>
   <si>
-    <t xml:space="preserve">block_by</t>
+    <t xml:space="preserve">Blocked Together Vertical Brand</t>
   </si>
   <si>
     <t xml:space="preserve">Codisplay: Venus/Male</t>
@@ -872,14 +873,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCFE7F5"/>
-        <bgColor rgb="FFCCFFFF"/>
+        <fgColor rgb="FFF4BE49"/>
+        <bgColor rgb="FFFFD966"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF4BE49"/>
-        <bgColor rgb="FFFFD966"/>
+        <fgColor rgb="FFCFE7F5"/>
+        <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -1012,7 +1013,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1053,6 +1054,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1061,11 +1066,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1073,7 +1074,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1117,15 +1118,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1137,7 +1138,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1195,6 +1196,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1291,9 +1296,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.1012145748988"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="1018" min="5" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="1019" style="0" width="8.57085020242915"/>
   </cols>
@@ -1500,46 +1505,47 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMF35"/>
+  <dimension ref="1:35"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AA34" activeCellId="0" sqref="AA34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.1821862348178"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="48.6315789473684"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="8" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="8" width="17.7813765182186"/>
-    <col collapsed="false" hidden="true" max="9" min="7" style="8" width="0"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="8" width="27.4210526315789"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="8" width="15.3886639676113"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="8" width="84.6032388663968"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="8" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="8" width="32.3481781376518"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="8" width="17.2591093117409"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="8" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="8" width="17.2591093117409"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="8" width="18.9514170040486"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="8" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="8" width="41.3481781376518"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="8" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="8" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="24" min="23" style="8" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="8" width="11.3198380566802"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="8" width="18.3157894736842"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="8" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="8" width="30.7449392712551"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="8" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="8" width="14.7813765182186"/>
-    <col collapsed="false" hidden="false" max="1020" min="31" style="8" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="1025" min="1021" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0526315789474"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="49.0607287449393"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="8" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="8" width="14.8825910931174"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="8" width="11.8704453441296"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="8" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="8" width="21.4939271255061"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="8" width="28.1578947368421"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="8" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="8" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="8" width="32.5627530364372"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="8" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="8" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="8" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="8" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="8" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="8" width="30.7004048582996"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="8" width="13.7125506072874"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="8" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="8" width="16.9595141700405"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="8" width="10.497975708502"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="8" width="11.3562753036437"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="8" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="28" min="26" style="8" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="8" width="14.8906882591093"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="8" width="85.2672064777328"/>
+    <col collapsed="false" hidden="false" max="1019" min="31" style="8" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1025" min="1020" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" s="10" customFormat="true" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="11" customFormat="true" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
         <v>18</v>
       </c>
@@ -1553,14 +1559,14 @@
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9" t="s">
+      <c r="K1" s="10"/>
+      <c r="L1" s="9" t="s">
         <v>21</v>
       </c>
+      <c r="M1" s="9"/>
       <c r="N1" s="9"/>
       <c r="O1" s="9"/>
       <c r="P1" s="9"/>
@@ -1576,12 +1582,15 @@
       <c r="Z1" s="9"/>
       <c r="AA1" s="9"/>
       <c r="AB1" s="9"/>
-      <c r="AC1" s="9"/>
-      <c r="AD1" s="9" t="s">
+      <c r="AC1" s="9" t="s">
         <v>22</v>
       </c>
+      <c r="AD1" s="9"/>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" s="10" customFormat="true" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="11" customFormat="true" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -1593,18 +1602,22 @@
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
+      <c r="L2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
       <c r="X2" s="9"/>
       <c r="Y2" s="9"/>
       <c r="Z2" s="9"/>
@@ -1612,98 +1625,104 @@
       <c r="AB2" s="9"/>
       <c r="AC2" s="9"/>
       <c r="AD2" s="9"/>
+      <c r="AMH2" s="0"/>
+      <c r="AMI2" s="0"/>
+      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>24</v>
+      <c r="A3" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N3" s="12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="P3" s="12" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="R3" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="S3" s="12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="T3" s="12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="U3" s="12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="V3" s="12" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="W3" s="12" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="X3" s="12" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="Y3" s="12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="Z3" s="12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AA3" s="12" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="AB3" s="12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AC3" s="12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AD3" s="12" t="s">
-        <v>51</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="AMH3" s="0"/>
+      <c r="AMI3" s="0"/>
+      <c r="AMJ3" s="0"/>
     </row>
     <row r="4" s="20" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="15"/>
@@ -1711,45 +1730,43 @@
         <v>1</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G4" s="19"/>
       <c r="H4" s="19"/>
       <c r="I4" s="19"/>
       <c r="J4" s="19" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="K4" s="19" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L4" s="19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M4" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="N4" s="19" t="s">
-        <v>60</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="N4" s="19"/>
       <c r="O4" s="19"/>
       <c r="P4" s="19"/>
       <c r="Q4" s="19"/>
-      <c r="R4" s="19"/>
+      <c r="R4" s="19" t="s">
+        <v>62</v>
+      </c>
       <c r="S4" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="T4" s="19" t="s">
-        <v>62</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="T4" s="19"/>
       <c r="U4" s="19"/>
       <c r="V4" s="19"/>
       <c r="W4" s="19"/>
@@ -1758,10 +1775,15 @@
       <c r="Z4" s="19"/>
       <c r="AA4" s="19"/>
       <c r="AB4" s="19"/>
-      <c r="AC4" s="19"/>
-      <c r="AD4" s="19" t="n">
+      <c r="AC4" s="19" t="n">
         <v>50</v>
       </c>
+      <c r="AD4" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="AMH4" s="0"/>
+      <c r="AMI4" s="0"/>
+      <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="15"/>
@@ -1769,45 +1791,43 @@
         <v>2</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
       <c r="J5" s="19" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="K5" s="19" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L5" s="19" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M5" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="N5" s="19" t="s">
-        <v>68</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="N5" s="19"/>
       <c r="O5" s="19"/>
       <c r="P5" s="19"/>
       <c r="Q5" s="19"/>
-      <c r="R5" s="19"/>
+      <c r="R5" s="19" t="s">
+        <v>60</v>
+      </c>
       <c r="S5" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="T5" s="19" t="s">
-        <v>69</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="T5" s="19"/>
       <c r="U5" s="19"/>
       <c r="V5" s="19"/>
       <c r="W5" s="19"/>
@@ -1816,9 +1836,11 @@
       <c r="Z5" s="19"/>
       <c r="AA5" s="19"/>
       <c r="AB5" s="19"/>
-      <c r="AC5" s="19"/>
-      <c r="AD5" s="19" t="n">
+      <c r="AC5" s="19" t="n">
         <v>40</v>
+      </c>
+      <c r="AD5" s="19" t="s">
+        <v>71</v>
       </c>
       <c r="AE5" s="0"/>
       <c r="AF5" s="0"/>
@@ -2809,7 +2831,6 @@
       <c r="AMC5" s="0"/>
       <c r="AMD5" s="0"/>
       <c r="AME5" s="0"/>
-      <c r="AMF5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="15"/>
@@ -2817,45 +2838,43 @@
         <v>3</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G6" s="19"/>
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
       <c r="J6" s="19" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="K6" s="19" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="L6" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="M6" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="N6" s="22" t="s">
         <v>76</v>
       </c>
+      <c r="M6" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="N6" s="22"/>
       <c r="O6" s="22"/>
       <c r="P6" s="22"/>
       <c r="Q6" s="22"/>
-      <c r="R6" s="22"/>
+      <c r="R6" s="19" t="s">
+        <v>78</v>
+      </c>
       <c r="S6" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="T6" s="19" t="s">
-        <v>78</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="T6" s="19"/>
       <c r="U6" s="19"/>
       <c r="V6" s="19"/>
       <c r="W6" s="19"/>
@@ -2865,7 +2884,9 @@
       <c r="AA6" s="19"/>
       <c r="AB6" s="19"/>
       <c r="AC6" s="19"/>
-      <c r="AD6" s="19"/>
+      <c r="AD6" s="19" t="s">
+        <v>80</v>
+      </c>
       <c r="AE6" s="0"/>
       <c r="AF6" s="0"/>
       <c r="AG6" s="0"/>
@@ -3855,7 +3876,6 @@
       <c r="AMC6" s="0"/>
       <c r="AMD6" s="0"/>
       <c r="AME6" s="0"/>
-      <c r="AMF6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="15"/>
@@ -3863,60 +3883,60 @@
         <v>4</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G7" s="19"/>
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
       <c r="J7" s="19" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="K7" s="19" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L7" s="19" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="M7" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="N7" s="19" t="s">
-        <v>83</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="N7" s="19"/>
       <c r="O7" s="19"/>
       <c r="P7" s="19"/>
       <c r="Q7" s="19"/>
-      <c r="R7" s="19"/>
+      <c r="R7" s="19" t="s">
+        <v>85</v>
+      </c>
       <c r="S7" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="T7" s="19" t="s">
-        <v>85</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="T7" s="19"/>
       <c r="U7" s="19"/>
       <c r="V7" s="19"/>
       <c r="W7" s="19"/>
-      <c r="X7" s="19"/>
+      <c r="X7" s="19" t="s">
+        <v>87</v>
+      </c>
       <c r="Y7" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="Z7" s="19" t="s">
-        <v>87</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="Z7" s="19"/>
       <c r="AA7" s="19"/>
       <c r="AB7" s="19"/>
-      <c r="AC7" s="19"/>
-      <c r="AD7" s="19" t="n">
+      <c r="AC7" s="19" t="n">
         <v>15</v>
+      </c>
+      <c r="AD7" s="19" t="s">
+        <v>89</v>
       </c>
       <c r="AE7" s="0"/>
       <c r="AF7" s="0"/>
@@ -4907,7 +4927,6 @@
       <c r="AMC7" s="0"/>
       <c r="AMD7" s="0"/>
       <c r="AME7" s="0"/>
-      <c r="AMF7" s="0"/>
     </row>
     <row r="8" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="15"/>
@@ -4915,61 +4934,64 @@
         <v>5</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G8" s="19"/>
       <c r="H8" s="19"/>
       <c r="I8" s="19"/>
       <c r="J8" s="19" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="K8" s="19" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L8" s="19" t="s">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="M8" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="N8" s="19" t="s">
-        <v>91</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="N8" s="19"/>
       <c r="O8" s="19"/>
       <c r="P8" s="19"/>
       <c r="Q8" s="19"/>
-      <c r="R8" s="19"/>
+      <c r="R8" s="19" t="s">
+        <v>93</v>
+      </c>
       <c r="S8" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="T8" s="19" t="s">
-        <v>93</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="T8" s="19"/>
       <c r="U8" s="19"/>
       <c r="V8" s="19"/>
       <c r="W8" s="19"/>
-      <c r="X8" s="19"/>
+      <c r="X8" s="19" t="s">
+        <v>87</v>
+      </c>
       <c r="Y8" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="Z8" s="19" t="s">
-        <v>94</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="Z8" s="19"/>
       <c r="AA8" s="19"/>
       <c r="AB8" s="19"/>
-      <c r="AC8" s="19"/>
-      <c r="AD8" s="19" t="n">
+      <c r="AC8" s="19" t="n">
         <v>15</v>
       </c>
+      <c r="AD8" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="AMH8" s="0"/>
+      <c r="AMI8" s="0"/>
+      <c r="AMJ8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="15"/>
@@ -4977,60 +4999,60 @@
         <v>6</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G9" s="19"/>
       <c r="H9" s="19"/>
       <c r="I9" s="19"/>
       <c r="J9" s="19" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="K9" s="19" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L9" s="19" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="M9" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="N9" s="19" t="s">
-        <v>98</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="N9" s="19"/>
       <c r="O9" s="19"/>
       <c r="P9" s="19"/>
       <c r="Q9" s="19"/>
-      <c r="R9" s="19"/>
+      <c r="R9" s="19" t="s">
+        <v>60</v>
+      </c>
       <c r="S9" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="T9" s="19" t="s">
-        <v>99</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="T9" s="19"/>
       <c r="U9" s="19"/>
       <c r="V9" s="19"/>
       <c r="W9" s="19"/>
-      <c r="X9" s="19"/>
+      <c r="X9" s="19" t="s">
+        <v>68</v>
+      </c>
       <c r="Y9" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z9" s="19" t="s">
-        <v>100</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="Z9" s="19"/>
       <c r="AA9" s="19"/>
       <c r="AB9" s="19"/>
-      <c r="AC9" s="19"/>
-      <c r="AD9" s="19" t="n">
+      <c r="AC9" s="19" t="n">
         <v>30</v>
+      </c>
+      <c r="AD9" s="19" t="s">
+        <v>102</v>
       </c>
       <c r="AE9" s="0"/>
       <c r="AF9" s="0"/>
@@ -6021,7 +6043,6 @@
       <c r="AMC9" s="0"/>
       <c r="AMD9" s="0"/>
       <c r="AME9" s="0"/>
-      <c r="AMF9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="15"/>
@@ -6029,60 +6050,60 @@
         <v>7</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
       <c r="I10" s="19"/>
       <c r="J10" s="19" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="K10" s="19" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L10" s="19" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="M10" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="N10" s="19" t="s">
-        <v>104</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="N10" s="19"/>
       <c r="O10" s="19"/>
       <c r="P10" s="19"/>
       <c r="Q10" s="19"/>
-      <c r="R10" s="19"/>
+      <c r="R10" s="19" t="s">
+        <v>60</v>
+      </c>
       <c r="S10" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="T10" s="19" t="s">
-        <v>105</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="T10" s="19"/>
       <c r="U10" s="19"/>
       <c r="V10" s="19"/>
       <c r="W10" s="19"/>
-      <c r="X10" s="19"/>
+      <c r="X10" s="19" t="s">
+        <v>87</v>
+      </c>
       <c r="Y10" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="Z10" s="19" t="s">
-        <v>106</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="Z10" s="19"/>
       <c r="AA10" s="19"/>
       <c r="AB10" s="19"/>
-      <c r="AC10" s="19"/>
-      <c r="AD10" s="19" t="n">
+      <c r="AC10" s="19" t="n">
         <v>25</v>
+      </c>
+      <c r="AD10" s="19" t="s">
+        <v>108</v>
       </c>
       <c r="AE10" s="0"/>
       <c r="AF10" s="0"/>
@@ -7073,7 +7094,6 @@
       <c r="AMC10" s="0"/>
       <c r="AMD10" s="0"/>
       <c r="AME10" s="0"/>
-      <c r="AMF10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="15"/>
@@ -7081,7 +7101,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D11" s="17" t="s">
         <v>5</v>
@@ -7090,36 +7110,34 @@
         <v>5</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G11" s="19"/>
       <c r="H11" s="19"/>
       <c r="I11" s="19"/>
       <c r="J11" s="19" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="K11" s="19" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="L11" s="19" t="s">
-        <v>109</v>
+        <v>62</v>
       </c>
       <c r="M11" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="N11" s="19" t="s">
-        <v>110</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="N11" s="19"/>
       <c r="O11" s="19"/>
       <c r="P11" s="19"/>
       <c r="Q11" s="19"/>
-      <c r="R11" s="19"/>
+      <c r="R11" s="19" t="s">
+        <v>93</v>
+      </c>
       <c r="S11" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="T11" s="19" t="s">
-        <v>111</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="T11" s="19"/>
       <c r="U11" s="19"/>
       <c r="V11" s="19"/>
       <c r="W11" s="19"/>
@@ -7129,7 +7147,9 @@
       <c r="AA11" s="19"/>
       <c r="AB11" s="19"/>
       <c r="AC11" s="19"/>
-      <c r="AD11" s="19"/>
+      <c r="AD11" s="19" t="s">
+        <v>113</v>
+      </c>
       <c r="AE11" s="0"/>
       <c r="AF11" s="0"/>
       <c r="AG11" s="0"/>
@@ -8119,7 +8139,6 @@
       <c r="AMC11" s="0"/>
       <c r="AMD11" s="0"/>
       <c r="AME11" s="0"/>
-      <c r="AMF11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="15"/>
@@ -8127,45 +8146,43 @@
         <v>9</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G12" s="19"/>
       <c r="H12" s="19"/>
       <c r="I12" s="19"/>
       <c r="J12" s="19" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="K12" s="19" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="L12" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="M12" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="N12" s="22" t="s">
-        <v>114</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="M12" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="N12" s="22"/>
       <c r="O12" s="22"/>
       <c r="P12" s="22"/>
       <c r="Q12" s="22"/>
-      <c r="R12" s="22"/>
+      <c r="R12" s="19" t="s">
+        <v>78</v>
+      </c>
       <c r="S12" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="T12" s="19" t="s">
-        <v>78</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="T12" s="19"/>
       <c r="U12" s="19"/>
       <c r="V12" s="19"/>
       <c r="W12" s="19"/>
@@ -8175,7 +8192,9 @@
       <c r="AA12" s="19"/>
       <c r="AB12" s="19"/>
       <c r="AC12" s="19"/>
-      <c r="AD12" s="19"/>
+      <c r="AD12" s="19" t="s">
+        <v>80</v>
+      </c>
       <c r="AE12" s="0"/>
       <c r="AF12" s="0"/>
       <c r="AG12" s="0"/>
@@ -9165,7 +9184,6 @@
       <c r="AMC12" s="0"/>
       <c r="AMD12" s="0"/>
       <c r="AME12" s="0"/>
-      <c r="AMF12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="15"/>
@@ -9173,7 +9191,7 @@
         <v>10</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D13" s="17" t="s">
         <v>5</v>
@@ -9182,36 +9200,34 @@
         <v>5</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G13" s="19"/>
       <c r="H13" s="19"/>
       <c r="I13" s="19"/>
       <c r="J13" s="19" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="K13" s="19" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="L13" s="19" t="s">
-        <v>117</v>
+        <v>62</v>
       </c>
       <c r="M13" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="N13" s="19" t="s">
-        <v>110</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="N13" s="19"/>
       <c r="O13" s="19"/>
       <c r="P13" s="19"/>
       <c r="Q13" s="19"/>
-      <c r="R13" s="19"/>
+      <c r="R13" s="19" t="s">
+        <v>119</v>
+      </c>
       <c r="S13" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="T13" s="19" t="s">
-        <v>119</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="T13" s="19"/>
       <c r="U13" s="19"/>
       <c r="V13" s="19"/>
       <c r="W13" s="19"/>
@@ -9220,9 +9236,11 @@
       <c r="Z13" s="19"/>
       <c r="AA13" s="19"/>
       <c r="AB13" s="19"/>
-      <c r="AC13" s="19"/>
+      <c r="AC13" s="19" t="s">
+        <v>11</v>
+      </c>
       <c r="AD13" s="19" t="s">
-        <v>11</v>
+        <v>121</v>
       </c>
       <c r="AE13" s="0"/>
       <c r="AF13" s="0"/>
@@ -10213,7 +10231,6 @@
       <c r="AMC13" s="0"/>
       <c r="AMD13" s="0"/>
       <c r="AME13" s="0"/>
-      <c r="AMF13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="15"/>
@@ -10221,43 +10238,43 @@
         <v>11</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G14" s="25"/>
       <c r="H14" s="25"/>
       <c r="I14" s="25"/>
       <c r="J14" s="26" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K14" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="L14" s="25"/>
-      <c r="M14" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="N14" s="25" t="s">
-        <v>122</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="L14" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="M14" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="N14" s="25"/>
       <c r="O14" s="25"/>
       <c r="P14" s="25"/>
       <c r="Q14" s="25"/>
-      <c r="R14" s="25"/>
+      <c r="R14" s="25" t="s">
+        <v>125</v>
+      </c>
       <c r="S14" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="T14" s="25" t="s">
-        <v>124</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="T14" s="25"/>
       <c r="U14" s="25"/>
       <c r="V14" s="25"/>
       <c r="W14" s="25"/>
@@ -11257,63 +11274,62 @@
       <c r="AMC14" s="0"/>
       <c r="AMD14" s="0"/>
       <c r="AME14" s="0"/>
-      <c r="AMF14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="15" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B15" s="15" t="n">
         <v>12</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F15" s="26" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
       <c r="I15" s="15"/>
       <c r="J15" s="27" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="K15" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="L15" s="15"/>
+        <v>59</v>
+      </c>
+      <c r="L15" s="15" t="s">
+        <v>131</v>
+      </c>
       <c r="M15" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="N15" s="15" t="s">
-        <v>129</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="N15" s="15"/>
       <c r="O15" s="15"/>
       <c r="P15" s="15"/>
       <c r="Q15" s="15"/>
-      <c r="R15" s="15"/>
+      <c r="R15" s="15" t="s">
+        <v>60</v>
+      </c>
       <c r="S15" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="T15" s="15" t="s">
-        <v>69</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="T15" s="15"/>
       <c r="U15" s="15"/>
       <c r="V15" s="15"/>
       <c r="W15" s="15"/>
-      <c r="X15" s="15"/>
+      <c r="X15" s="28"/>
       <c r="Y15" s="28"/>
       <c r="Z15" s="28"/>
       <c r="AA15" s="28"/>
       <c r="AB15" s="28"/>
-      <c r="AC15" s="28"/>
-      <c r="AD15" s="26"/>
+      <c r="AC15" s="26"/>
+      <c r="AD15" s="15"/>
       <c r="AE15" s="0"/>
       <c r="AF15" s="0"/>
       <c r="AG15" s="0"/>
@@ -12303,43 +12319,42 @@
       <c r="AMC15" s="0"/>
       <c r="AMD15" s="0"/>
       <c r="AME15" s="0"/>
-      <c r="AMF15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="15" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B16" s="15" t="n">
         <v>13</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F16" s="26" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
       <c r="J16" s="26" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="K16" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="L16" s="26"/>
+        <v>67</v>
+      </c>
+      <c r="L16" s="26" t="s">
+        <v>60</v>
+      </c>
       <c r="M16" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="N16" s="26" t="s">
-        <v>122</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="N16" s="26"/>
       <c r="O16" s="26"/>
       <c r="P16" s="26"/>
       <c r="Q16" s="26"/>
@@ -13345,43 +13360,42 @@
       <c r="AMC16" s="0"/>
       <c r="AMD16" s="0"/>
       <c r="AME16" s="0"/>
-      <c r="AMF16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="15" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B17" s="15" t="n">
         <v>14</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D17" s="29"/>
       <c r="E17" s="29"/>
       <c r="F17" s="26" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
       <c r="I17" s="15"/>
       <c r="J17" s="26" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="K17" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26" t="s">
-        <v>135</v>
-      </c>
-      <c r="N17" s="30" t="s">
-        <v>136</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="L17" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="M17" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="N17" s="31"/>
       <c r="O17" s="31"/>
       <c r="P17" s="31"/>
       <c r="Q17" s="31"/>
-      <c r="R17" s="31"/>
+      <c r="R17" s="26"/>
       <c r="S17" s="26"/>
       <c r="T17" s="26"/>
       <c r="U17" s="26"/>
@@ -14383,43 +14397,42 @@
       <c r="AMC17" s="0"/>
       <c r="AMD17" s="0"/>
       <c r="AME17" s="0"/>
-      <c r="AMF17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="15" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B18" s="15" t="n">
         <v>15</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D18" s="29"/>
       <c r="E18" s="29"/>
       <c r="F18" s="26" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
       <c r="I18" s="15"/>
       <c r="J18" s="26" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="K18" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="L18" s="26"/>
-      <c r="M18" s="26" t="s">
-        <v>135</v>
-      </c>
-      <c r="N18" s="30" t="s">
-        <v>136</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="L18" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="M18" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="N18" s="31"/>
       <c r="O18" s="31"/>
       <c r="P18" s="31"/>
       <c r="Q18" s="31"/>
-      <c r="R18" s="31"/>
+      <c r="R18" s="26"/>
       <c r="S18" s="26"/>
       <c r="T18" s="26"/>
       <c r="U18" s="26"/>
@@ -15421,43 +15434,42 @@
       <c r="AMC18" s="0"/>
       <c r="AMD18" s="0"/>
       <c r="AME18" s="0"/>
-      <c r="AMF18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="15" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B19" s="15" t="n">
         <v>16</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D19" s="29"/>
       <c r="E19" s="29"/>
       <c r="F19" s="26" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G19" s="15"/>
       <c r="H19" s="15"/>
       <c r="I19" s="15"/>
       <c r="J19" s="26" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="K19" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26" t="s">
-        <v>135</v>
-      </c>
-      <c r="N19" s="30" t="s">
-        <v>136</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="L19" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="M19" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="N19" s="31"/>
       <c r="O19" s="31"/>
       <c r="P19" s="31"/>
       <c r="Q19" s="31"/>
-      <c r="R19" s="31"/>
+      <c r="R19" s="26"/>
       <c r="S19" s="26"/>
       <c r="T19" s="26"/>
       <c r="U19" s="26"/>
@@ -16459,43 +16471,42 @@
       <c r="AMC19" s="0"/>
       <c r="AMD19" s="0"/>
       <c r="AME19" s="0"/>
-      <c r="AMF19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="15" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B20" s="15" t="n">
         <v>17</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D20" s="29"/>
       <c r="E20" s="29"/>
       <c r="F20" s="26" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
       <c r="I20" s="15"/>
       <c r="J20" s="26" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="K20" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="L20" s="26"/>
-      <c r="M20" s="26" t="s">
-        <v>135</v>
-      </c>
-      <c r="N20" s="30" t="s">
-        <v>136</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="L20" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="M20" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="N20" s="31"/>
       <c r="O20" s="31"/>
       <c r="P20" s="31"/>
       <c r="Q20" s="31"/>
-      <c r="R20" s="31"/>
+      <c r="R20" s="26"/>
       <c r="S20" s="26"/>
       <c r="T20" s="26"/>
       <c r="U20" s="26"/>
@@ -17497,49 +17508,48 @@
       <c r="AMC20" s="0"/>
       <c r="AMD20" s="0"/>
       <c r="AME20" s="0"/>
-      <c r="AMF20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="15" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B21" s="15" t="n">
         <v>18</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D21" s="29"/>
       <c r="E21" s="29"/>
       <c r="F21" s="26" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G21" s="15"/>
       <c r="H21" s="15"/>
       <c r="I21" s="15"/>
       <c r="J21" s="26" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="K21" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="L21" s="15"/>
+        <v>75</v>
+      </c>
+      <c r="L21" s="15" t="s">
+        <v>93</v>
+      </c>
       <c r="M21" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="N21" s="15" t="s">
-        <v>142</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="N21" s="15"/>
       <c r="O21" s="15"/>
       <c r="P21" s="15"/>
       <c r="Q21" s="15"/>
-      <c r="R21" s="15"/>
+      <c r="R21" s="15" t="s">
+        <v>93</v>
+      </c>
       <c r="S21" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="T21" s="15" t="s">
-        <v>143</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="T21" s="15"/>
       <c r="U21" s="15"/>
       <c r="V21" s="15"/>
       <c r="W21" s="15"/>
@@ -17547,10 +17557,10 @@
       <c r="Y21" s="15"/>
       <c r="Z21" s="15"/>
       <c r="AA21" s="15"/>
-      <c r="AB21" s="15"/>
-      <c r="AC21" s="26" t="s">
-        <v>144</v>
-      </c>
+      <c r="AB21" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="AC21" s="15"/>
       <c r="AD21" s="15"/>
       <c r="AE21" s="0"/>
       <c r="AF21" s="0"/>
@@ -18541,49 +18551,48 @@
       <c r="AMC21" s="0"/>
       <c r="AMD21" s="0"/>
       <c r="AME21" s="0"/>
-      <c r="AMF21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="15" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B22" s="15" t="n">
         <v>19</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D22" s="29"/>
       <c r="E22" s="29"/>
       <c r="F22" s="26" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
       <c r="I22" s="15"/>
       <c r="J22" s="26" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="K22" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="L22" s="15"/>
+        <v>75</v>
+      </c>
+      <c r="L22" s="15" t="s">
+        <v>93</v>
+      </c>
       <c r="M22" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="N22" s="15" t="s">
-        <v>142</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="N22" s="15"/>
       <c r="O22" s="15"/>
       <c r="P22" s="15"/>
       <c r="Q22" s="15"/>
-      <c r="R22" s="15"/>
+      <c r="R22" s="15" t="s">
+        <v>93</v>
+      </c>
       <c r="S22" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="T22" s="15" t="s">
-        <v>143</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="T22" s="15"/>
       <c r="U22" s="15"/>
       <c r="V22" s="15"/>
       <c r="W22" s="15"/>
@@ -18591,11 +18600,11 @@
       <c r="Y22" s="15"/>
       <c r="Z22" s="15"/>
       <c r="AA22" s="15"/>
-      <c r="AB22" s="15"/>
-      <c r="AC22" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="AD22" s="26"/>
+      <c r="AB22" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="AC22" s="26"/>
+      <c r="AD22" s="15"/>
       <c r="AE22" s="0"/>
       <c r="AF22" s="0"/>
       <c r="AG22" s="0"/>
@@ -19585,69 +19594,64 @@
       <c r="AMC22" s="0"/>
       <c r="AMD22" s="0"/>
       <c r="AME22" s="0"/>
-      <c r="AMF22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="15" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B23" s="15" t="n">
         <v>20</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D23" s="29"/>
       <c r="E23" s="29"/>
       <c r="F23" s="15" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
       <c r="I23" s="15"/>
       <c r="J23" s="15" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="K23" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="L23" s="15"/>
+        <v>75</v>
+      </c>
+      <c r="L23" s="15" t="s">
+        <v>60</v>
+      </c>
       <c r="M23" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="N23" s="15" t="s">
-        <v>148</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="N23" s="15"/>
       <c r="O23" s="15"/>
       <c r="P23" s="15"/>
       <c r="Q23" s="15"/>
-      <c r="R23" s="15"/>
+      <c r="R23" s="15" t="s">
+        <v>93</v>
+      </c>
       <c r="S23" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="T23" s="15" t="s">
-        <v>149</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="T23" s="15"/>
       <c r="U23" s="15"/>
       <c r="V23" s="15"/>
       <c r="W23" s="15"/>
       <c r="X23" s="15"/>
-      <c r="Y23" s="15" t="s">
-        <v>150</v>
-      </c>
+      <c r="Y23" s="15"/>
       <c r="Z23" s="15" t="n">
         <v>2</v>
       </c>
-      <c r="AA23" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="AB23" s="15" t="n">
+      <c r="AA23" s="15" t="n">
         <v>2</v>
       </c>
-      <c r="AC23" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="AD23" s="26"/>
+      <c r="AB23" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="AC23" s="26"/>
+      <c r="AD23" s="15"/>
       <c r="AE23" s="0"/>
       <c r="AF23" s="0"/>
       <c r="AG23" s="0"/>
@@ -20637,11 +20641,10 @@
       <c r="AMC23" s="0"/>
       <c r="AMD23" s="0"/>
       <c r="AME23" s="0"/>
-      <c r="AMF23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="15" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B24" s="15" t="n">
         <v>21</v>
@@ -20652,30 +20655,26 @@
       <c r="D24" s="29"/>
       <c r="E24" s="29"/>
       <c r="F24" s="15" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
       <c r="I24" s="15"/>
       <c r="J24" s="15" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="K24" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="L24" s="15"/>
+        <v>75</v>
+      </c>
+      <c r="L24" s="15" t="s">
+        <v>93</v>
+      </c>
       <c r="M24" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="N24" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="O24" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="P24" s="15" t="s">
-        <v>59</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
       <c r="Q24" s="15"/>
       <c r="R24" s="15"/>
       <c r="S24" s="15"/>
@@ -20684,22 +20683,18 @@
       <c r="V24" s="15"/>
       <c r="W24" s="15"/>
       <c r="X24" s="15"/>
-      <c r="Y24" s="15" t="s">
-        <v>150</v>
-      </c>
+      <c r="Y24" s="15"/>
       <c r="Z24" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="AA24" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="AB24" s="15" t="n">
+      <c r="AA24" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="AC24" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="AD24" s="26"/>
+      <c r="AB24" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="AC24" s="26"/>
+      <c r="AD24" s="15"/>
       <c r="AE24" s="0"/>
       <c r="AF24" s="0"/>
       <c r="AG24" s="0"/>
@@ -21689,11 +21684,10 @@
       <c r="AMC24" s="0"/>
       <c r="AMD24" s="0"/>
       <c r="AME24" s="0"/>
-      <c r="AMF24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="15" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B25" s="15" t="n">
         <v>22</v>
@@ -21704,7 +21698,7 @@
       <c r="D25" s="29"/>
       <c r="E25" s="29"/>
       <c r="F25" s="15" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G25" s="15"/>
       <c r="H25" s="15"/>
@@ -21713,41 +21707,39 @@
         <v>155</v>
       </c>
       <c r="K25" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="L25" s="15"/>
+        <v>67</v>
+      </c>
+      <c r="L25" s="15" t="s">
+        <v>85</v>
+      </c>
       <c r="M25" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="N25" s="15" t="s">
         <v>156</v>
       </c>
+      <c r="N25" s="15"/>
       <c r="O25" s="15"/>
       <c r="P25" s="15"/>
       <c r="Q25" s="15"/>
-      <c r="R25" s="15"/>
+      <c r="R25" s="15" t="s">
+        <v>60</v>
+      </c>
       <c r="S25" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="T25" s="15" t="s">
         <v>157</v>
       </c>
+      <c r="T25" s="15"/>
       <c r="U25" s="15"/>
       <c r="V25" s="15"/>
       <c r="W25" s="15"/>
-      <c r="X25" s="15"/>
-      <c r="Y25" s="15" t="s">
-        <v>150</v>
-      </c>
+      <c r="X25" s="29"/>
+      <c r="Y25" s="29"/>
       <c r="Z25" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="AA25" s="29"/>
-      <c r="AB25" s="29"/>
-      <c r="AC25" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="AD25" s="26"/>
+      <c r="AA25" s="26"/>
+      <c r="AB25" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="AC25" s="26"/>
+      <c r="AD25" s="15"/>
       <c r="AE25" s="0"/>
       <c r="AF25" s="0"/>
       <c r="AG25" s="0"/>
@@ -22737,11 +22729,10 @@
       <c r="AMC25" s="0"/>
       <c r="AMD25" s="0"/>
       <c r="AME25" s="0"/>
-      <c r="AMF25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="15" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B26" s="15" t="n">
         <v>23</v>
@@ -22752,7 +22743,7 @@
       <c r="D26" s="29"/>
       <c r="E26" s="29"/>
       <c r="F26" s="15" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G26" s="15"/>
       <c r="H26" s="15"/>
@@ -22761,45 +22752,43 @@
         <v>155</v>
       </c>
       <c r="K26" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="L26" s="15"/>
+        <v>67</v>
+      </c>
+      <c r="L26" s="15" t="s">
+        <v>93</v>
+      </c>
       <c r="M26" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="N26" s="15" t="s">
-        <v>142</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="N26" s="15"/>
       <c r="O26" s="15"/>
       <c r="P26" s="15"/>
       <c r="Q26" s="15"/>
-      <c r="R26" s="15"/>
+      <c r="R26" s="15" t="s">
+        <v>93</v>
+      </c>
       <c r="S26" s="15" t="s">
-        <v>92</v>
+        <v>145</v>
       </c>
       <c r="T26" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="U26" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="V26" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="U26" s="29" t="s">
         <v>159</v>
       </c>
+      <c r="V26" s="29"/>
       <c r="W26" s="29"/>
       <c r="X26" s="29"/>
-      <c r="Y26" s="15" t="s">
-        <v>150</v>
-      </c>
+      <c r="Y26" s="29"/>
       <c r="Z26" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="AA26" s="29"/>
-      <c r="AB26" s="29"/>
-      <c r="AC26" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="AD26" s="26"/>
+      <c r="AA26" s="26"/>
+      <c r="AB26" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="AC26" s="26"/>
+      <c r="AD26" s="15"/>
       <c r="AE26" s="0"/>
       <c r="AF26" s="0"/>
       <c r="AG26" s="0"/>
@@ -23789,11 +23778,10 @@
       <c r="AMC26" s="0"/>
       <c r="AMD26" s="0"/>
       <c r="AME26" s="0"/>
-      <c r="AMF26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="15" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B27" s="15" t="n">
         <v>24</v>
@@ -23804,7 +23792,7 @@
       <c r="D27" s="29"/>
       <c r="E27" s="29"/>
       <c r="F27" s="15" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
@@ -23813,49 +23801,47 @@
         <v>155</v>
       </c>
       <c r="K27" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="N27" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="L27" s="15" t="s">
         <v>93</v>
       </c>
+      <c r="M27" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="N27" s="15" t="s">
+        <v>87</v>
+      </c>
       <c r="O27" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="P27" s="15" t="s">
         <v>161</v>
       </c>
+      <c r="P27" s="15"/>
       <c r="Q27" s="15"/>
-      <c r="R27" s="15"/>
-      <c r="S27" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="T27" s="29" t="s">
+      <c r="R27" s="15" t="s">
         <v>93</v>
       </c>
+      <c r="S27" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="T27" s="15" t="s">
+        <v>87</v>
+      </c>
       <c r="U27" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="V27" s="15" t="s">
-        <v>94</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="V27" s="15"/>
       <c r="W27" s="15"/>
-      <c r="X27" s="15"/>
-      <c r="Y27" s="15" t="s">
-        <v>150</v>
-      </c>
+      <c r="X27" s="29"/>
+      <c r="Y27" s="29"/>
       <c r="Z27" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="AA27" s="29"/>
-      <c r="AB27" s="29"/>
-      <c r="AC27" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="AD27" s="26"/>
+      <c r="AA27" s="26"/>
+      <c r="AB27" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="AC27" s="26"/>
+      <c r="AD27" s="15"/>
       <c r="AE27" s="0"/>
       <c r="AF27" s="0"/>
       <c r="AG27" s="0"/>
@@ -24845,11 +24831,10 @@
       <c r="AMC27" s="0"/>
       <c r="AMD27" s="0"/>
       <c r="AME27" s="0"/>
-      <c r="AMF27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="15" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B28" s="15" t="n">
         <v>25</v>
@@ -24860,7 +24845,7 @@
       <c r="D28" s="29"/>
       <c r="E28" s="29"/>
       <c r="F28" s="15" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
@@ -24869,45 +24854,43 @@
         <v>155</v>
       </c>
       <c r="K28" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="L28" s="15"/>
+        <v>67</v>
+      </c>
+      <c r="L28" s="15" t="s">
+        <v>93</v>
+      </c>
       <c r="M28" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="N28" s="15" t="s">
         <v>163</v>
       </c>
+      <c r="N28" s="15"/>
       <c r="O28" s="15"/>
       <c r="P28" s="15"/>
       <c r="Q28" s="15"/>
-      <c r="R28" s="15"/>
+      <c r="R28" s="15" t="s">
+        <v>93</v>
+      </c>
       <c r="S28" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="T28" s="15" t="s">
         <v>164</v>
       </c>
+      <c r="T28" s="15"/>
       <c r="U28" s="15"/>
       <c r="V28" s="15"/>
       <c r="W28" s="15"/>
-      <c r="X28" s="15"/>
+      <c r="X28" s="15" t="s">
+        <v>165</v>
+      </c>
       <c r="Y28" s="15" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="Z28" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="AA28" s="15" t="s">
-        <v>165</v>
-      </c>
+      <c r="AA28" s="26"/>
       <c r="AB28" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="AC28" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="AD28" s="26"/>
+        <v>146</v>
+      </c>
+      <c r="AC28" s="26"/>
+      <c r="AD28" s="15"/>
       <c r="AE28" s="0"/>
       <c r="AF28" s="0"/>
       <c r="AG28" s="0"/>
@@ -25897,11 +25880,10 @@
       <c r="AMC28" s="0"/>
       <c r="AMD28" s="0"/>
       <c r="AME28" s="0"/>
-      <c r="AMF28" s="0"/>
     </row>
     <row r="29" s="32" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="15" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B29" s="15" t="n">
         <v>26</v>
@@ -25912,7 +25894,7 @@
       <c r="D29" s="29"/>
       <c r="E29" s="29"/>
       <c r="F29" s="15" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
@@ -25921,53 +25903,54 @@
         <v>155</v>
       </c>
       <c r="K29" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="L29" s="15"/>
+        <v>67</v>
+      </c>
+      <c r="L29" s="15" t="s">
+        <v>93</v>
+      </c>
       <c r="M29" s="15" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="N29" s="15" t="s">
-        <v>104</v>
+        <v>60</v>
       </c>
       <c r="O29" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="P29" s="15" t="s">
         <v>167</v>
       </c>
+      <c r="P29" s="15"/>
       <c r="Q29" s="15"/>
-      <c r="R29" s="15"/>
+      <c r="R29" s="15" t="s">
+        <v>60</v>
+      </c>
       <c r="S29" s="15" t="s">
-        <v>59</v>
+        <v>167</v>
       </c>
       <c r="T29" s="15" t="s">
-        <v>167</v>
+        <v>62</v>
       </c>
       <c r="U29" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="V29" s="15" t="s">
         <v>168</v>
       </c>
+      <c r="V29" s="15"/>
       <c r="W29" s="15"/>
-      <c r="X29" s="15"/>
-      <c r="Y29" s="15" t="s">
-        <v>150</v>
-      </c>
+      <c r="X29" s="29"/>
+      <c r="Y29" s="29"/>
       <c r="Z29" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="AA29" s="29"/>
-      <c r="AB29" s="29"/>
-      <c r="AC29" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="AD29" s="26"/>
+      <c r="AA29" s="26"/>
+      <c r="AB29" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="AC29" s="26"/>
+      <c r="AD29" s="15"/>
+      <c r="AMH29" s="0"/>
+      <c r="AMI29" s="0"/>
+      <c r="AMJ29" s="0"/>
     </row>
     <row r="30" s="32" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="15" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B30" s="15" t="n">
         <v>27</v>
@@ -25978,7 +25961,7 @@
       <c r="D30" s="29"/>
       <c r="E30" s="29"/>
       <c r="F30" s="15" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G30" s="15"/>
       <c r="H30" s="15"/>
@@ -25987,49 +25970,50 @@
         <v>155</v>
       </c>
       <c r="K30" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="L30" s="15"/>
+        <v>67</v>
+      </c>
+      <c r="L30" s="15" t="s">
+        <v>93</v>
+      </c>
       <c r="M30" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="N30" s="15" t="s">
         <v>170</v>
       </c>
+      <c r="N30" s="15"/>
       <c r="O30" s="15"/>
       <c r="P30" s="15"/>
       <c r="Q30" s="15"/>
-      <c r="R30" s="15"/>
+      <c r="R30" s="15" t="s">
+        <v>93</v>
+      </c>
       <c r="S30" s="15" t="s">
-        <v>92</v>
+        <v>170</v>
       </c>
       <c r="T30" s="15" t="s">
-        <v>170</v>
+        <v>62</v>
       </c>
       <c r="U30" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="V30" s="15" t="s">
         <v>171</v>
       </c>
+      <c r="V30" s="15"/>
       <c r="W30" s="15"/>
-      <c r="X30" s="15"/>
-      <c r="Y30" s="15" t="s">
-        <v>150</v>
-      </c>
+      <c r="X30" s="29"/>
+      <c r="Y30" s="29"/>
       <c r="Z30" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="AA30" s="29"/>
-      <c r="AB30" s="29"/>
-      <c r="AC30" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="AD30" s="26"/>
+      <c r="AA30" s="26"/>
+      <c r="AB30" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="AC30" s="26"/>
+      <c r="AD30" s="15"/>
+      <c r="AMH30" s="0"/>
+      <c r="AMI30" s="0"/>
+      <c r="AMJ30" s="0"/>
     </row>
     <row r="31" s="32" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="15" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B31" s="15" t="n">
         <v>28</v>
@@ -26040,7 +26024,7 @@
       <c r="D31" s="29"/>
       <c r="E31" s="29"/>
       <c r="F31" s="15" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G31" s="15"/>
       <c r="H31" s="15"/>
@@ -26049,49 +26033,50 @@
         <v>155</v>
       </c>
       <c r="K31" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="L31" s="15"/>
+        <v>67</v>
+      </c>
+      <c r="L31" s="15" t="s">
+        <v>85</v>
+      </c>
       <c r="M31" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="N31" s="15" t="s">
-        <v>85</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="N31" s="15"/>
       <c r="O31" s="15"/>
       <c r="P31" s="15"/>
       <c r="Q31" s="15"/>
-      <c r="R31" s="15"/>
+      <c r="R31" s="15" t="s">
+        <v>85</v>
+      </c>
       <c r="S31" s="15" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="T31" s="15" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="U31" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="V31" s="15" t="s">
-        <v>87</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="V31" s="15"/>
       <c r="W31" s="15"/>
-      <c r="X31" s="15"/>
-      <c r="Y31" s="15" t="s">
-        <v>150</v>
-      </c>
+      <c r="X31" s="29"/>
+      <c r="Y31" s="29"/>
       <c r="Z31" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="AA31" s="29"/>
-      <c r="AB31" s="29"/>
-      <c r="AC31" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="AD31" s="26"/>
+      <c r="AA31" s="26"/>
+      <c r="AB31" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="AC31" s="26"/>
+      <c r="AD31" s="15"/>
+      <c r="AMH31" s="0"/>
+      <c r="AMI31" s="0"/>
+      <c r="AMJ31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="15" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B32" s="15" t="n">
         <v>29</v>
@@ -26102,7 +26087,7 @@
       <c r="D32" s="29"/>
       <c r="E32" s="29"/>
       <c r="F32" s="15" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G32" s="15"/>
       <c r="H32" s="15"/>
@@ -26111,57 +26096,55 @@
         <v>155</v>
       </c>
       <c r="K32" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="L32" s="15"/>
+        <v>67</v>
+      </c>
+      <c r="L32" s="15" t="s">
+        <v>93</v>
+      </c>
       <c r="M32" s="15" t="s">
-        <v>92</v>
+        <v>174</v>
       </c>
       <c r="N32" s="15" t="s">
-        <v>174</v>
+        <v>60</v>
       </c>
       <c r="O32" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="P32" s="15" t="s">
-        <v>69</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="P32" s="15"/>
       <c r="Q32" s="15"/>
-      <c r="R32" s="15"/>
+      <c r="R32" s="15" t="s">
+        <v>93</v>
+      </c>
       <c r="S32" s="15" t="s">
-        <v>92</v>
+        <v>145</v>
       </c>
       <c r="T32" s="15" t="s">
-        <v>143</v>
+        <v>60</v>
       </c>
       <c r="U32" s="15" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="V32" s="15" t="s">
-        <v>69</v>
+        <v>125</v>
       </c>
       <c r="W32" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="X32" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="Y32" s="15" t="s">
-        <v>150</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="X32" s="29"/>
+      <c r="Y32" s="33"/>
       <c r="Z32" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="AA32" s="33"/>
-      <c r="AB32" s="33"/>
-      <c r="AC32" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="AD32" s="26"/>
+      <c r="AA32" s="26"/>
+      <c r="AB32" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="AC32" s="26"/>
+      <c r="AD32" s="15"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="15" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B33" s="15" t="n">
         <v>30</v>
@@ -26172,7 +26155,7 @@
       <c r="D33" s="29"/>
       <c r="E33" s="29"/>
       <c r="F33" s="15" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G33" s="15"/>
       <c r="H33" s="15"/>
@@ -26181,49 +26164,47 @@
         <v>155</v>
       </c>
       <c r="K33" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="L33" s="15"/>
+        <v>67</v>
+      </c>
+      <c r="L33" s="15" t="s">
+        <v>93</v>
+      </c>
       <c r="M33" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="N33" s="15" t="s">
         <v>164</v>
       </c>
+      <c r="N33" s="15"/>
       <c r="O33" s="15"/>
       <c r="P33" s="15"/>
       <c r="Q33" s="15"/>
-      <c r="R33" s="15"/>
+      <c r="R33" s="15" t="s">
+        <v>93</v>
+      </c>
       <c r="S33" s="15" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="T33" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="U33" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="U33" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="V33" s="15" t="s">
-        <v>110</v>
-      </c>
+      <c r="V33" s="15"/>
       <c r="W33" s="15"/>
-      <c r="X33" s="15"/>
-      <c r="Y33" s="15" t="s">
-        <v>150</v>
-      </c>
+      <c r="X33" s="29"/>
+      <c r="Y33" s="29"/>
       <c r="Z33" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="AA33" s="29"/>
-      <c r="AB33" s="29"/>
-      <c r="AC33" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="AD33" s="26"/>
+      <c r="AA33" s="26"/>
+      <c r="AB33" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="AC33" s="26"/>
+      <c r="AD33" s="15"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="15" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B34" s="15" t="n">
         <v>31</v>
@@ -26234,7 +26215,7 @@
       <c r="D34" s="29"/>
       <c r="E34" s="29"/>
       <c r="F34" s="15" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G34" s="15"/>
       <c r="H34" s="15"/>
@@ -26243,53 +26224,51 @@
         <v>155</v>
       </c>
       <c r="K34" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="L34" s="15"/>
+        <v>67</v>
+      </c>
+      <c r="L34" s="15" t="s">
+        <v>93</v>
+      </c>
       <c r="M34" s="15" t="s">
-        <v>92</v>
+        <v>177</v>
       </c>
       <c r="N34" s="15" t="s">
-        <v>177</v>
+        <v>85</v>
       </c>
       <c r="O34" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="P34" s="15" t="s">
         <v>156</v>
       </c>
+      <c r="P34" s="15"/>
       <c r="Q34" s="15"/>
-      <c r="R34" s="15"/>
+      <c r="R34" s="15" t="s">
+        <v>85</v>
+      </c>
       <c r="S34" s="15" t="s">
-        <v>84</v>
+        <v>156</v>
       </c>
       <c r="T34" s="15" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
       <c r="U34" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="V34" s="15" t="s">
         <v>178</v>
       </c>
+      <c r="V34" s="15"/>
       <c r="W34" s="15"/>
-      <c r="X34" s="15"/>
-      <c r="Y34" s="15" t="s">
-        <v>150</v>
-      </c>
+      <c r="X34" s="29"/>
+      <c r="Y34" s="29"/>
       <c r="Z34" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="AA34" s="29"/>
-      <c r="AB34" s="29"/>
-      <c r="AC34" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="AD34" s="26"/>
+      <c r="AA34" s="26"/>
+      <c r="AB34" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="AC34" s="26"/>
+      <c r="AD34" s="15"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="15" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B35" s="15" t="n">
         <v>32</v>
@@ -26300,7 +26279,7 @@
       <c r="D35" s="29"/>
       <c r="E35" s="29"/>
       <c r="F35" s="15" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G35" s="15"/>
       <c r="H35" s="15"/>
@@ -26309,49 +26288,49 @@
         <v>155</v>
       </c>
       <c r="K35" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="L35" s="15"/>
+        <v>75</v>
+      </c>
+      <c r="L35" s="15" t="s">
+        <v>93</v>
+      </c>
       <c r="M35" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="N35" s="15" t="s">
         <v>163</v>
       </c>
+      <c r="N35" s="15"/>
       <c r="O35" s="15"/>
       <c r="P35" s="15"/>
       <c r="Q35" s="15"/>
-      <c r="R35" s="15"/>
+      <c r="R35" s="15" t="s">
+        <v>62</v>
+      </c>
       <c r="S35" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="T35" s="15" t="s">
-        <v>110</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="T35" s="15"/>
       <c r="U35" s="15"/>
       <c r="V35" s="15"/>
       <c r="W35" s="15"/>
       <c r="X35" s="15"/>
-      <c r="Y35" s="15" t="s">
-        <v>150</v>
-      </c>
+      <c r="Y35" s="15"/>
       <c r="Z35" s="15" t="n">
         <v>4</v>
       </c>
       <c r="AA35" s="15"/>
-      <c r="AB35" s="15"/>
-      <c r="AC35" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="AD35" s="26"/>
+      <c r="AB35" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="AC35" s="26"/>
+      <c r="AD35" s="15"/>
     </row>
   </sheetData>
   <autoFilter ref="A3:AD35"/>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="M1:Z1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:Y1"/>
+    <mergeCell ref="L2:Q2"/>
+    <mergeCell ref="R2:W2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -26558,9 +26537,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.7813765182186"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -26673,179 +26652,179 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="17.3522267206478"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="46" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="46" t="s">
         <v>205</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="46" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="46" t="n">
+      <c r="A2" s="47" t="n">
         <v>12</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="47" t="s">
         <v>207</v>
       </c>
-      <c r="C2" s="46" t="n">
+      <c r="C2" s="47" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="46" t="n">
+      <c r="A3" s="47" t="n">
         <v>12</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="46" t="n">
+      <c r="C3" s="47" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="46" t="n">
+      <c r="A4" s="47" t="n">
         <v>12</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="47" t="s">
         <v>208</v>
       </c>
-      <c r="C4" s="46" t="n">
+      <c r="C4" s="47" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="46" t="n">
+      <c r="A5" s="47" t="n">
         <v>13</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="47" t="s">
         <v>208</v>
       </c>
-      <c r="C5" s="46" t="n">
+      <c r="C5" s="47" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="46" t="n">
+      <c r="A6" s="47" t="n">
         <v>14</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="46" t="n">
+      <c r="C6" s="47" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="46" t="n">
+      <c r="A7" s="47" t="n">
         <v>14</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="47" t="s">
         <v>208</v>
       </c>
-      <c r="C7" s="46" t="n">
+      <c r="C7" s="47" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="46" t="n">
+      <c r="A8" s="47" t="n">
         <v>15</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="46" t="n">
+      <c r="C8" s="47" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="46" t="n">
+      <c r="A9" s="47" t="n">
         <v>18</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="47" t="s">
         <v>208</v>
       </c>
-      <c r="C9" s="46" t="n">
+      <c r="C9" s="47" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="46" t="n">
+      <c r="A10" s="47" t="n">
         <v>18</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="47" t="s">
         <v>207</v>
       </c>
-      <c r="C10" s="46" t="n">
+      <c r="C10" s="47" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="46" t="n">
+      <c r="A11" s="47" t="n">
         <v>20</v>
       </c>
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="47" t="s">
         <v>208</v>
       </c>
-      <c r="C11" s="46"/>
+      <c r="C11" s="47"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="46" t="n">
+      <c r="A12" s="47" t="n">
         <v>21</v>
       </c>
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="47" t="s">
         <v>208</v>
       </c>
-      <c r="C12" s="46"/>
+      <c r="C12" s="47"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="46" t="n">
+      <c r="A13" s="47" t="n">
         <v>22</v>
       </c>
-      <c r="B13" s="46" t="s">
+      <c r="B13" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="46" t="n">
+      <c r="C13" s="47" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="46" t="n">
+      <c r="A14" s="47" t="n">
         <v>23</v>
       </c>
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="47" t="s">
         <v>207</v>
       </c>
-      <c r="C14" s="46" t="n">
+      <c r="C14" s="47" t="n">
         <v>60</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="46" t="n">
+      <c r="A15" s="47" t="n">
         <v>24</v>
       </c>
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="47" t="s">
         <v>208</v>
       </c>
-      <c r="C15" s="46" t="n">
+      <c r="C15" s="47" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="46" t="n">
+      <c r="A16" s="47" t="n">
         <v>25</v>
       </c>
-      <c r="B16" s="46" t="s">
+      <c r="B16" s="47" t="s">
         <v>208</v>
       </c>
-      <c r="C16" s="46" t="n">
+      <c r="C16" s="47" t="n">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
template changes, score changes for product presence
</commit_message>
<xml_diff>
--- a/Projects/PNGRO/Data/Template.xlsx
+++ b/Projects/PNGRO/Data/Template.xlsx
@@ -14,7 +14,7 @@
     <sheet name="retailer_targets" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">SBD_kpis!$A$3:$AD$35</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">SBD_kpis!$A$3:$AC$35</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
@@ -29,12 +29,13 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">SBD_kpis!$A$3:$AC$35</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">SBD_kpis!$A$3:$AD$35</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">SBD_kpis!$A$3:$AC$35</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">SBD_kpis!$A$3:$AC$35</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">SBD_kpis!$A$3:$AD$35</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">SBD_kpis!$A$3:$AC$35</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">SBD_kpis!$A$3:$AD$35</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">SBD_kpis!$A$3:$AC$35</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">SBD_kpis!$A$3:$AC$35</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -55,25 +56,13 @@
       <text>
         <r>
           <rPr>
-            <b val="true"/>
-            <sz val="9"/>
+            <sz val="11"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Maya Dror:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Product Policy</t>
+          <t xml:space="preserve">For this kpi type, the parameter indicates product policy</t>
         </r>
       </text>
     </comment>
@@ -82,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="212">
   <si>
     <t xml:space="preserve">General Data</t>
   </si>
@@ -421,9 +410,6 @@
     <t xml:space="preserve">Male</t>
   </si>
   <si>
-    <t xml:space="preserve">Y</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fairy SRPs implemented at shelf</t>
   </si>
   <si>
@@ -457,10 +443,10 @@
     <t xml:space="preserve">Display Presence</t>
   </si>
   <si>
-    <t xml:space="preserve">display_name</t>
+    <t xml:space="preserve">product_name</t>
   </si>
   <si>
-    <t xml:space="preserve">tbd</t>
+    <t xml:space="preserve">Venus Rack</t>
   </si>
   <si>
     <t xml:space="preserve">share of displays with certain display_name out of all displays</t>
@@ -472,7 +458,13 @@
     <t xml:space="preserve">Display: 2 x Oral Care rack</t>
   </si>
   <si>
+    <t xml:space="preserve">2 x Oral Care rack</t>
+  </si>
+  <si>
     <t xml:space="preserve">Display: Liquid Tabs racks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liquid Tabs racks</t>
   </si>
   <si>
     <t xml:space="preserve">One Dish Display</t>
@@ -490,10 +482,13 @@
     <t xml:space="preserve">P&amp;G</t>
   </si>
   <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
     <t xml:space="preserve">One Dish shelving</t>
   </si>
   <si>
-    <t xml:space="preserve">Pantene Golden River</t>
+    <t xml:space="preserve">Pantene Golden River display</t>
   </si>
   <si>
     <t xml:space="preserve">Blocked Together Vertical</t>
@@ -514,6 +509,9 @@
     <t xml:space="preserve">Codisplay: Venus/Male</t>
   </si>
   <si>
+    <t xml:space="preserve">Shave Care (Male)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Product Presence</t>
   </si>
   <si>
@@ -523,10 +521,16 @@
     <t xml:space="preserve">Venus</t>
   </si>
   <si>
+    <t xml:space="preserve">SHAVE CARE</t>
+  </si>
+  <si>
     <t xml:space="preserve">Codisplay: Fairy HDW w. Fairy ADW/Proper</t>
   </si>
   <si>
     <t xml:space="preserve">MR. Proper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HAND DISH, AUTO DISH</t>
   </si>
   <si>
     <t xml:space="preserve">Codisplay: Liquid Tabs w Laundry</t>
@@ -536,6 +540,9 @@
   </si>
   <si>
     <t xml:space="preserve">Co-display: Oral Care with Beauty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beauty</t>
   </si>
   <si>
     <t xml:space="preserve">SHAVE CARE,HAIR CARE,FEM CARE</t>
@@ -556,7 +563,7 @@
     <t xml:space="preserve">Pants</t>
   </si>
   <si>
-    <t xml:space="preserve">CODISPLAY OF PREMIUM &amp; BEEDS WITHIN LENOR FE</t>
+    <t xml:space="preserve">CODISPLAY OF PREMIUM &amp; BEADS WITHIN LENOR FE</t>
   </si>
   <si>
     <t xml:space="preserve">FABRIC ENHANCERS</t>
@@ -566,6 +573,9 @@
   </si>
   <si>
     <t xml:space="preserve">CODISPLAY PLATINUM WITH PADS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FEM CARE</t>
   </si>
   <si>
     <t xml:space="preserve">CO-DISPLAY PLATINUM ADW WITH FAIRY</t>
@@ -578,9 +588,6 @@
   </si>
   <si>
     <t xml:space="preserve">CO-DISPLAY GILLETTE BLADES WITH GILLETTE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHAVE CARE</t>
   </si>
   <si>
     <t xml:space="preserve">Blades</t>
@@ -670,29 +677,48 @@
     <t xml:space="preserve">Retailer Target</t>
   </si>
   <si>
-    <t xml:space="preserve">AUCHAN</t>
+    <t xml:space="preserve">SELGROS</t>
   </si>
   <si>
     <t xml:space="preserve">PROFI</t>
   </si>
   <si>
-    <t xml:space="preserve">SELGROS</t>
+    <t xml:space="preserve">AUCHAN</t>
   </si>
   <si>
     <t xml:space="preserve">CARREFOUR</t>
   </si>
   <si>
+    <t xml:space="preserve">CARREFOUR M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CORA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KAUFLAND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIDL</t>
+  </si>
+  <si>
     <t xml:space="preserve">MEGA IMAGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">METRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PENNY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF626468"/>
@@ -779,19 +805,11 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="9"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Tahoma"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="1"/>
+      <charset val="177"/>
     </font>
     <font>
       <b val="true"/>
@@ -959,7 +977,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1060,23 +1078,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1207,40 +1233,42 @@
   </sheetPr>
   <dimension ref="1:35"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AD18" activeCellId="0" sqref="AD18"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="C31" activeCellId="0" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="49.8097165991903"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.1052631578947"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.1052631578947"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="21.8542510121457"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="28.4939271255061"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="32.9919028340081"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="24.3157894736842"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.7246963562753"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="50.2388663967611"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.2105263157895"/>
+    <col collapsed="false" hidden="true" max="9" min="7" style="1" width="0"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="33.2064777327935"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="31.4939271255061"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="1" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="17.3522267206478"/>
     <col collapsed="false" hidden="false" max="23" min="23" style="1" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="24" min="24" style="1" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="28" min="26" style="1" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="15.1052631578947"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="86.7651821862348"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="25.5384615384615"/>
+    <col collapsed="false" hidden="false" max="28" min="26" style="1" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="87.5141700404858"/>
     <col collapsed="false" hidden="false" max="1019" min="31" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="1020" style="0" width="8.57085020242915"/>
   </cols>
@@ -11962,20 +11990,18 @@
       <c r="AME14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="s">
-        <v>112</v>
-      </c>
+      <c r="A15" s="8"/>
       <c r="B15" s="8" t="n">
         <v>12</v>
       </c>
       <c r="C15" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>114</v>
-      </c>
       <c r="E15" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F15" s="19" t="s">
         <v>40</v>
@@ -11984,16 +12010,16 @@
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
       <c r="J15" s="20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K15" s="20" t="s">
         <v>42</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N15" s="8"/>
       <c r="O15" s="8"/>
@@ -12014,9 +12040,11 @@
       <c r="Z15" s="21"/>
       <c r="AA15" s="21"/>
       <c r="AB15" s="21"/>
-      <c r="AC15" s="19"/>
+      <c r="AC15" s="19" t="n">
+        <v>30</v>
+      </c>
       <c r="AD15" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AE15" s="0"/>
       <c r="AF15" s="0"/>
@@ -13009,14 +13037,12 @@
       <c r="AME15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="s">
-        <v>112</v>
-      </c>
+      <c r="A16" s="8"/>
       <c r="B16" s="8" t="n">
         <v>13</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>56</v>
@@ -13031,7 +13057,7 @@
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
       <c r="J16" s="19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K16" s="19" t="s">
         <v>50</v>
@@ -13057,9 +13083,11 @@
       <c r="Z16" s="19"/>
       <c r="AA16" s="19"/>
       <c r="AB16" s="19"/>
-      <c r="AC16" s="19"/>
+      <c r="AC16" s="19" t="n">
+        <v>10</v>
+      </c>
       <c r="AD16" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AE16" s="0"/>
       <c r="AF16" s="0"/>
@@ -14052,34 +14080,36 @@
       <c r="AME16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8" t="s">
-        <v>112</v>
-      </c>
+      <c r="A17" s="8"/>
       <c r="B17" s="8" t="n">
         <v>14</v>
       </c>
       <c r="C17" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="19" t="s">
         <v>121</v>
-      </c>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="19" t="s">
-        <v>122</v>
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
       <c r="J17" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K17" s="19" t="s">
         <v>50</v>
       </c>
       <c r="L17" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="M17" s="23" t="s">
         <v>124</v>
-      </c>
-      <c r="M17" s="23" t="s">
-        <v>125</v>
       </c>
       <c r="N17" s="24"/>
       <c r="O17" s="24"/>
@@ -14096,9 +14126,11 @@
       <c r="Z17" s="19"/>
       <c r="AA17" s="19"/>
       <c r="AB17" s="19"/>
-      <c r="AC17" s="19"/>
+      <c r="AC17" s="19" t="n">
+        <v>2</v>
+      </c>
       <c r="AD17" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AE17" s="0"/>
       <c r="AF17" s="0"/>
@@ -15091,34 +15123,36 @@
       <c r="AME17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8" t="s">
-        <v>112</v>
-      </c>
+      <c r="A18" s="8"/>
       <c r="B18" s="8" t="n">
         <v>15</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
+        <v>126</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>49</v>
+      </c>
       <c r="F18" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
       <c r="J18" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K18" s="19" t="s">
         <v>50</v>
       </c>
       <c r="L18" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M18" s="23" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="N18" s="24"/>
       <c r="O18" s="24"/>
@@ -15135,9 +15169,11 @@
       <c r="Z18" s="19"/>
       <c r="AA18" s="19"/>
       <c r="AB18" s="19"/>
-      <c r="AC18" s="19"/>
+      <c r="AC18" s="19" t="n">
+        <v>2</v>
+      </c>
       <c r="AD18" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AE18" s="0"/>
       <c r="AF18" s="0"/>
@@ -16130,34 +16166,36 @@
       <c r="AME18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8" t="s">
-        <v>112</v>
-      </c>
+      <c r="A19" s="8"/>
       <c r="B19" s="8" t="n">
         <v>16</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>128</v>
-      </c>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
+        <v>127</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>93</v>
+      </c>
       <c r="F19" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
       <c r="J19" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K19" s="19" t="s">
         <v>50</v>
       </c>
       <c r="L19" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M19" s="23" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="N19" s="24"/>
       <c r="O19" s="24"/>
@@ -16174,9 +16212,11 @@
       <c r="Z19" s="19"/>
       <c r="AA19" s="19"/>
       <c r="AB19" s="19"/>
-      <c r="AC19" s="19"/>
+      <c r="AC19" s="19" t="n">
+        <v>2</v>
+      </c>
       <c r="AD19" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AE19" s="0"/>
       <c r="AF19" s="0"/>
@@ -17169,34 +17209,36 @@
       <c r="AME19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8" t="s">
-        <v>112</v>
-      </c>
+      <c r="A20" s="8"/>
       <c r="B20" s="8" t="n">
         <v>17</v>
       </c>
       <c r="C20" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
+      <c r="D20" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>74</v>
+      </c>
       <c r="F20" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
       <c r="J20" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K20" s="19" t="s">
         <v>50</v>
       </c>
       <c r="L20" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M20" s="23" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="N20" s="24"/>
       <c r="O20" s="24"/>
@@ -17213,9 +17255,11 @@
       <c r="Z20" s="19"/>
       <c r="AA20" s="19"/>
       <c r="AB20" s="19"/>
-      <c r="AC20" s="19"/>
+      <c r="AC20" s="19" t="n">
+        <v>3</v>
+      </c>
       <c r="AD20" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AE20" s="0"/>
       <c r="AF20" s="0"/>
@@ -18208,25 +18252,27 @@
       <c r="AME20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="8" t="s">
-        <v>112</v>
-      </c>
+      <c r="A21" s="8"/>
       <c r="B21" s="8" t="n">
         <v>18</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
+        <v>131</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>49</v>
+      </c>
       <c r="F21" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
       <c r="J21" s="19" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K21" s="8" t="s">
         <v>58</v>
@@ -18235,7 +18281,7 @@
         <v>76</v>
       </c>
       <c r="M21" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="N21" s="8"/>
       <c r="O21" s="8"/>
@@ -18245,7 +18291,7 @@
         <v>76</v>
       </c>
       <c r="S21" s="8" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="T21" s="8"/>
       <c r="U21" s="8"/>
@@ -18256,9 +18302,11 @@
       <c r="Z21" s="8"/>
       <c r="AA21" s="8"/>
       <c r="AB21" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="AC21" s="8"/>
+        <v>135</v>
+      </c>
+      <c r="AC21" s="25" t="n">
+        <v>100</v>
+      </c>
       <c r="AD21" s="8"/>
       <c r="AE21" s="0"/>
       <c r="AF21" s="0"/>
@@ -19252,16 +19300,20 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
-        <v>112</v>
+        <v>136</v>
       </c>
       <c r="B22" s="8" t="n">
         <v>19</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
+        <v>137</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>49</v>
+      </c>
       <c r="F22" s="19" t="s">
         <v>40</v>
       </c>
@@ -19269,7 +19321,7 @@
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
       <c r="J22" s="19" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K22" s="8" t="s">
         <v>58</v>
@@ -19278,7 +19330,7 @@
         <v>76</v>
       </c>
       <c r="M22" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="N22" s="8"/>
       <c r="O22" s="8"/>
@@ -19288,7 +19340,7 @@
         <v>76</v>
       </c>
       <c r="S22" s="8" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="T22" s="8"/>
       <c r="U22" s="8"/>
@@ -19299,7 +19351,7 @@
       <c r="Z22" s="8"/>
       <c r="AA22" s="8"/>
       <c r="AB22" s="8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="AC22" s="19"/>
       <c r="AD22" s="8"/>
@@ -20294,25 +20346,27 @@
       <c r="AME22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="8" t="s">
-        <v>112</v>
-      </c>
+      <c r="A23" s="8"/>
       <c r="B23" s="8" t="n">
         <v>20</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
+        <v>138</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>56</v>
+      </c>
       <c r="F23" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
       <c r="J23" s="8" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="K23" s="20" t="s">
         <v>58</v>
@@ -20321,7 +20375,7 @@
         <v>43</v>
       </c>
       <c r="M23" s="8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="N23" s="8"/>
       <c r="O23" s="8"/>
@@ -20331,7 +20385,7 @@
         <v>76</v>
       </c>
       <c r="S23" s="8" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="T23" s="8"/>
       <c r="U23" s="8"/>
@@ -20346,9 +20400,11 @@
         <v>2</v>
       </c>
       <c r="AB23" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="AC23" s="19"/>
+        <v>135</v>
+      </c>
+      <c r="AC23" s="19" t="n">
+        <v>33</v>
+      </c>
       <c r="AD23" s="8"/>
       <c r="AE23" s="0"/>
       <c r="AF23" s="0"/>
@@ -21341,17 +21397,19 @@
       <c r="AME23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="8" t="s">
-        <v>112</v>
-      </c>
+      <c r="A24" s="8"/>
       <c r="B24" s="8" t="n">
         <v>21</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
+        <v>142</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>56</v>
+      </c>
       <c r="F24" s="8" t="s">
         <v>40</v>
       </c>
@@ -21359,7 +21417,7 @@
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
       <c r="J24" s="8" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="K24" s="8" t="s">
         <v>58</v>
@@ -21368,7 +21426,7 @@
         <v>76</v>
       </c>
       <c r="M24" s="8" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="N24" s="8"/>
       <c r="O24" s="8"/>
@@ -21389,9 +21447,11 @@
         <v>3</v>
       </c>
       <c r="AB24" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="AC24" s="19"/>
+        <v>135</v>
+      </c>
+      <c r="AC24" s="19" t="n">
+        <v>90</v>
+      </c>
       <c r="AD24" s="8"/>
       <c r="AE24" s="0"/>
       <c r="AF24" s="0"/>
@@ -22384,25 +22444,27 @@
       <c r="AME24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="8" t="s">
-        <v>112</v>
-      </c>
+      <c r="A25" s="8"/>
       <c r="B25" s="8" t="n">
         <v>22</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
+        <v>144</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="26" t="s">
+        <v>145</v>
+      </c>
       <c r="F25" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
       <c r="J25" s="8" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="K25" s="19" t="s">
         <v>50</v>
@@ -22411,7 +22473,7 @@
         <v>68</v>
       </c>
       <c r="M25" s="8" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="N25" s="8"/>
       <c r="O25" s="8"/>
@@ -22421,22 +22483,28 @@
         <v>43</v>
       </c>
       <c r="S25" s="8" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="T25" s="8"/>
       <c r="U25" s="8"/>
       <c r="V25" s="8"/>
       <c r="W25" s="8"/>
-      <c r="X25" s="22"/>
-      <c r="Y25" s="22"/>
+      <c r="X25" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y25" s="22" t="s">
+        <v>149</v>
+      </c>
       <c r="Z25" s="8" t="n">
         <v>4</v>
       </c>
       <c r="AA25" s="19"/>
       <c r="AB25" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="AC25" s="19"/>
+        <v>135</v>
+      </c>
+      <c r="AC25" s="19" t="n">
+        <v>100</v>
+      </c>
       <c r="AD25" s="8"/>
       <c r="AE25" s="0"/>
       <c r="AF25" s="0"/>
@@ -23430,24 +23498,28 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="8" t="s">
-        <v>112</v>
+        <v>136</v>
       </c>
       <c r="B26" s="8" t="n">
         <v>23</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
+        <v>150</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>49</v>
+      </c>
       <c r="F26" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
       <c r="I26" s="8"/>
       <c r="J26" s="8" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="K26" s="19" t="s">
         <v>50</v>
@@ -23456,7 +23528,7 @@
         <v>76</v>
       </c>
       <c r="M26" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="N26" s="8"/>
       <c r="O26" s="8"/>
@@ -23466,24 +23538,28 @@
         <v>76</v>
       </c>
       <c r="S26" s="8" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="T26" s="8" t="s">
         <v>43</v>
       </c>
       <c r="U26" s="22" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="V26" s="22"/>
       <c r="W26" s="22"/>
-      <c r="X26" s="22"/>
-      <c r="Y26" s="22"/>
+      <c r="X26" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y26" s="22" t="s">
+        <v>152</v>
+      </c>
       <c r="Z26" s="8" t="n">
         <v>4</v>
       </c>
       <c r="AA26" s="19"/>
       <c r="AB26" s="8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="AC26" s="19"/>
       <c r="AD26" s="8"/>
@@ -24478,25 +24554,27 @@
       <c r="AME26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="8" t="s">
-        <v>112</v>
-      </c>
+      <c r="A27" s="8"/>
       <c r="B27" s="8" t="n">
         <v>24</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
+        <v>153</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="E27" s="22" t="s">
+        <v>74</v>
+      </c>
       <c r="F27" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
       <c r="J27" s="8" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="K27" s="19" t="s">
         <v>50</v>
@@ -24511,7 +24589,7 @@
         <v>70</v>
       </c>
       <c r="O27" s="8" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="P27" s="8"/>
       <c r="Q27" s="8"/>
@@ -24529,16 +24607,22 @@
       </c>
       <c r="V27" s="8"/>
       <c r="W27" s="8"/>
-      <c r="X27" s="22"/>
-      <c r="Y27" s="22"/>
+      <c r="X27" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y27" s="22" t="s">
+        <v>77</v>
+      </c>
       <c r="Z27" s="8" t="n">
         <v>4</v>
       </c>
       <c r="AA27" s="19"/>
       <c r="AB27" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="AC27" s="19"/>
+        <v>135</v>
+      </c>
+      <c r="AC27" s="19" t="n">
+        <v>100</v>
+      </c>
       <c r="AD27" s="8"/>
       <c r="AE27" s="0"/>
       <c r="AF27" s="0"/>
@@ -25531,25 +25615,27 @@
       <c r="AME27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="8" t="s">
-        <v>112</v>
-      </c>
+      <c r="A28" s="8"/>
       <c r="B28" s="8" t="n">
         <v>25</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
+        <v>155</v>
+      </c>
+      <c r="D28" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="E28" s="22" t="s">
+        <v>156</v>
+      </c>
       <c r="F28" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
       <c r="J28" s="8" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="K28" s="19" t="s">
         <v>50</v>
@@ -25558,7 +25644,7 @@
         <v>76</v>
       </c>
       <c r="M28" s="8" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="N28" s="8"/>
       <c r="O28" s="8"/>
@@ -25568,26 +25654,28 @@
         <v>76</v>
       </c>
       <c r="S28" s="8" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="T28" s="8"/>
       <c r="U28" s="8"/>
       <c r="V28" s="8"/>
       <c r="W28" s="8"/>
       <c r="X28" s="8" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="Y28" s="8" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="Z28" s="8" t="n">
         <v>4</v>
       </c>
       <c r="AA28" s="19"/>
       <c r="AB28" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="AC28" s="19"/>
+        <v>135</v>
+      </c>
+      <c r="AC28" s="19" t="n">
+        <v>50</v>
+      </c>
       <c r="AD28" s="8"/>
       <c r="AE28" s="0"/>
       <c r="AF28" s="0"/>
@@ -26579,26 +26667,28 @@
       <c r="AMD28" s="0"/>
       <c r="AME28" s="0"/>
     </row>
-    <row r="29" s="25" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="8" t="s">
-        <v>112</v>
-      </c>
+    <row r="29" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="8"/>
       <c r="B29" s="8" t="n">
         <v>26</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
+        <v>160</v>
+      </c>
+      <c r="D29" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>87</v>
+      </c>
       <c r="F29" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
       <c r="I29" s="8"/>
       <c r="J29" s="8" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="K29" s="19" t="s">
         <v>50</v>
@@ -26613,7 +26703,7 @@
         <v>43</v>
       </c>
       <c r="O29" s="8" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="P29" s="8"/>
       <c r="Q29" s="8"/>
@@ -26621,51 +26711,59 @@
         <v>43</v>
       </c>
       <c r="S29" s="8" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="T29" s="8" t="s">
         <v>45</v>
       </c>
       <c r="U29" s="8" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="V29" s="8"/>
       <c r="W29" s="8"/>
-      <c r="X29" s="22"/>
-      <c r="Y29" s="22"/>
+      <c r="X29" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y29" s="22" t="s">
+        <v>88</v>
+      </c>
       <c r="Z29" s="8" t="n">
         <v>4</v>
       </c>
       <c r="AA29" s="19"/>
       <c r="AB29" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="AC29" s="19"/>
+        <v>135</v>
+      </c>
+      <c r="AC29" s="19" t="n">
+        <v>100</v>
+      </c>
       <c r="AD29" s="8"/>
       <c r="AMH29" s="0"/>
       <c r="AMI29" s="0"/>
       <c r="AMJ29" s="0"/>
     </row>
-    <row r="30" s="25" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="8" t="s">
-        <v>112</v>
-      </c>
+    <row r="30" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="8"/>
       <c r="B30" s="8" t="n">
         <v>27</v>
       </c>
-      <c r="C30" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
+      <c r="C30" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="D30" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>81</v>
+      </c>
       <c r="F30" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
       <c r="I30" s="8"/>
       <c r="J30" s="8" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="K30" s="19" t="s">
         <v>50</v>
@@ -26674,7 +26772,7 @@
         <v>76</v>
       </c>
       <c r="M30" s="8" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="N30" s="8"/>
       <c r="O30" s="8"/>
@@ -26684,51 +26782,59 @@
         <v>76</v>
       </c>
       <c r="S30" s="8" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="T30" s="8" t="s">
         <v>45</v>
       </c>
       <c r="U30" s="8" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="V30" s="8"/>
       <c r="W30" s="8"/>
-      <c r="X30" s="22"/>
-      <c r="Y30" s="22"/>
+      <c r="X30" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y30" s="22" t="s">
+        <v>164</v>
+      </c>
       <c r="Z30" s="8" t="n">
         <v>4</v>
       </c>
       <c r="AA30" s="19"/>
       <c r="AB30" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="AC30" s="19"/>
+        <v>135</v>
+      </c>
+      <c r="AC30" s="19" t="n">
+        <v>50</v>
+      </c>
       <c r="AD30" s="8"/>
       <c r="AMH30" s="0"/>
       <c r="AMI30" s="0"/>
       <c r="AMJ30" s="0"/>
     </row>
-    <row r="31" s="25" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="8" t="s">
-        <v>112</v>
-      </c>
+    <row r="31" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="8"/>
       <c r="B31" s="8" t="n">
         <v>28</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
+        <v>166</v>
+      </c>
+      <c r="D31" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E31" s="22" t="s">
+        <v>66</v>
+      </c>
       <c r="F31" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
       <c r="I31" s="8"/>
       <c r="J31" s="8" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="K31" s="19" t="s">
         <v>50</v>
@@ -26757,41 +26863,49 @@
       </c>
       <c r="V31" s="8"/>
       <c r="W31" s="8"/>
-      <c r="X31" s="22"/>
-      <c r="Y31" s="22"/>
+      <c r="X31" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y31" s="22" t="s">
+        <v>167</v>
+      </c>
       <c r="Z31" s="8" t="n">
         <v>4</v>
       </c>
       <c r="AA31" s="19"/>
       <c r="AB31" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="AC31" s="19"/>
+        <v>135</v>
+      </c>
+      <c r="AC31" s="19" t="n">
+        <v>100</v>
+      </c>
       <c r="AD31" s="8"/>
       <c r="AMH31" s="0"/>
       <c r="AMI31" s="0"/>
       <c r="AMJ31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="8" t="s">
-        <v>112</v>
-      </c>
+      <c r="A32" s="8"/>
       <c r="B32" s="8" t="n">
         <v>29</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
+        <v>168</v>
+      </c>
+      <c r="D32" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E32" s="22" t="s">
+        <v>49</v>
+      </c>
       <c r="F32" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
       <c r="I32" s="8"/>
       <c r="J32" s="8" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="K32" s="19" t="s">
         <v>50</v>
@@ -26800,7 +26914,7 @@
         <v>76</v>
       </c>
       <c r="M32" s="8" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="N32" s="8" t="s">
         <v>43</v>
@@ -26814,7 +26928,7 @@
         <v>76</v>
       </c>
       <c r="S32" s="8" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="T32" s="8" t="s">
         <v>43</v>
@@ -26828,38 +26942,46 @@
       <c r="W32" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="X32" s="22"/>
-      <c r="Y32" s="26"/>
+      <c r="X32" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y32" s="22" t="s">
+        <v>169</v>
+      </c>
       <c r="Z32" s="8" t="n">
         <v>4</v>
       </c>
       <c r="AA32" s="19"/>
       <c r="AB32" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="AC32" s="19"/>
+        <v>135</v>
+      </c>
+      <c r="AC32" s="19" t="n">
+        <v>50</v>
+      </c>
       <c r="AD32" s="8"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="8" t="s">
-        <v>112</v>
-      </c>
+      <c r="A33" s="8"/>
       <c r="B33" s="8" t="n">
         <v>30</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
+        <v>170</v>
+      </c>
+      <c r="D33" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="E33" s="22" t="s">
+        <v>93</v>
+      </c>
       <c r="F33" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G33" s="8"/>
       <c r="H33" s="8"/>
       <c r="I33" s="8"/>
       <c r="J33" s="8" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="K33" s="19" t="s">
         <v>50</v>
@@ -26868,7 +26990,7 @@
         <v>76</v>
       </c>
       <c r="M33" s="8" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="N33" s="8"/>
       <c r="O33" s="8"/>
@@ -26888,38 +27010,46 @@
       </c>
       <c r="V33" s="8"/>
       <c r="W33" s="8"/>
-      <c r="X33" s="22"/>
-      <c r="Y33" s="22"/>
+      <c r="X33" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y33" s="22" t="s">
+        <v>158</v>
+      </c>
       <c r="Z33" s="8" t="n">
         <v>4</v>
       </c>
       <c r="AA33" s="19"/>
       <c r="AB33" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="AC33" s="19"/>
+        <v>135</v>
+      </c>
+      <c r="AC33" s="19" t="n">
+        <v>50</v>
+      </c>
       <c r="AD33" s="8"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="8" t="s">
-        <v>112</v>
-      </c>
+      <c r="A34" s="8"/>
       <c r="B34" s="8" t="n">
         <v>31</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
+        <v>171</v>
+      </c>
+      <c r="D34" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E34" s="26" t="s">
+        <v>145</v>
+      </c>
       <c r="F34" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
       <c r="J34" s="8" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="K34" s="19" t="s">
         <v>50</v>
@@ -26928,13 +27058,13 @@
         <v>76</v>
       </c>
       <c r="M34" s="8" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="N34" s="8" t="s">
         <v>68</v>
       </c>
       <c r="O34" s="8" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="P34" s="8"/>
       <c r="Q34" s="8"/>
@@ -26942,40 +27072,48 @@
         <v>68</v>
       </c>
       <c r="S34" s="8" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="T34" s="8" t="s">
         <v>110</v>
       </c>
       <c r="U34" s="8" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="V34" s="8"/>
       <c r="W34" s="8"/>
-      <c r="X34" s="22"/>
-      <c r="Y34" s="22"/>
+      <c r="X34" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y34" s="22" t="s">
+        <v>149</v>
+      </c>
       <c r="Z34" s="8" t="n">
         <v>4</v>
       </c>
       <c r="AA34" s="19"/>
       <c r="AB34" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="AC34" s="19"/>
+        <v>135</v>
+      </c>
+      <c r="AC34" s="19" t="n">
+        <v>50</v>
+      </c>
       <c r="AD34" s="8"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="8" t="s">
-        <v>112</v>
-      </c>
+      <c r="A35" s="8"/>
       <c r="B35" s="8" t="n">
         <v>32</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
+        <v>173</v>
+      </c>
+      <c r="D35" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="E35" s="22" t="s">
+        <v>156</v>
+      </c>
       <c r="F35" s="8" t="s">
         <v>40</v>
       </c>
@@ -26983,7 +27121,7 @@
       <c r="H35" s="8"/>
       <c r="I35" s="8"/>
       <c r="J35" s="8" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="K35" s="8" t="s">
         <v>58</v>
@@ -26992,7 +27130,7 @@
         <v>76</v>
       </c>
       <c r="M35" s="8" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="N35" s="8"/>
       <c r="O35" s="8"/>
@@ -27015,13 +27153,15 @@
       </c>
       <c r="AA35" s="8"/>
       <c r="AB35" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="AC35" s="19"/>
+        <v>135</v>
+      </c>
+      <c r="AC35" s="19" t="n">
+        <v>1</v>
+      </c>
       <c r="AD35" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:AD35"/>
+  <autoFilter ref="A3:AC35"/>
   <mergeCells count="6">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="F1:I1"/>
@@ -27049,8 +27189,8 @@
   </sheetPr>
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -27061,15 +27201,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>2</v>
@@ -27077,7 +27217,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>1.5</v>
@@ -27085,7 +27225,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>2</v>
@@ -27093,7 +27233,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>2</v>
@@ -27101,7 +27241,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>3</v>
@@ -27109,7 +27249,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>4</v>
@@ -27117,7 +27257,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>5</v>
@@ -27125,7 +27265,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>2</v>
@@ -27133,7 +27273,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>4</v>
@@ -27141,7 +27281,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>6</v>
@@ -27149,7 +27289,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>1</v>
@@ -27157,7 +27297,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>1</v>
@@ -27165,7 +27305,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>0.5</v>
@@ -27173,7 +27313,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>0.25</v>
@@ -27181,7 +27321,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>0.5</v>
@@ -27189,7 +27329,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>1</v>
@@ -27197,7 +27337,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="B18" s="1" t="n">
         <v>0.3</v>
@@ -27205,7 +27345,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="B19" s="1" t="n">
         <v>0.1</v>
@@ -27229,99 +27369,99 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="23.6720647773279"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.1012145748988"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="27" t="s">
-        <v>188</v>
-      </c>
-      <c r="B1" s="27" t="s">
-        <v>189</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>190</v>
-      </c>
-      <c r="D1" s="29" t="s">
-        <v>191</v>
+      <c r="A1" s="29" t="s">
+        <v>194</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="n">
+      <c r="A2" s="32" t="n">
         <v>3</v>
       </c>
-      <c r="B2" s="30" t="n">
+      <c r="B2" s="32" t="n">
         <v>3</v>
       </c>
-      <c r="C2" s="31" t="n">
+      <c r="C2" s="33" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="32" t="n">
+      <c r="D2" s="34" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="33" t="n">
+      <c r="A3" s="35" t="n">
         <v>4</v>
       </c>
-      <c r="B3" s="33" t="n">
+      <c r="B3" s="35" t="n">
         <v>4</v>
       </c>
-      <c r="C3" s="34" t="n">
+      <c r="C3" s="36" t="n">
         <v>0</v>
       </c>
-      <c r="D3" s="35" t="n">
+      <c r="D3" s="37" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="33" t="n">
+      <c r="A4" s="35" t="n">
         <v>5</v>
       </c>
-      <c r="B4" s="33" t="n">
+      <c r="B4" s="35" t="n">
         <v>5</v>
       </c>
-      <c r="C4" s="34" t="n">
+      <c r="C4" s="36" t="n">
         <v>1</v>
       </c>
-      <c r="D4" s="35" t="n">
+      <c r="D4" s="37" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="33" t="n">
+      <c r="A5" s="35" t="n">
         <v>6</v>
       </c>
-      <c r="B5" s="33" t="n">
+      <c r="B5" s="35" t="n">
         <v>6</v>
       </c>
-      <c r="C5" s="34" t="n">
+      <c r="C5" s="36" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="35" t="n">
+      <c r="D5" s="37" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="36" t="n">
+      <c r="A6" s="38" t="n">
         <v>7</v>
       </c>
-      <c r="B6" s="36" t="n">
+      <c r="B6" s="38" t="n">
         <v>100</v>
       </c>
-      <c r="C6" s="37" t="n">
+      <c r="C6" s="39" t="n">
         <v>1</v>
       </c>
-      <c r="D6" s="38" t="n">
+      <c r="D6" s="40" t="n">
         <v>2</v>
       </c>
     </row>
@@ -27341,189 +27481,271 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M24" activeCellId="0" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2834008097166"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1983805668016"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="39" t="s">
-        <v>192</v>
-      </c>
-      <c r="B1" s="39" t="s">
-        <v>193</v>
-      </c>
-      <c r="C1" s="39" t="s">
-        <v>194</v>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="41" t="s">
+        <v>198</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>199</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="40" t="n">
-        <v>12</v>
-      </c>
-      <c r="B2" s="40" t="s">
-        <v>195</v>
-      </c>
-      <c r="C2" s="40" t="n">
-        <v>30</v>
+      <c r="A2" s="42" t="n">
+        <v>19</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>201</v>
+      </c>
+      <c r="C2" s="42" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="40" t="n">
-        <v>12</v>
-      </c>
-      <c r="B3" s="40" t="s">
-        <v>196</v>
-      </c>
-      <c r="C3" s="40" t="n">
-        <v>30</v>
+      <c r="A3" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="40" t="n">
-        <v>12</v>
-      </c>
-      <c r="B4" s="40" t="s">
-        <v>197</v>
-      </c>
-      <c r="C4" s="40" t="n">
-        <v>30</v>
+      <c r="A4" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="40" t="n">
-        <v>13</v>
-      </c>
-      <c r="B5" s="40" t="s">
-        <v>197</v>
-      </c>
-      <c r="C5" s="40" t="n">
-        <v>10</v>
+      <c r="A5" s="42" t="n">
+        <v>19</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="40" t="n">
-        <v>14</v>
-      </c>
-      <c r="B6" s="40" t="s">
-        <v>198</v>
-      </c>
-      <c r="C6" s="40" t="n">
-        <v>2</v>
+      <c r="A6" s="42" t="n">
+        <v>19</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="40" t="n">
-        <v>14</v>
-      </c>
-      <c r="B7" s="40" t="s">
-        <v>197</v>
-      </c>
-      <c r="C7" s="40" t="n">
-        <v>2</v>
+      <c r="A7" s="42" t="n">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="40" t="n">
-        <v>15</v>
-      </c>
-      <c r="B8" s="40" t="s">
-        <v>196</v>
-      </c>
-      <c r="C8" s="40" t="n">
-        <v>2</v>
+      <c r="A8" s="42" t="n">
+        <v>19</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="40" t="n">
-        <v>18</v>
-      </c>
-      <c r="B9" s="40" t="s">
-        <v>197</v>
-      </c>
-      <c r="C9" s="40" t="n">
-        <v>1</v>
+      <c r="A9" s="42" t="n">
+        <v>19</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="40" t="n">
-        <v>18</v>
-      </c>
-      <c r="B10" s="40" t="s">
-        <v>195</v>
-      </c>
-      <c r="C10" s="40" t="n">
-        <v>1</v>
+      <c r="A10" s="42" t="n">
+        <v>19</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="40" t="n">
-        <v>20</v>
-      </c>
-      <c r="B11" s="40" t="s">
-        <v>197</v>
-      </c>
-      <c r="C11" s="40"/>
+      <c r="A11" s="42" t="n">
+        <v>19</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="40" t="n">
-        <v>21</v>
-      </c>
-      <c r="B12" s="40" t="s">
-        <v>197</v>
-      </c>
-      <c r="C12" s="40"/>
+      <c r="A12" s="42" t="n">
+        <v>19</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="40" t="n">
-        <v>22</v>
-      </c>
-      <c r="B13" s="40" t="s">
-        <v>199</v>
-      </c>
-      <c r="C13" s="40" t="n">
+      <c r="A13" s="42" t="n">
+        <v>19</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="C13" s="0" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="40" t="n">
-        <v>23</v>
-      </c>
-      <c r="B14" s="40" t="s">
-        <v>195</v>
-      </c>
-      <c r="C14" s="40" t="n">
-        <v>60</v>
+      <c r="A14" s="42" t="n">
+        <v>19</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="40" t="n">
-        <v>24</v>
-      </c>
-      <c r="B15" s="40" t="s">
-        <v>197</v>
-      </c>
-      <c r="C15" s="40" t="n">
+      <c r="A15" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="C15" s="0" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="40" t="n">
-        <v>25</v>
-      </c>
-      <c r="B16" s="40" t="s">
-        <v>197</v>
-      </c>
-      <c r="C16" s="40" t="n">
-        <v>50</v>
+      <c r="A16" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding comments to template
</commit_message>
<xml_diff>
--- a/Projects/PNGRO/Data/Template.xlsx
+++ b/Projects/PNGRO/Data/Template.xlsx
@@ -14,7 +14,7 @@
     <sheet name="retailer_targets" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">SBD_kpis!$A$3:$AC$35</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">SBD_kpis!$A$3:$AD$35</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
@@ -29,13 +29,14 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">SBD_kpis!$A$3:$AD$35</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">SBD_kpis!$A$3:$AC$35</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">SBD_kpis!$A$3:$AD$35</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">SBD_kpis!$A$3:$AC$35</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">SBD_kpis!$A$3:$AC$35</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">SBD_kpis!$A$3:$AC$35</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">SBD_kpis!$A$3:$AD$35</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">SBD_kpis!$A$3:$AC$35</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">SBD_kpis!$A$3:$AD$35</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">SBD_kpis!$A$3:$AC$35</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$A$3:$AC$35</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">SBD_kpis!$C$3:$AJ$42</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -71,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="213">
   <si>
     <t xml:space="preserve">General Data</t>
   </si>
@@ -480,6 +481,9 @@
   </si>
   <si>
     <t xml:space="preserve">P&amp;G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the kpi passes if there is at least one display that has product blocks from both groups adjacent together. Target policy is ignored</t>
   </si>
   <si>
     <t xml:space="preserve">Y</t>
@@ -1234,41 +1238,41 @@
   <dimension ref="1:35"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="Y4" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topRight" activeCell="Y1" activeCellId="0" sqref="Y1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C31" activeCellId="0" sqref="C31"/>
+      <selection pane="bottomRight" activeCell="AE23" activeCellId="0" sqref="AE23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.7246963562753"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="50.2388663967611"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.8178137651822"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="50.668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.3198380566802"/>
     <col collapsed="false" hidden="true" max="9" min="7" style="1" width="0"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="33.2064777327935"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="17.6761133603239"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="17.6761133603239"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="24.5303643724696"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="31.4939271255061"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="33.5263157894737"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="31.7085020242915"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="1" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="17.4615384615385"/>
     <col collapsed="false" hidden="false" max="23" min="23" style="1" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="24" min="24" style="1" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="25.5384615384615"/>
-    <col collapsed="false" hidden="false" max="28" min="26" style="1" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="87.5141700404858"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="28" min="26" style="1" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="88.3724696356275"/>
     <col collapsed="false" hidden="false" max="1019" min="31" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="1020" style="0" width="8.57085020242915"/>
   </cols>
@@ -18307,7 +18311,9 @@
       <c r="AC21" s="25" t="n">
         <v>100</v>
       </c>
-      <c r="AD21" s="8"/>
+      <c r="AD21" s="8" t="s">
+        <v>136</v>
+      </c>
       <c r="AE21" s="0"/>
       <c r="AF21" s="0"/>
       <c r="AG21" s="0"/>
@@ -19300,13 +19306,13 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B22" s="8" t="n">
         <v>19</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D22" s="22" t="s">
         <v>49</v>
@@ -19354,7 +19360,9 @@
         <v>135</v>
       </c>
       <c r="AC22" s="19"/>
-      <c r="AD22" s="8"/>
+      <c r="AD22" s="8" t="s">
+        <v>136</v>
+      </c>
       <c r="AE22" s="0"/>
       <c r="AF22" s="0"/>
       <c r="AG22" s="0"/>
@@ -20351,7 +20359,7 @@
         <v>20</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D23" s="22" t="s">
         <v>56</v>
@@ -20366,7 +20374,7 @@
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
       <c r="J23" s="8" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="K23" s="20" t="s">
         <v>58</v>
@@ -20375,7 +20383,7 @@
         <v>43</v>
       </c>
       <c r="M23" s="8" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="N23" s="8"/>
       <c r="O23" s="8"/>
@@ -20385,7 +20393,7 @@
         <v>76</v>
       </c>
       <c r="S23" s="8" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="T23" s="8"/>
       <c r="U23" s="8"/>
@@ -21402,7 +21410,7 @@
         <v>21</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D24" s="22" t="s">
         <v>56</v>
@@ -21417,7 +21425,7 @@
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
       <c r="J24" s="8" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="K24" s="8" t="s">
         <v>58</v>
@@ -21426,7 +21434,7 @@
         <v>76</v>
       </c>
       <c r="M24" s="8" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="N24" s="8"/>
       <c r="O24" s="8"/>
@@ -22449,13 +22457,13 @@
         <v>22</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D25" s="22" t="s">
         <v>38</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>121</v>
@@ -22464,7 +22472,7 @@
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
       <c r="J25" s="8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="K25" s="19" t="s">
         <v>50</v>
@@ -22473,7 +22481,7 @@
         <v>68</v>
       </c>
       <c r="M25" s="8" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="N25" s="8"/>
       <c r="O25" s="8"/>
@@ -22483,7 +22491,7 @@
         <v>43</v>
       </c>
       <c r="S25" s="8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="T25" s="8"/>
       <c r="U25" s="8"/>
@@ -22493,7 +22501,7 @@
         <v>76</v>
       </c>
       <c r="Y25" s="22" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="Z25" s="8" t="n">
         <v>4</v>
@@ -23498,13 +23506,13 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B26" s="8" t="n">
         <v>23</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D26" s="22" t="s">
         <v>49</v>
@@ -23519,7 +23527,7 @@
       <c r="H26" s="8"/>
       <c r="I26" s="8"/>
       <c r="J26" s="8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="K26" s="19" t="s">
         <v>50</v>
@@ -23544,7 +23552,7 @@
         <v>43</v>
       </c>
       <c r="U26" s="22" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="V26" s="22"/>
       <c r="W26" s="22"/>
@@ -23552,7 +23560,7 @@
         <v>76</v>
       </c>
       <c r="Y26" s="22" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="Z26" s="8" t="n">
         <v>4</v>
@@ -24559,7 +24567,7 @@
         <v>24</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D27" s="22" t="s">
         <v>74</v>
@@ -24574,7 +24582,7 @@
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
       <c r="J27" s="8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="K27" s="19" t="s">
         <v>50</v>
@@ -24589,7 +24597,7 @@
         <v>70</v>
       </c>
       <c r="O27" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="P27" s="8"/>
       <c r="Q27" s="8"/>
@@ -25620,13 +25628,13 @@
         <v>25</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F28" s="8" t="s">
         <v>121</v>
@@ -25635,7 +25643,7 @@
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
       <c r="J28" s="8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="K28" s="19" t="s">
         <v>50</v>
@@ -25644,7 +25652,7 @@
         <v>76</v>
       </c>
       <c r="M28" s="8" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="N28" s="8"/>
       <c r="O28" s="8"/>
@@ -25654,17 +25662,17 @@
         <v>76</v>
       </c>
       <c r="S28" s="8" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="T28" s="8"/>
       <c r="U28" s="8"/>
       <c r="V28" s="8"/>
       <c r="W28" s="8"/>
       <c r="X28" s="8" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="Y28" s="8" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="Z28" s="8" t="n">
         <v>4</v>
@@ -26673,7 +26681,7 @@
         <v>26</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D29" s="22" t="s">
         <v>87</v>
@@ -26688,7 +26696,7 @@
       <c r="H29" s="8"/>
       <c r="I29" s="8"/>
       <c r="J29" s="8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="K29" s="19" t="s">
         <v>50</v>
@@ -26703,7 +26711,7 @@
         <v>43</v>
       </c>
       <c r="O29" s="8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="P29" s="8"/>
       <c r="Q29" s="8"/>
@@ -26711,13 +26719,13 @@
         <v>43</v>
       </c>
       <c r="S29" s="8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="T29" s="8" t="s">
         <v>45</v>
       </c>
       <c r="U29" s="8" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="V29" s="8"/>
       <c r="W29" s="8"/>
@@ -26742,13 +26750,13 @@
       <c r="AMI29" s="0"/>
       <c r="AMJ29" s="0"/>
     </row>
-    <row r="30" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="8"/>
       <c r="B30" s="8" t="n">
         <v>27</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D30" s="22" t="s">
         <v>81</v>
@@ -26763,7 +26771,7 @@
       <c r="H30" s="8"/>
       <c r="I30" s="8"/>
       <c r="J30" s="8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="K30" s="19" t="s">
         <v>50</v>
@@ -26772,7 +26780,7 @@
         <v>76</v>
       </c>
       <c r="M30" s="8" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="N30" s="8"/>
       <c r="O30" s="8"/>
@@ -26782,13 +26790,13 @@
         <v>76</v>
       </c>
       <c r="S30" s="8" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="T30" s="8" t="s">
         <v>45</v>
       </c>
       <c r="U30" s="8" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="V30" s="8"/>
       <c r="W30" s="8"/>
@@ -26796,7 +26804,7 @@
         <v>76</v>
       </c>
       <c r="Y30" s="22" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="Z30" s="8" t="n">
         <v>4</v>
@@ -26809,17 +26817,14 @@
         <v>50</v>
       </c>
       <c r="AD30" s="8"/>
-      <c r="AMH30" s="0"/>
-      <c r="AMI30" s="0"/>
-      <c r="AMJ30" s="0"/>
     </row>
-    <row r="31" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="8"/>
       <c r="B31" s="8" t="n">
         <v>28</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D31" s="22" t="s">
         <v>65</v>
@@ -26834,7 +26839,7 @@
       <c r="H31" s="8"/>
       <c r="I31" s="8"/>
       <c r="J31" s="8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="K31" s="19" t="s">
         <v>50</v>
@@ -26867,7 +26872,7 @@
         <v>76</v>
       </c>
       <c r="Y31" s="22" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="Z31" s="8" t="n">
         <v>4</v>
@@ -26880,9 +26885,6 @@
         <v>100</v>
       </c>
       <c r="AD31" s="8"/>
-      <c r="AMH31" s="0"/>
-      <c r="AMI31" s="0"/>
-      <c r="AMJ31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="8"/>
@@ -26890,7 +26892,7 @@
         <v>29</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D32" s="22" t="s">
         <v>49</v>
@@ -26905,7 +26907,7 @@
       <c r="H32" s="8"/>
       <c r="I32" s="8"/>
       <c r="J32" s="8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="K32" s="19" t="s">
         <v>50</v>
@@ -26914,7 +26916,7 @@
         <v>76</v>
       </c>
       <c r="M32" s="8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="N32" s="8" t="s">
         <v>43</v>
@@ -26946,7 +26948,7 @@
         <v>76</v>
       </c>
       <c r="Y32" s="22" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="Z32" s="8" t="n">
         <v>4</v>
@@ -26966,7 +26968,7 @@
         <v>30</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D33" s="22" t="s">
         <v>93</v>
@@ -26981,7 +26983,7 @@
       <c r="H33" s="8"/>
       <c r="I33" s="8"/>
       <c r="J33" s="8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="K33" s="19" t="s">
         <v>50</v>
@@ -26990,7 +26992,7 @@
         <v>76</v>
       </c>
       <c r="M33" s="8" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N33" s="8"/>
       <c r="O33" s="8"/>
@@ -27014,7 +27016,7 @@
         <v>76</v>
       </c>
       <c r="Y33" s="22" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="Z33" s="8" t="n">
         <v>4</v>
@@ -27034,13 +27036,13 @@
         <v>31</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D34" s="22" t="s">
         <v>38</v>
       </c>
       <c r="E34" s="26" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>121</v>
@@ -27049,7 +27051,7 @@
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
       <c r="J34" s="8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="K34" s="19" t="s">
         <v>50</v>
@@ -27058,13 +27060,13 @@
         <v>76</v>
       </c>
       <c r="M34" s="8" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="N34" s="8" t="s">
         <v>68</v>
       </c>
       <c r="O34" s="8" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="P34" s="8"/>
       <c r="Q34" s="8"/>
@@ -27072,13 +27074,13 @@
         <v>68</v>
       </c>
       <c r="S34" s="8" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="T34" s="8" t="s">
         <v>110</v>
       </c>
       <c r="U34" s="8" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="V34" s="8"/>
       <c r="W34" s="8"/>
@@ -27086,7 +27088,7 @@
         <v>76</v>
       </c>
       <c r="Y34" s="22" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="Z34" s="8" t="n">
         <v>4</v>
@@ -27106,13 +27108,13 @@
         <v>32</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>40</v>
@@ -27121,7 +27123,7 @@
       <c r="H35" s="8"/>
       <c r="I35" s="8"/>
       <c r="J35" s="8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="K35" s="8" t="s">
         <v>58</v>
@@ -27130,7 +27132,7 @@
         <v>76</v>
       </c>
       <c r="M35" s="8" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="N35" s="8"/>
       <c r="O35" s="8"/>
@@ -27161,7 +27163,7 @@
       <c r="AD35" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:AC35"/>
+  <autoFilter ref="A3:AD35"/>
   <mergeCells count="6">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="F1:I1"/>
@@ -27201,15 +27203,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>2</v>
@@ -27217,7 +27219,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>1.5</v>
@@ -27225,7 +27227,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>2</v>
@@ -27233,7 +27235,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>2</v>
@@ -27241,7 +27243,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>3</v>
@@ -27249,7 +27251,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>4</v>
@@ -27257,7 +27259,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>5</v>
@@ -27265,7 +27267,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>2</v>
@@ -27273,7 +27275,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>4</v>
@@ -27281,7 +27283,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>6</v>
@@ -27289,7 +27291,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>1</v>
@@ -27297,7 +27299,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>1</v>
@@ -27305,7 +27307,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>0.5</v>
@@ -27313,7 +27315,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>0.25</v>
@@ -27321,7 +27323,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>0.5</v>
@@ -27329,7 +27331,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>1</v>
@@ -27337,7 +27339,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B18" s="1" t="n">
         <v>0.3</v>
@@ -27345,7 +27347,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B19" s="1" t="n">
         <v>0.1</v>
@@ -27375,24 +27377,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="23.8866396761134"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.2105263157895"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="29" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27490,20 +27492,20 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2834008097166"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1983805668016"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.3198380566802"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="41" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B1" s="41" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C1" s="41" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27511,7 +27513,7 @@
         <v>19</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C2" s="42" t="n">
         <v>60</v>
@@ -27522,7 +27524,7 @@
         <v>23</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>50</v>
@@ -27533,7 +27535,7 @@
         <v>23</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>60</v>
@@ -27544,7 +27546,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>100</v>
@@ -27555,7 +27557,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>100</v>
@@ -27566,7 +27568,7 @@
         <v>19</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>100</v>
@@ -27577,7 +27579,7 @@
         <v>19</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>100</v>
@@ -27588,7 +27590,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>100</v>
@@ -27599,7 +27601,7 @@
         <v>19</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>100</v>
@@ -27610,7 +27612,7 @@
         <v>19</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>100</v>
@@ -27621,7 +27623,7 @@
         <v>19</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>100</v>
@@ -27632,7 +27634,7 @@
         <v>19</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>100</v>
@@ -27643,7 +27645,7 @@
         <v>19</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>100</v>
@@ -27654,7 +27656,7 @@
         <v>23</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>100</v>
@@ -27665,7 +27667,7 @@
         <v>23</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>100</v>
@@ -27676,7 +27678,7 @@
         <v>23</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>100</v>
@@ -27687,7 +27689,7 @@
         <v>23</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>100</v>
@@ -27698,7 +27700,7 @@
         <v>23</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>100</v>
@@ -27709,7 +27711,7 @@
         <v>23</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>100</v>
@@ -27720,7 +27722,7 @@
         <v>23</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>100</v>
@@ -27731,7 +27733,7 @@
         <v>23</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>100</v>
@@ -27742,7 +27744,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>100</v>

</xml_diff>